<commit_message>
Add Probability Distribution & Poisson
</commit_message>
<xml_diff>
--- a/Midterm Excel Sheet.xlsx
+++ b/Midterm Excel Sheet.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanninoa/Desktop/STA-2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A176650-059F-C94F-8880-0BEF7CDCCE03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600ABD3F-9437-EA42-8905-01C50977DCB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
+    <workbookView xWindow="15480" yWindow="2100" windowWidth="20320" windowHeight="16000" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
   </bookViews>
   <sheets>
     <sheet name="Random Variable x" sheetId="1" r:id="rId1"/>
-    <sheet name="sdfk" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Binomial Probability" sheetId="2" r:id="rId2"/>
+    <sheet name="x &amp; Probability" sheetId="4" r:id="rId3"/>
+    <sheet name="Expected Value" sheetId="5" r:id="rId4"/>
+    <sheet name="Poisson" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
   <si>
     <t>x</t>
   </si>
@@ -170,6 +172,72 @@
   </si>
   <si>
     <t>// move horizontally</t>
+  </si>
+  <si>
+    <t>Binomial Distribution</t>
+  </si>
+  <si>
+    <t>Exactly</t>
+  </si>
+  <si>
+    <t>Exactly (==)</t>
+  </si>
+  <si>
+    <t>Less Than or Equal to (&lt;=)</t>
+  </si>
+  <si>
+    <t>Greater Than (&gt;)</t>
+  </si>
+  <si>
+    <t>Great Than or Equal to (&gt;=)</t>
+  </si>
+  <si>
+    <t>Less Than ( &lt; )</t>
+  </si>
+  <si>
+    <t>The probability of two or more successes in any sufficiently small subinterval is 0.</t>
+  </si>
+  <si>
+    <t>The number of successes in any interval is independent of the number of successes in any other interval provided the intervals are not overlapping.</t>
+  </si>
+  <si>
+    <t>The experiment is performed a fixed number of times.</t>
+  </si>
+  <si>
+    <t>Discrete Probability Distribution (FREQUENCY)</t>
+  </si>
+  <si>
+    <t>Frequency(x)</t>
+  </si>
+  <si>
+    <t>Frequency Sum</t>
+  </si>
+  <si>
+    <t>P(x) sum</t>
+  </si>
+  <si>
+    <t>x * P(x)</t>
+  </si>
+  <si>
+    <t>Compute the probabiloty between two time intervals</t>
+  </si>
+  <si>
+    <t>Time Interval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean </t>
+  </si>
+  <si>
+    <t>Poisson</t>
+  </si>
+  <si>
+    <t>Fewer Than</t>
+  </si>
+  <si>
+    <t>At least</t>
+  </si>
+  <si>
+    <t>Lambda</t>
   </si>
 </sst>
 </file>
@@ -181,7 +249,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="185" formatCode="_(* #,##0.000000000000000000000_);_(* \(#,##0.000000000000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -224,6 +292,35 @@
       <color rgb="FFBD00C7"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFBD00C7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -255,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -274,6 +371,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -281,6 +381,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -602,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E068083-BD50-CB42-8AAE-F1525497B3A5}">
-  <dimension ref="A1:AE226"/>
+  <dimension ref="A1:AN226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -614,29 +735,37 @@
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="29.6640625" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
     <col min="9" max="9" width="16.5" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" customWidth="1"/>
     <col min="12" max="12" width="11.33203125" customWidth="1"/>
     <col min="14" max="14" width="17.1640625" customWidth="1"/>
     <col min="15" max="15" width="33" customWidth="1"/>
-    <col min="24" max="24" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="11" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:40">
       <c r="A1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="H1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U1" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AK1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:40">
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
@@ -644,26 +773,26 @@
         <f>SUM(C7:C169)</f>
         <v>0.29472871700000003</v>
       </c>
-      <c r="L2" t="s">
+      <c r="U2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="4">
+      <c r="V2" s="4">
         <v>54</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Z2" t="s">
         <v>12</v>
       </c>
-      <c r="R2" t="s">
+      <c r="AA2" t="s">
         <v>16</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AK2" t="s">
         <v>30</v>
       </c>
-      <c r="AC2">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31">
+      <c r="AL2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40">
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
@@ -674,23 +803,30 @@
       <c r="F3" t="s">
         <v>36</v>
       </c>
-      <c r="L3" t="s">
+      <c r="H3" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="19">
+        <f>SUM(I7:I11)</f>
+        <v>26171</v>
+      </c>
+      <c r="U3" t="s">
         <v>10</v>
       </c>
-      <c r="M3">
+      <c r="V3">
         <v>9.3200000000000005E-2</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AK3" t="s">
         <v>31</v>
       </c>
-      <c r="AC3">
-        <v>109</v>
-      </c>
-      <c r="AE3" t="s">
+      <c r="AL3">
+        <v>3</v>
+      </c>
+      <c r="AN3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:40">
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
@@ -701,69 +837,98 @@
       <c r="F4" t="s">
         <v>37</v>
       </c>
-      <c r="L4" t="s">
+      <c r="H4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="19">
+        <f>SUM(K7:K11)</f>
+        <v>3.7648160177295482</v>
+      </c>
+      <c r="U4" t="s">
         <v>11</v>
       </c>
-      <c r="M4">
+      <c r="V4">
         <v>53</v>
       </c>
-      <c r="N4" t="s">
+      <c r="W4" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="11">
-        <f>_xlfn.BINOM.DIST(M4, M2, M3, M5)</f>
+      <c r="X4" s="12">
+        <f>_xlfn.BINOM.DIST(V4, V2, V3, V5)</f>
         <v>1.1720567113389351E-53</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Z4" t="s">
         <v>17</v>
       </c>
-      <c r="R4">
+      <c r="AA4">
         <f>_xlfn.BINOM.DIST(8, 10, 0.9, FALSE)</f>
         <v>0.19371024450000002</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AJ4" t="s">
         <v>32</v>
       </c>
-      <c r="AC4">
-        <f>AC2*AC3</f>
-        <v>2943</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31">
+      <c r="AL4">
+        <f>AL2*AL3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40">
       <c r="F5" t="s">
         <v>38</v>
       </c>
-      <c r="L5" t="s">
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="19">
+        <f>SQRT(L13 - I4^2)</f>
+        <v>1.3875299946447814</v>
+      </c>
+      <c r="U5" t="s">
         <v>15</v>
       </c>
-      <c r="M5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31">
-      <c r="A6" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="10" t="s">
+      <c r="V5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40">
+      <c r="A6" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="H6" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK6" t="s">
         <v>11</v>
       </c>
-      <c r="AC6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31">
+      <c r="AL6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40">
       <c r="A7" s="7">
         <v>18000000</v>
       </c>
@@ -781,18 +946,36 @@
       <c r="F7" t="s">
         <v>40</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="H7" s="16">
+        <v>1</v>
+      </c>
+      <c r="I7" s="16">
+        <v>2828</v>
+      </c>
+      <c r="J7" s="16">
+        <f>I7/I$3</f>
+        <v>0.10805853807649689</v>
+      </c>
+      <c r="K7">
+        <f>H7*J7</f>
+        <v>0.10805853807649689</v>
+      </c>
+      <c r="L7">
+        <f>H7^2 * J7</f>
+        <v>0.10805853807649689</v>
+      </c>
+      <c r="AI7" t="s">
         <v>34</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AK7" t="s">
         <v>33</v>
       </c>
-      <c r="AC7">
-        <f>_xlfn.POISSON.DIST(AC6, AC4, TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31">
+      <c r="AL7">
+        <f>_xlfn.POISSON.DIST(AL6, AL4, FALSE)</f>
+        <v>0.16062314104798003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40">
       <c r="A8" s="7">
         <v>200000</v>
       </c>
@@ -810,14 +993,32 @@
       <c r="F8" t="s">
         <v>41</v>
       </c>
-      <c r="L8" t="s">
+      <c r="H8" s="16">
+        <v>2</v>
+      </c>
+      <c r="I8" s="16">
+        <v>2499</v>
+      </c>
+      <c r="J8" s="16">
+        <f>I8/I$3</f>
+        <v>9.5487371518092543E-2</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ref="K8:K11" si="2">H8*J8</f>
+        <v>0.19097474303618509</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ref="L8:L11" si="3">H8^2 * J8</f>
+        <v>0.38194948607237017</v>
+      </c>
+      <c r="U8" t="s">
         <v>18</v>
       </c>
-      <c r="N8" t="s">
+      <c r="W8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:40">
       <c r="A9" s="7">
         <v>10000</v>
       </c>
@@ -838,21 +1039,39 @@
       <c r="G9" t="s">
         <v>43</v>
       </c>
+      <c r="H9" s="16">
+        <v>3</v>
+      </c>
+      <c r="I9" s="16">
+        <v>4529</v>
+      </c>
+      <c r="J9" s="16">
+        <f>I9/I$3</f>
+        <v>0.17305414389973636</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>0.51916243169920906</v>
+      </c>
       <c r="L9">
-        <f>_xlfn.BINOM.DIST(0, O$9, O$10, FALSE)</f>
+        <f t="shared" si="3"/>
+        <v>1.5574872950976273</v>
+      </c>
+      <c r="U9">
+        <f>_xlfn.BINOM.DIST(0, X$9, X$10, FALSE)</f>
         <v>2.4399573321127992E-147</v>
       </c>
-      <c r="N9" t="s">
+      <c r="W9" t="s">
         <v>20</v>
       </c>
-      <c r="O9">
+      <c r="X9">
         <v>400</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AK9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:40">
       <c r="A10">
         <v>100</v>
       </c>
@@ -867,25 +1086,43 @@
         <f t="shared" si="1"/>
         <v>1.46627</v>
       </c>
+      <c r="H10" s="16">
+        <v>4</v>
+      </c>
+      <c r="I10" s="16">
+        <v>4459</v>
+      </c>
+      <c r="J10" s="16">
+        <f>I10/I$3</f>
+        <v>0.17037942761071415</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>0.68151771044285658</v>
+      </c>
       <c r="L10">
-        <f>_xlfn.BINOM.DIST(1, O$9, O$10, FALSE)</f>
+        <f t="shared" si="3"/>
+        <v>2.7260708417714263</v>
+      </c>
+      <c r="U10">
+        <f>_xlfn.BINOM.DIST(1, X$9, X$10, FALSE)</f>
         <v>1.2937448179575126E-144</v>
       </c>
-      <c r="N10" t="s">
+      <c r="W10" t="s">
         <v>21</v>
       </c>
-      <c r="O10">
+      <c r="X10">
         <v>0.56999999999999995</v>
       </c>
-      <c r="AB10" s="6"/>
-      <c r="AC10" s="6" t="s">
+      <c r="AK10" s="6"/>
+      <c r="AL10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AD10" s="6">
+      <c r="AM10" s="6">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:40">
       <c r="A11">
         <v>7</v>
       </c>
@@ -900,22 +1137,40 @@
         <f t="shared" si="1"/>
         <v>0.17368103900000001</v>
       </c>
+      <c r="H11" s="16">
+        <v>5</v>
+      </c>
+      <c r="I11" s="17">
+        <v>11856</v>
+      </c>
+      <c r="J11" s="16">
+        <f>I11/I$3</f>
+        <v>0.45302051889496009</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>2.2651025944748007</v>
+      </c>
       <c r="L11">
-        <f>_xlfn.BINOM.DIST(2, O$9, O$10, FALSE)</f>
+        <f t="shared" si="3"/>
+        <v>11.325512972374002</v>
+      </c>
+      <c r="U11">
+        <f>_xlfn.BINOM.DIST(2, X$9, X$10, FALSE)</f>
         <v>3.4213533017217944E-142</v>
       </c>
-      <c r="O11">
+      <c r="X11">
         <v>0.56999999999999995</v>
       </c>
-      <c r="AB11" s="6"/>
-      <c r="AC11" s="6" t="s">
+      <c r="AK11" s="6"/>
+      <c r="AL11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AD11" s="6">
+      <c r="AM11" s="6">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:40">
       <c r="A12">
         <v>4</v>
       </c>
@@ -930,27 +1185,27 @@
         <f t="shared" si="1"/>
         <v>0.10186824</v>
       </c>
-      <c r="L12">
-        <f>_xlfn.BINOM.DIST(3, O$9, O$10, FALSE)</f>
+      <c r="U12">
+        <f>_xlfn.BINOM.DIST(3, X$9, X$10, FALSE)</f>
         <v>6.0168078296788888E-140</v>
       </c>
-      <c r="N12" t="s">
+      <c r="W12" t="s">
         <v>22</v>
       </c>
-      <c r="O12">
-        <f>O9*O10</f>
+      <c r="X12">
+        <f>X9*X10</f>
         <v>227.99999999999997</v>
       </c>
-      <c r="AB12" s="6" t="s">
+      <c r="AK12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AC12" s="6"/>
-      <c r="AD12" s="6">
-        <f>-AD10/AD11</f>
+      <c r="AL12" s="6"/>
+      <c r="AM12" s="6">
+        <f>-AM10/AM11</f>
         <v>-0.34905660377358488</v>
       </c>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:40">
       <c r="A13">
         <v>3</v>
       </c>
@@ -965,19 +1220,30 @@
         <f t="shared" si="1"/>
         <v>0.15959213999999999</v>
       </c>
+      <c r="I13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="19">
+        <f>SUM(J7:J11)</f>
+        <v>1</v>
+      </c>
       <c r="L13">
-        <f>_xlfn.BINOM.DIST(4, O$9, O$10, FALSE)</f>
+        <f>SUM(L7:L11)</f>
+        <v>16.099079133391921</v>
+      </c>
+      <c r="U13">
+        <f>_xlfn.BINOM.DIST(4, X$9, X$10, FALSE)</f>
         <v>7.9159502545234828E-138</v>
       </c>
-      <c r="N13" t="s">
+      <c r="W13" t="s">
         <v>23</v>
       </c>
-      <c r="O13">
-        <f>SQRT((O9*O10)*(1-O10))</f>
+      <c r="X13">
+        <f>SQRT((X9*X10)*(1-X10))</f>
         <v>9.9015150355892505</v>
       </c>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:40">
       <c r="A14">
         <v>0</v>
       </c>
@@ -992,252 +1258,252 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L14">
-        <f>_xlfn.BINOM.DIST(5, O$9, O$10, FALSE)</f>
+      <c r="U14">
+        <f>_xlfn.BINOM.DIST(5, X$9, X$10, FALSE)</f>
         <v>8.3106432160515925E-136</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AL14" t="s">
         <v>11</v>
       </c>
-      <c r="AD14">
+      <c r="AM14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:40">
       <c r="C15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L15">
-        <f>_xlfn.BINOM.DIST(6, O$9, O$10, FALSE)</f>
+      <c r="U15">
+        <f>_xlfn.BINOM.DIST(6, X$9, X$10, FALSE)</f>
         <v>7.2524857367988658E-134</v>
       </c>
-      <c r="AC15" s="6" t="s">
+      <c r="AL15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AD15">
-        <f>AD14*EXP(AD12)</f>
+      <c r="AM15">
+        <f>AM14*EXP(AM12)</f>
         <v>0.7053532034869342</v>
       </c>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:40">
       <c r="C16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L16">
-        <f>_xlfn.BINOM.DIST(7, O$9, O$10, FALSE)</f>
+      <c r="U16">
+        <f>_xlfn.BINOM.DIST(7, X$9, X$10, FALSE)</f>
         <v>5.411173577309513E-132</v>
       </c>
     </row>
-    <row r="17" spans="3:17">
+    <row r="17" spans="3:26">
       <c r="C17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L17">
-        <f>_xlfn.BINOM.DIST(8, O$9, O$10, FALSE)</f>
+      <c r="U17">
+        <f>_xlfn.BINOM.DIST(8, X$9, X$10, FALSE)</f>
         <v>3.5237121891079178E-130</v>
       </c>
     </row>
-    <row r="18" spans="3:17">
+    <row r="18" spans="3:26">
       <c r="C18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L18">
-        <f>_xlfn.BINOM.DIST(9, O$9, O$10, FALSE)</f>
+      <c r="U18">
+        <f>_xlfn.BINOM.DIST(9, X$9, X$10, FALSE)</f>
         <v>2.0344657662384347E-128</v>
       </c>
     </row>
-    <row r="19" spans="3:17">
+    <row r="19" spans="3:26">
       <c r="C19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L19">
-        <f>_xlfn.BINOM.DIST(10, O$9, O$10, FALSE)</f>
+      <c r="U19">
+        <f>_xlfn.BINOM.DIST(10, X$9, X$10, FALSE)</f>
         <v>1.0544683379570883E-126</v>
       </c>
     </row>
-    <row r="20" spans="3:17">
+    <row r="20" spans="3:26">
       <c r="C20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L20" s="12" t="s">
+      <c r="U20" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="3:17">
+    <row r="21" spans="3:26">
       <c r="C21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L21" t="s">
+      <c r="U21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="3:17">
+    <row r="22" spans="3:26">
       <c r="C22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L22" t="s">
+      <c r="U22" t="s">
         <v>25</v>
       </c>
-      <c r="M22" t="s">
+      <c r="V22" t="s">
         <v>26</v>
       </c>
-      <c r="N22" t="s">
+      <c r="W22" t="s">
         <v>27</v>
       </c>
-      <c r="O22">
+      <c r="X22">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="3:17">
+    <row r="23" spans="3:26">
       <c r="C23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23" s="5">
-        <f>_xlfn.BINOM.DIST(L23,O$22,O$23, FALSE)</f>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23" s="5">
+        <f>_xlfn.BINOM.DIST(U23,X$22,X$23, FALSE)</f>
         <v>7.2900000000000037E-4</v>
       </c>
-      <c r="N23" t="s">
+      <c r="W23" t="s">
         <v>28</v>
       </c>
-      <c r="O23">
+      <c r="X23">
         <v>0.7</v>
       </c>
     </row>
-    <row r="24" spans="3:17">
+    <row r="24" spans="3:26">
       <c r="C24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L24">
+      <c r="U24">
         <v>1</v>
       </c>
-      <c r="M24" s="5">
-        <f>_xlfn.BINOM.DIST(L24,O$22,O$23, FALSE)</f>
+      <c r="V24" s="5">
+        <f>_xlfn.BINOM.DIST(U24,X$22,X$23, FALSE)</f>
         <v>1.0206000000000015E-2</v>
       </c>
     </row>
-    <row r="25" spans="3:17">
+    <row r="25" spans="3:26">
       <c r="C25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L25">
+      <c r="U25">
         <v>2</v>
       </c>
-      <c r="M25" s="5">
-        <f>_xlfn.BINOM.DIST(L25,O$22,O$23, FALSE)</f>
+      <c r="V25" s="5">
+        <f>_xlfn.BINOM.DIST(U25,X$22,X$23, FALSE)</f>
         <v>5.9535000000000053E-2</v>
       </c>
     </row>
-    <row r="26" spans="3:17">
+    <row r="26" spans="3:26">
       <c r="C26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L26">
+      <c r="U26">
         <v>3</v>
       </c>
-      <c r="M26" s="5">
-        <f>_xlfn.BINOM.DIST(L26,O$22,O$23, FALSE)</f>
+      <c r="V26" s="5">
+        <f>_xlfn.BINOM.DIST(U26,X$22,X$23, FALSE)</f>
         <v>0.18522</v>
       </c>
     </row>
-    <row r="27" spans="3:17">
+    <row r="27" spans="3:26">
       <c r="C27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L27">
+      <c r="U27">
         <v>4</v>
       </c>
-      <c r="M27" s="5">
-        <f>_xlfn.BINOM.DIST(L27,O$22,O$23, FALSE)</f>
+      <c r="V27" s="5">
+        <f>_xlfn.BINOM.DIST(U27,X$22,X$23, FALSE)</f>
         <v>0.32413500000000006</v>
       </c>
     </row>
-    <row r="28" spans="3:17">
+    <row r="28" spans="3:26">
       <c r="C28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L28">
+      <c r="U28">
         <v>5</v>
       </c>
-      <c r="M28" s="5">
-        <f>_xlfn.BINOM.DIST(L28,O$22,O$23, FALSE)</f>
+      <c r="V28" s="5">
+        <f>_xlfn.BINOM.DIST(U28,X$22,X$23, FALSE)</f>
         <v>0.30252599999999991</v>
       </c>
     </row>
-    <row r="29" spans="3:17">
+    <row r="29" spans="3:26">
       <c r="C29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L29">
+      <c r="U29">
         <v>6</v>
       </c>
-      <c r="M29" s="5">
-        <f>_xlfn.BINOM.DIST(L29,O$22,O$23, FALSE)</f>
+      <c r="V29" s="5">
+        <f>_xlfn.BINOM.DIST(U29,X$22,X$23, FALSE)</f>
         <v>0.11764899999999995</v>
       </c>
-      <c r="Q29">
+      <c r="Z29">
         <f>_xlfn.BINOM.DIST(23, 25, 0.61, FALSE)</f>
         <v>5.2703162233064466E-4</v>
       </c>
     </row>
-    <row r="30" spans="3:17">
+    <row r="30" spans="3:26">
       <c r="C30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q30">
+      <c r="Z30">
         <f>_xlfn.BINOM.DIST(24, 25, 0.61, FALSE)</f>
         <v>6.8694292654207783E-5</v>
       </c>
     </row>
-    <row r="31" spans="3:17">
+    <row r="31" spans="3:26">
       <c r="C31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L31" t="s">
+      <c r="U31" t="s">
         <v>22</v>
       </c>
-      <c r="M31">
-        <f>O22*O23</f>
+      <c r="V31">
+        <f>X22*X23</f>
         <v>4.1999999999999993</v>
       </c>
-      <c r="Q31">
+      <c r="Z31">
         <f>_xlfn.BINOM.DIST(25, 25, 0.61, FALSE)</f>
         <v>4.2977967711863337E-6</v>
       </c>
     </row>
-    <row r="32" spans="3:17">
+    <row r="32" spans="3:26">
       <c r="C32">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L32" t="s">
+      <c r="U32" t="s">
         <v>23</v>
       </c>
-      <c r="N32">
-        <f>SQRT((O22*O23)*(1-O23))</f>
+      <c r="W32">
+        <f>SQRT((X22*X23)*(1-X23))</f>
         <v>1.1224972160321824</v>
       </c>
-      <c r="Q32">
-        <f>SUM(Q29:Q31)</f>
+      <c r="Z32">
+        <f>SUM(Z29:Z31)</f>
         <v>6.0002371175603886E-4</v>
       </c>
     </row>
@@ -1477,931 +1743,931 @@
     </row>
     <row r="72" spans="3:3">
       <c r="C72">
-        <f t="shared" ref="C72:C135" si="2">A72*B72</f>
+        <f t="shared" ref="C72:C135" si="4">A72*B72</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="3:3">
       <c r="C73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="3:3">
       <c r="C74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="3:3">
       <c r="C75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="3:3">
       <c r="C76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="3:3">
       <c r="C77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="3:3">
       <c r="C78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="3:3">
       <c r="C79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="3:3">
       <c r="C80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="3:3">
       <c r="C98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="3:3">
       <c r="C99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="3:3">
       <c r="C100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="3:3">
       <c r="C101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="3:3">
       <c r="C102">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="3:3">
       <c r="C103">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="3:3">
       <c r="C104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="3:3">
       <c r="C105">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="3:3">
       <c r="C106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="3:3">
       <c r="C107">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="3:3">
       <c r="C108">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="109" spans="3:3">
       <c r="C109">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="3:3">
       <c r="C110">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="3:3">
       <c r="C111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="3:3">
       <c r="C112">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="3:3">
       <c r="C113">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="3:3">
       <c r="C114">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="3:3">
       <c r="C115">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="3:3">
       <c r="C116">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="3:3">
       <c r="C117">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="3:3">
       <c r="C118">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="3:3">
       <c r="C119">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="3:3">
       <c r="C120">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="3:3">
       <c r="C121">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="3:3">
       <c r="C122">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="3:3">
       <c r="C123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="3:3">
       <c r="C124">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="3:3">
       <c r="C125">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="3:3">
       <c r="C126">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="3:3">
       <c r="C127">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="3:3">
       <c r="C128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="3:3">
       <c r="C129">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="3:3">
       <c r="C130">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="3:3">
       <c r="C131">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="3:3">
       <c r="C132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="3:3">
       <c r="C133">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="3:3">
       <c r="C134">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="3:3">
       <c r="C135">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="136" spans="3:3">
       <c r="C136">
-        <f t="shared" ref="C136:C199" si="3">A136*B136</f>
+        <f t="shared" ref="C136:C199" si="5">A136*B136</f>
         <v>0</v>
       </c>
     </row>
     <row r="137" spans="3:3">
       <c r="C137">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="3:3">
       <c r="C138">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="3:3">
       <c r="C139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="140" spans="3:3">
       <c r="C140">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="141" spans="3:3">
       <c r="C141">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="142" spans="3:3">
       <c r="C142">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="143" spans="3:3">
       <c r="C143">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="144" spans="3:3">
       <c r="C144">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="145" spans="3:3">
       <c r="C145">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="146" spans="3:3">
       <c r="C146">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="147" spans="3:3">
       <c r="C147">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="148" spans="3:3">
       <c r="C148">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="149" spans="3:3">
       <c r="C149">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="150" spans="3:3">
       <c r="C150">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="151" spans="3:3">
       <c r="C151">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="152" spans="3:3">
       <c r="C152">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="153" spans="3:3">
       <c r="C153">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="154" spans="3:3">
       <c r="C154">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="155" spans="3:3">
       <c r="C155">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="156" spans="3:3">
       <c r="C156">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="157" spans="3:3">
       <c r="C157">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="158" spans="3:3">
       <c r="C158">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="159" spans="3:3">
       <c r="C159">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="160" spans="3:3">
       <c r="C160">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="161" spans="3:3">
       <c r="C161">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="162" spans="3:3">
       <c r="C162">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="163" spans="3:3">
       <c r="C163">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="164" spans="3:3">
       <c r="C164">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="165" spans="3:3">
       <c r="C165">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="166" spans="3:3">
       <c r="C166">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="167" spans="3:3">
       <c r="C167">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="168" spans="3:3">
       <c r="C168">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="169" spans="3:3">
       <c r="C169">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="170" spans="3:3">
       <c r="C170">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="171" spans="3:3">
       <c r="C171">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="172" spans="3:3">
       <c r="C172">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="173" spans="3:3">
       <c r="C173">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="174" spans="3:3">
       <c r="C174">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="175" spans="3:3">
       <c r="C175">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="176" spans="3:3">
       <c r="C176">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="177" spans="3:3">
       <c r="C177">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="178" spans="3:3">
       <c r="C178">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="179" spans="3:3">
       <c r="C179">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="180" spans="3:3">
       <c r="C180">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="181" spans="3:3">
       <c r="C181">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="182" spans="3:3">
       <c r="C182">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="183" spans="3:3">
       <c r="C183">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="184" spans="3:3">
       <c r="C184">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="185" spans="3:3">
       <c r="C185">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="186" spans="3:3">
       <c r="C186">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="187" spans="3:3">
       <c r="C187">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="188" spans="3:3">
       <c r="C188">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="189" spans="3:3">
       <c r="C189">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="190" spans="3:3">
       <c r="C190">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="191" spans="3:3">
       <c r="C191">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="192" spans="3:3">
       <c r="C192">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="193" spans="3:3">
       <c r="C193">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="194" spans="3:3">
       <c r="C194">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="195" spans="3:3">
       <c r="C195">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="196" spans="3:3">
       <c r="C196">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="197" spans="3:3">
       <c r="C197">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="198" spans="3:3">
       <c r="C198">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="199" spans="3:3">
       <c r="C199">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="200" spans="3:3">
       <c r="C200">
-        <f t="shared" ref="C200:C226" si="4">A200*B200</f>
+        <f t="shared" ref="C200:C226" si="6">A200*B200</f>
         <v>0</v>
       </c>
     </row>
     <row r="201" spans="3:3">
       <c r="C201">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="202" spans="3:3">
       <c r="C202">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="203" spans="3:3">
       <c r="C203">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="204" spans="3:3">
       <c r="C204">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="205" spans="3:3">
       <c r="C205">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="206" spans="3:3">
       <c r="C206">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="207" spans="3:3">
       <c r="C207">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="208" spans="3:3">
       <c r="C208">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="209" spans="3:3">
       <c r="C209">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="210" spans="3:3">
       <c r="C210">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="211" spans="3:3">
       <c r="C211">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="212" spans="3:3">
       <c r="C212">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="213" spans="3:3">
       <c r="C213">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="214" spans="3:3">
       <c r="C214">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="215" spans="3:3">
       <c r="C215">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="216" spans="3:3">
       <c r="C216">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="217" spans="3:3">
       <c r="C217">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="218" spans="3:3">
       <c r="C218">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="219" spans="3:3">
       <c r="C219">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="220" spans="3:3">
       <c r="C220">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="221" spans="3:3">
       <c r="C221">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="222" spans="3:3">
       <c r="C222">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="223" spans="3:3">
       <c r="C223">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="224" spans="3:3">
       <c r="C224">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="225" spans="3:3">
       <c r="C225">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="226" spans="3:3">
       <c r="C226">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2412,18 +2678,175 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74F7077-45B6-E742-951B-BF30C929E163}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="12">
+        <f>_xlfn.BINOM.DIST(B$2, B$3, B$4, FALSE)</f>
+        <v>2.7525119999999965E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="12">
+        <f>_xlfn.BINOM.DIST(B$2 - 1, B$3, B$4, TRUE)</f>
+        <v>3.1385599999999973E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="12">
+        <f>_xlfn.BINOM.DIST(B$2, B$3, B$4, TRUE)</f>
+        <v>3.0663680000000003E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="12">
+        <f xml:space="preserve"> 1 - B8</f>
+        <v>0.999686144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11">
+        <f>1 - _xlfn.BINOM.DIST(B$2 - 1, B$3, B$4, FALSE)</f>
+        <v>0.99970508800000002</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD5251E-A9B7-7F4B-A78E-2F9C7E161BB7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1764C7-EB3F-884D-A423-6A64CF5D743E}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="23">
+        <v>450</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="19">
+        <f>B2*B3</f>
+        <v>220.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="23">
+        <v>0.49</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="19">
+        <f>SQRT((B2*B3)*(1-B3))</f>
+        <v>10.604480185280181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="C6" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7883183-3309-E141-80C9-0F546E3ED993}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2432,4 +2855,107 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD5251E-A9B7-7F4B-A78E-2F9C7E161BB7}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17">
+      <c r="A1" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17">
+      <c r="A2" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17">
+      <c r="A3" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17">
+      <c r="A5" s="21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17">
+      <c r="A6" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17">
+      <c r="A7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17">
+      <c r="A8" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="17">
+      <c r="A9" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="20">
+        <f>B6*B8</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17">
+      <c r="A12" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="20">
+        <f>_xlfn.POISSON.DIST(B7,B9, FALSE)</f>
+        <v>0.16062314104798003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="17">
+      <c r="A13" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="20">
+        <f>_xlfn.POISSON.DIST(B7 - 1, B9, TRUE)</f>
+        <v>0.44567964136461113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="17">
+      <c r="A14" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="20">
+        <f>1 - B13</f>
+        <v>0.55432035863538887</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Binomial Probability, Normal Distribution & Expected Value
</commit_message>
<xml_diff>
--- a/Midterm Excel Sheet.xlsx
+++ b/Midterm Excel Sheet.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanninoa/Desktop/STA-2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600ABD3F-9437-EA42-8905-01C50977DCB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6F935E-7000-3842-A9C0-EE10D936D9C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15480" yWindow="2100" windowWidth="20320" windowHeight="16000" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
+    <workbookView xWindow="17340" yWindow="2160" windowWidth="20320" windowHeight="16000" activeTab="4" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
   </bookViews>
   <sheets>
     <sheet name="Random Variable x" sheetId="1" r:id="rId1"/>
-    <sheet name="Binomial Probability" sheetId="2" r:id="rId2"/>
-    <sheet name="x &amp; Probability" sheetId="4" r:id="rId3"/>
-    <sheet name="Expected Value" sheetId="5" r:id="rId4"/>
-    <sheet name="Poisson" sheetId="3" r:id="rId5"/>
+    <sheet name="Normal Distribution" sheetId="6" r:id="rId2"/>
+    <sheet name="Binomial Probability" sheetId="2" r:id="rId3"/>
+    <sheet name="x &amp; Probability" sheetId="4" r:id="rId4"/>
+    <sheet name="Expected Value" sheetId="5" r:id="rId5"/>
+    <sheet name="Poisson" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t>x</t>
   </si>
@@ -238,6 +239,15 @@
   </si>
   <si>
     <t>Lambda</t>
+  </si>
+  <si>
+    <t>The probability of success is the same for any two intervals of equal length.</t>
+  </si>
+  <si>
+    <t>There are two mutually exclusive​ outcomes, success or failure.</t>
+  </si>
+  <si>
+    <t>The trials are independent.</t>
   </si>
 </sst>
 </file>
@@ -249,7 +259,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="185" formatCode="_(* #,##0.000000000000000000000_);_(* \(#,##0.000000000000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -321,6 +331,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -352,7 +370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -402,6 +420,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -725,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E068083-BD50-CB42-8AAE-F1525497B3A5}">
   <dimension ref="A1:AN226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+    <sheetView topLeftCell="E1" zoomScale="82" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -808,7 +829,7 @@
       </c>
       <c r="I3" s="19">
         <f>SUM(I7:I11)</f>
-        <v>26171</v>
+        <v>25869</v>
       </c>
       <c r="U3" t="s">
         <v>10</v>
@@ -842,7 +863,7 @@
       </c>
       <c r="I4" s="19">
         <f>SUM(K7:K11)</f>
-        <v>3.7648160177295482</v>
+        <v>3.7699949746801193</v>
       </c>
       <c r="U4" t="s">
         <v>11</v>
@@ -881,7 +902,7 @@
       </c>
       <c r="I5" s="19">
         <f>SQRT(L13 - I4^2)</f>
-        <v>1.3875299946447814</v>
+        <v>1.3818272126164455</v>
       </c>
       <c r="U5" t="s">
         <v>15</v>
@@ -950,19 +971,19 @@
         <v>1</v>
       </c>
       <c r="I7" s="16">
-        <v>2828</v>
+        <v>2492</v>
       </c>
       <c r="J7" s="16">
         <f>I7/I$3</f>
-        <v>0.10805853807649689</v>
+        <v>9.6331516486914834E-2</v>
       </c>
       <c r="K7">
         <f>H7*J7</f>
-        <v>0.10805853807649689</v>
+        <v>9.6331516486914834E-2</v>
       </c>
       <c r="L7">
         <f>H7^2 * J7</f>
-        <v>0.10805853807649689</v>
+        <v>9.6331516486914834E-2</v>
       </c>
       <c r="AI7" t="s">
         <v>34</v>
@@ -997,19 +1018,19 @@
         <v>2</v>
       </c>
       <c r="I8" s="16">
-        <v>2499</v>
+        <v>2941</v>
       </c>
       <c r="J8" s="16">
         <f>I8/I$3</f>
-        <v>9.5487371518092543E-2</v>
+        <v>0.11368819822954115</v>
       </c>
       <c r="K8">
         <f t="shared" ref="K8:K11" si="2">H8*J8</f>
-        <v>0.19097474303618509</v>
+        <v>0.22737639645908231</v>
       </c>
       <c r="L8">
         <f t="shared" ref="L8:L11" si="3">H8^2 * J8</f>
-        <v>0.38194948607237017</v>
+        <v>0.45475279291816462</v>
       </c>
       <c r="U8" t="s">
         <v>18</v>
@@ -1043,19 +1064,19 @@
         <v>3</v>
       </c>
       <c r="I9" s="16">
-        <v>4529</v>
+        <v>4582</v>
       </c>
       <c r="J9" s="16">
         <f>I9/I$3</f>
-        <v>0.17305414389973636</v>
+        <v>0.17712319764969656</v>
       </c>
       <c r="K9">
         <f t="shared" si="2"/>
-        <v>0.51916243169920906</v>
+        <v>0.5313695929490897</v>
       </c>
       <c r="L9">
         <f t="shared" si="3"/>
-        <v>1.5574872950976273</v>
+        <v>1.594108778847269</v>
       </c>
       <c r="U9">
         <f>_xlfn.BINOM.DIST(0, X$9, X$10, FALSE)</f>
@@ -1090,19 +1111,19 @@
         <v>4</v>
       </c>
       <c r="I10" s="16">
-        <v>4459</v>
+        <v>3864</v>
       </c>
       <c r="J10" s="16">
         <f>I10/I$3</f>
-        <v>0.17037942761071415</v>
+        <v>0.14936796938420505</v>
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
-        <v>0.68151771044285658</v>
+        <v>0.59747187753682018</v>
       </c>
       <c r="L10">
         <f t="shared" si="3"/>
-        <v>2.7260708417714263</v>
+        <v>2.3898875101472807</v>
       </c>
       <c r="U10">
         <f>_xlfn.BINOM.DIST(1, X$9, X$10, FALSE)</f>
@@ -1141,19 +1162,19 @@
         <v>5</v>
       </c>
       <c r="I11" s="17">
-        <v>11856</v>
+        <v>11990</v>
       </c>
       <c r="J11" s="16">
         <f>I11/I$3</f>
-        <v>0.45302051889496009</v>
+        <v>0.46348911824964245</v>
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
-        <v>2.2651025944748007</v>
+        <v>2.3174455912482124</v>
       </c>
       <c r="L11">
         <f t="shared" si="3"/>
-        <v>11.325512972374002</v>
+        <v>11.587227956241062</v>
       </c>
       <c r="U11">
         <f>_xlfn.BINOM.DIST(2, X$9, X$10, FALSE)</f>
@@ -1229,7 +1250,7 @@
       </c>
       <c r="L13">
         <f>SUM(L7:L11)</f>
-        <v>16.099079133391921</v>
+        <v>16.122308554640689</v>
       </c>
       <c r="U13">
         <f>_xlfn.BINOM.DIST(4, X$9, X$10, FALSE)</f>
@@ -2677,11 +2698,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C96CE9-B77B-704D-8A1F-7836B7353FCF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74F7077-45B6-E742-951B-BF30C929E163}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2716,7 +2749,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2733,7 +2766,7 @@
       </c>
       <c r="B7" s="12">
         <f>_xlfn.BINOM.DIST(B$2, B$3, B$4, FALSE)</f>
-        <v>2.7525119999999965E-3</v>
+        <v>7.4317824000000032E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2742,7 +2775,7 @@
       </c>
       <c r="B8" s="12">
         <f>_xlfn.BINOM.DIST(B$2 - 1, B$3, B$4, TRUE)</f>
-        <v>3.1385599999999973E-4</v>
+        <v>2.5034752000000014E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2751,7 +2784,7 @@
       </c>
       <c r="B9" s="12">
         <f>_xlfn.BINOM.DIST(B$2, B$3, B$4, TRUE)</f>
-        <v>3.0663680000000003E-3</v>
+        <v>9.935257600000004E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2759,8 +2792,8 @@
         <v>49</v>
       </c>
       <c r="B10" s="12">
-        <f xml:space="preserve"> 1 - B8</f>
-        <v>0.999686144</v>
+        <f xml:space="preserve"> 1 - B9</f>
+        <v>0.90064742399999997</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2769,7 +2802,49 @@
       </c>
       <c r="B11">
         <f>1 - _xlfn.BINOM.DIST(B$2 - 1, B$3, B$4, FALSE)</f>
-        <v>0.99970508800000002</v>
+        <v>0.97876633599999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1"/>
+      <c r="B13">
+        <f>_xlfn.BINOM.DIST(8, B$3, B$4, FALSE)</f>
+        <v>6.0466175999999983E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1"/>
+      <c r="B14">
+        <f>_xlfn.BINOM.DIST(6, B$3, B$4, FALSE)</f>
+        <v>0.25082265600000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1"/>
+      <c r="B15">
+        <f>_xlfn.BINOM.DIST(7, B$3, B$4, FALSE)</f>
+        <v>0.16124313599999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="B16">
+        <f>SUM(B13:B15)</f>
+        <v>0.47253196799999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="17">
+      <c r="A18" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="17">
+      <c r="A19" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="17">
+      <c r="A20" s="15" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2777,12 +2852,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1764C7-EB3F-884D-A423-6A64CF5D743E}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2802,7 +2877,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="23">
-        <v>450</v>
+        <v>150</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="22" t="s">
@@ -2810,7 +2885,7 @@
       </c>
       <c r="E2" s="19">
         <f>B2*B3</f>
-        <v>220.5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2818,7 +2893,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="23">
-        <v>0.49</v>
+        <v>0.42</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="22" t="s">
@@ -2826,7 +2901,7 @@
       </c>
       <c r="E3" s="19">
         <f>SQRT((B2*B3)*(1-B3))</f>
-        <v>10.604480185280181</v>
+        <v>6.044832503882966</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2845,24 +2920,59 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7883183-3309-E141-80C9-0F546E3ED993}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>7</v>
+      </c>
+      <c r="B1">
+        <f>37/38</f>
+        <v>0.97368421052631582</v>
+      </c>
+      <c r="C1">
+        <f>A1*B1</f>
+        <v>6.8157894736842106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>-245</v>
+      </c>
+      <c r="B2">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="C2">
+        <f>A2*B2</f>
+        <v>-6.447368421052631</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="C3">
+        <f>SUM(C1:C2)</f>
+        <v>0.36842105263157965</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD5251E-A9B7-7F4B-A78E-2F9C7E161BB7}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2882,7 +2992,7 @@
     </row>
     <row r="3" spans="1:2" ht="17">
       <c r="A3" s="15" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17">
@@ -2923,8 +3033,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:2" ht="26">
+      <c r="A11" s="24" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Poisson Distributions + other stuff
</commit_message>
<xml_diff>
--- a/Midterm Excel Sheet.xlsx
+++ b/Midterm Excel Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanninoa/Desktop/STA-2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanninoa/Desktop/Business-Stats-Excel-Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6F935E-7000-3842-A9C0-EE10D936D9C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2FE2ED-D55D-D345-9581-29434AFA7836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17340" yWindow="2160" windowWidth="20320" windowHeight="16000" activeTab="4" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" activeTab="5" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
   </bookViews>
   <sheets>
     <sheet name="Random Variable x" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="x &amp; Probability" sheetId="4" r:id="rId4"/>
     <sheet name="Expected Value" sheetId="5" r:id="rId5"/>
     <sheet name="Poisson" sheetId="3" r:id="rId6"/>
+    <sheet name="Poisson v2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="110">
   <si>
     <t>x</t>
   </si>
@@ -178,9 +179,6 @@
     <t>Binomial Distribution</t>
   </si>
   <si>
-    <t>Exactly</t>
-  </si>
-  <si>
     <t>Exactly (==)</t>
   </si>
   <si>
@@ -220,9 +218,6 @@
     <t>x * P(x)</t>
   </si>
   <si>
-    <t>Compute the probabiloty between two time intervals</t>
-  </si>
-  <si>
     <t>Time Interval</t>
   </si>
   <si>
@@ -232,12 +227,6 @@
     <t>Poisson</t>
   </si>
   <si>
-    <t>Fewer Than</t>
-  </si>
-  <si>
-    <t>At least</t>
-  </si>
-  <si>
     <t>Lambda</t>
   </si>
   <si>
@@ -248,18 +237,151 @@
   </si>
   <si>
     <t>The trials are independent.</t>
+  </si>
+  <si>
+    <t>Area under Normal Curve</t>
+  </si>
+  <si>
+    <t>lower bound</t>
+  </si>
+  <si>
+    <t>upper bound</t>
+  </si>
+  <si>
+    <t>lower bound z-score</t>
+  </si>
+  <si>
+    <t>P(ZsubLower &lt;= lowerbound z-score)</t>
+  </si>
+  <si>
+    <t>P(ZsubHigher &lt;= upperbound z-score)</t>
+  </si>
+  <si>
+    <t>upper bound z-score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contains more than </t>
+  </si>
+  <si>
+    <t>bound</t>
+  </si>
+  <si>
+    <t>contains more than - use complement (1 - x)</t>
+  </si>
+  <si>
+    <t>percentile - =norm.dist</t>
+  </si>
+  <si>
+    <t>Normal Inverse (Percentile)</t>
+  </si>
+  <si>
+    <t>Percentile</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>If the z-score is positive, add .5 to the table value</t>
+  </si>
+  <si>
+    <t>Negative Z</t>
+  </si>
+  <si>
+    <t>positive Z</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Less than z1, greater than z2 AKA to the left of z1 to the right of z2</t>
+  </si>
+  <si>
+    <t>&lt;- Also expected profit</t>
+  </si>
+  <si>
+    <t>Sum(mean)</t>
+  </si>
+  <si>
+    <t>x^2 - P(x)</t>
+  </si>
+  <si>
+    <t>Hurricane</t>
+  </si>
+  <si>
+    <t>direct hits</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>Exactly X</t>
+  </si>
+  <si>
+    <t>Fewer Than X</t>
+  </si>
+  <si>
+    <t>At least X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FROM </t>
+  </si>
+  <si>
+    <t>TO</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>(add each number as an individual entry and sum them up)</t>
+  </si>
+  <si>
+    <t>Compute the probability between two time intervals</t>
+  </si>
+  <si>
+    <t>Poisson with a given lambda and time interval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lambda </t>
+  </si>
+  <si>
+    <t>time interval</t>
+  </si>
+  <si>
+    <t>Less Than X</t>
+  </si>
+  <si>
+    <t>At Least X</t>
+  </si>
+  <si>
+    <t>Computed Mean</t>
+  </si>
+  <si>
+    <t>Food Problem</t>
+  </si>
+  <si>
+    <t>fragment per gram</t>
+  </si>
+  <si>
+    <t># gram sample</t>
+  </si>
+  <si>
+    <t>Fewer than X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="185" formatCode="_(* #,##0.000000000000000000000_);_(* \(#,##0.000000000000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.000000000000000000000_);_(* \(#,##0.000000000000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="215" formatCode="0.0000000000000000000000000000000000000000000000000000E+00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -339,6 +461,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue Light"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -370,7 +505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -395,7 +530,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -422,6 +557,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="215" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -746,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E068083-BD50-CB42-8AAE-F1525497B3A5}">
   <dimension ref="A1:AN226"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="82" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:I11"/>
+    <sheetView zoomScale="82" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -774,7 +930,7 @@
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U1" t="s">
         <v>8</v>
@@ -792,7 +948,7 @@
       </c>
       <c r="D2" s="8">
         <f>SUM(C7:C169)</f>
-        <v>0.29472871700000003</v>
+        <v>1.6335</v>
       </c>
       <c r="U2" t="s">
         <v>9</v>
@@ -819,13 +975,13 @@
       </c>
       <c r="D3" s="9">
         <f>SUM(D7:D169)</f>
-        <v>2204487.4014114193</v>
+        <v>4.0903000000000009</v>
       </c>
       <c r="F3" t="s">
         <v>36</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I3" s="19">
         <f>SUM(I7:I11)</f>
@@ -853,7 +1009,7 @@
       </c>
       <c r="D4" s="8">
         <f>SQRT(D3 - D2^2)</f>
-        <v>1484.7516002841696</v>
+        <v>1.1924670854996382</v>
       </c>
       <c r="F4" t="s">
         <v>37</v>
@@ -931,13 +1087,13 @@
         <v>25</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J6" s="16" t="s">
         <v>1</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L6" s="16" t="s">
         <v>4</v>
@@ -951,18 +1107,18 @@
     </row>
     <row r="7" spans="1:40">
       <c r="A7" s="7">
-        <v>18000000</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>6.7800000000000002E-9</v>
+        <v>0.1663</v>
       </c>
       <c r="C7">
         <f>A7*B7</f>
-        <v>0.12204000000000001</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2">
         <f>(A7*A7)*B7</f>
-        <v>2196720</v>
+        <v>0</v>
       </c>
       <c r="F7" t="s">
         <v>40</v>
@@ -998,18 +1154,18 @@
     </row>
     <row r="8" spans="1:40">
       <c r="A8" s="7">
-        <v>200000</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>1.9000000000000001E-7</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="C8">
         <f t="shared" ref="C8:C71" si="0">A8*B8</f>
-        <v>3.7999999999999999E-2</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" ref="D8:D14" si="1">(A8*A8)*B8</f>
-        <v>7600</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="F8" t="s">
         <v>41</v>
@@ -1041,18 +1197,18 @@
     </row>
     <row r="9" spans="1:40">
       <c r="A9" s="7">
-        <v>10000</v>
+        <v>2</v>
       </c>
       <c r="B9">
-        <v>1.655E-6</v>
+        <v>0.27660000000000001</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>1.6549999999999999E-2</v>
+        <v>0.55320000000000003</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="1"/>
-        <v>165.5</v>
+        <v>1.1064000000000001</v>
       </c>
       <c r="F9" t="s">
         <v>42</v>
@@ -1094,18 +1250,18 @@
     </row>
     <row r="10" spans="1:40">
       <c r="A10">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>1.46627E-4</v>
+        <v>0.14960000000000001</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>1.4662700000000001E-2</v>
+        <v>0.44880000000000003</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="1"/>
-        <v>1.46627</v>
+        <v>1.3464</v>
       </c>
       <c r="H10" s="16">
         <v>4</v>
@@ -1145,18 +1301,18 @@
     </row>
     <row r="11" spans="1:40">
       <c r="A11">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>3.5445110000000002E-3</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>2.4811577000000001E-2</v>
+        <v>0.152</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="1"/>
-        <v>0.17368103900000001</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="H11" s="16">
         <v>5</v>
@@ -1193,18 +1349,18 @@
     </row>
     <row r="12" spans="1:40">
       <c r="A12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>6.3667649999999999E-3</v>
+        <v>2.75E-2</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>2.546706E-2</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="1"/>
-        <v>0.10186824</v>
+        <v>0.6875</v>
       </c>
       <c r="U12">
         <f>_xlfn.BINOM.DIST(3, X$9, X$10, FALSE)</f>
@@ -1227,22 +1383,16 @@
       </c>
     </row>
     <row r="13" spans="1:40">
-      <c r="A13">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>1.7732459999999999E-2</v>
-      </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>5.3197379999999996E-2</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="1"/>
-        <v>0.15959213999999999</v>
+        <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J13" s="19">
         <f>SUM(J7:J11)</f>
@@ -1265,12 +1415,6 @@
       </c>
     </row>
     <row r="14" spans="1:40">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>0.97220778521999995</v>
-      </c>
       <c r="C14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1392,7 +1536,7 @@
         <v>0</v>
       </c>
       <c r="V23" s="5">
-        <f>_xlfn.BINOM.DIST(U23,X$22,X$23, FALSE)</f>
+        <f t="shared" ref="V23:V29" si="4">_xlfn.BINOM.DIST(U23,X$22,X$23, FALSE)</f>
         <v>7.2900000000000037E-4</v>
       </c>
       <c r="W23" t="s">
@@ -1411,7 +1555,7 @@
         <v>1</v>
       </c>
       <c r="V24" s="5">
-        <f>_xlfn.BINOM.DIST(U24,X$22,X$23, FALSE)</f>
+        <f t="shared" si="4"/>
         <v>1.0206000000000015E-2</v>
       </c>
     </row>
@@ -1424,7 +1568,7 @@
         <v>2</v>
       </c>
       <c r="V25" s="5">
-        <f>_xlfn.BINOM.DIST(U25,X$22,X$23, FALSE)</f>
+        <f t="shared" si="4"/>
         <v>5.9535000000000053E-2</v>
       </c>
     </row>
@@ -1437,7 +1581,7 @@
         <v>3</v>
       </c>
       <c r="V26" s="5">
-        <f>_xlfn.BINOM.DIST(U26,X$22,X$23, FALSE)</f>
+        <f t="shared" si="4"/>
         <v>0.18522</v>
       </c>
     </row>
@@ -1450,7 +1594,7 @@
         <v>4</v>
       </c>
       <c r="V27" s="5">
-        <f>_xlfn.BINOM.DIST(U27,X$22,X$23, FALSE)</f>
+        <f t="shared" si="4"/>
         <v>0.32413500000000006</v>
       </c>
     </row>
@@ -1463,7 +1607,7 @@
         <v>5</v>
       </c>
       <c r="V28" s="5">
-        <f>_xlfn.BINOM.DIST(U28,X$22,X$23, FALSE)</f>
+        <f t="shared" si="4"/>
         <v>0.30252599999999991</v>
       </c>
     </row>
@@ -1476,7 +1620,7 @@
         <v>6</v>
       </c>
       <c r="V29" s="5">
-        <f>_xlfn.BINOM.DIST(U29,X$22,X$23, FALSE)</f>
+        <f t="shared" si="4"/>
         <v>0.11764899999999995</v>
       </c>
       <c r="Z29">
@@ -1764,931 +1908,931 @@
     </row>
     <row r="72" spans="3:3">
       <c r="C72">
-        <f t="shared" ref="C72:C135" si="4">A72*B72</f>
+        <f t="shared" ref="C72:C135" si="5">A72*B72</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="3:3">
       <c r="C73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="3:3">
       <c r="C74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="3:3">
       <c r="C75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="3:3">
       <c r="C76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="3:3">
       <c r="C77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="3:3">
       <c r="C78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="3:3">
       <c r="C79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="3:3">
       <c r="C80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="3:3">
       <c r="C98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="3:3">
       <c r="C99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="3:3">
       <c r="C100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="3:3">
       <c r="C101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="3:3">
       <c r="C102">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="3:3">
       <c r="C103">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="3:3">
       <c r="C104">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="3:3">
       <c r="C105">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="3:3">
       <c r="C106">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="3:3">
       <c r="C107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="3:3">
       <c r="C108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="109" spans="3:3">
       <c r="C109">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="3:3">
       <c r="C110">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="3:3">
       <c r="C111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="3:3">
       <c r="C112">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="3:3">
       <c r="C113">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="3:3">
       <c r="C114">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="3:3">
       <c r="C115">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="3:3">
       <c r="C116">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="3:3">
       <c r="C117">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="3:3">
       <c r="C118">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="3:3">
       <c r="C119">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="3:3">
       <c r="C120">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="3:3">
       <c r="C121">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="3:3">
       <c r="C122">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="3:3">
       <c r="C123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="3:3">
       <c r="C124">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="3:3">
       <c r="C125">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="3:3">
       <c r="C126">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="3:3">
       <c r="C127">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="3:3">
       <c r="C128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="3:3">
       <c r="C129">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="3:3">
       <c r="C130">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="3:3">
       <c r="C131">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="3:3">
       <c r="C132">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="3:3">
       <c r="C133">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="3:3">
       <c r="C134">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="3:3">
       <c r="C135">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="136" spans="3:3">
       <c r="C136">
-        <f t="shared" ref="C136:C199" si="5">A136*B136</f>
+        <f t="shared" ref="C136:C199" si="6">A136*B136</f>
         <v>0</v>
       </c>
     </row>
     <row r="137" spans="3:3">
       <c r="C137">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="3:3">
       <c r="C138">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="3:3">
       <c r="C139">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="140" spans="3:3">
       <c r="C140">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="141" spans="3:3">
       <c r="C141">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="142" spans="3:3">
       <c r="C142">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="143" spans="3:3">
       <c r="C143">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="144" spans="3:3">
       <c r="C144">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="145" spans="3:3">
       <c r="C145">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="146" spans="3:3">
       <c r="C146">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="147" spans="3:3">
       <c r="C147">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="148" spans="3:3">
       <c r="C148">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="149" spans="3:3">
       <c r="C149">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="150" spans="3:3">
       <c r="C150">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="151" spans="3:3">
       <c r="C151">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="152" spans="3:3">
       <c r="C152">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="153" spans="3:3">
       <c r="C153">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="154" spans="3:3">
       <c r="C154">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="155" spans="3:3">
       <c r="C155">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="156" spans="3:3">
       <c r="C156">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="157" spans="3:3">
       <c r="C157">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="158" spans="3:3">
       <c r="C158">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="159" spans="3:3">
       <c r="C159">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="160" spans="3:3">
       <c r="C160">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="161" spans="3:3">
       <c r="C161">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="162" spans="3:3">
       <c r="C162">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="163" spans="3:3">
       <c r="C163">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="164" spans="3:3">
       <c r="C164">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="165" spans="3:3">
       <c r="C165">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="166" spans="3:3">
       <c r="C166">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="167" spans="3:3">
       <c r="C167">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="168" spans="3:3">
       <c r="C168">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="169" spans="3:3">
       <c r="C169">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="170" spans="3:3">
       <c r="C170">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="171" spans="3:3">
       <c r="C171">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="172" spans="3:3">
       <c r="C172">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="173" spans="3:3">
       <c r="C173">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="174" spans="3:3">
       <c r="C174">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="175" spans="3:3">
       <c r="C175">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="176" spans="3:3">
       <c r="C176">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="177" spans="3:3">
       <c r="C177">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="178" spans="3:3">
       <c r="C178">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="179" spans="3:3">
       <c r="C179">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="180" spans="3:3">
       <c r="C180">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="181" spans="3:3">
       <c r="C181">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="182" spans="3:3">
       <c r="C182">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="183" spans="3:3">
       <c r="C183">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="184" spans="3:3">
       <c r="C184">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="185" spans="3:3">
       <c r="C185">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="186" spans="3:3">
       <c r="C186">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="187" spans="3:3">
       <c r="C187">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="188" spans="3:3">
       <c r="C188">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="189" spans="3:3">
       <c r="C189">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="190" spans="3:3">
       <c r="C190">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="191" spans="3:3">
       <c r="C191">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="192" spans="3:3">
       <c r="C192">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="193" spans="3:3">
       <c r="C193">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="194" spans="3:3">
       <c r="C194">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="195" spans="3:3">
       <c r="C195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="196" spans="3:3">
       <c r="C196">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="197" spans="3:3">
       <c r="C197">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="198" spans="3:3">
       <c r="C198">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="199" spans="3:3">
       <c r="C199">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="200" spans="3:3">
       <c r="C200">
-        <f t="shared" ref="C200:C226" si="6">A200*B200</f>
+        <f t="shared" ref="C200:C226" si="7">A200*B200</f>
         <v>0</v>
       </c>
     </row>
     <row r="201" spans="3:3">
       <c r="C201">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="202" spans="3:3">
       <c r="C202">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="203" spans="3:3">
       <c r="C203">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="204" spans="3:3">
       <c r="C204">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="205" spans="3:3">
       <c r="C205">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="206" spans="3:3">
       <c r="C206">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="207" spans="3:3">
       <c r="C207">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="208" spans="3:3">
       <c r="C208">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="209" spans="3:3">
       <c r="C209">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="210" spans="3:3">
       <c r="C210">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="211" spans="3:3">
       <c r="C211">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="212" spans="3:3">
       <c r="C212">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="213" spans="3:3">
       <c r="C213">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="214" spans="3:3">
       <c r="C214">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="215" spans="3:3">
       <c r="C215">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="216" spans="3:3">
       <c r="C216">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="217" spans="3:3">
       <c r="C217">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="218" spans="3:3">
       <c r="C218">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="219" spans="3:3">
       <c r="C219">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="220" spans="3:3">
       <c r="C220">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="221" spans="3:3">
       <c r="C221">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="222" spans="3:3">
       <c r="C222">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="223" spans="3:3">
       <c r="C223">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="224" spans="3:3">
       <c r="C224">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="225" spans="3:3">
       <c r="C225">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="226" spans="3:3">
       <c r="C226">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2699,12 +2843,226 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C96CE9-B77B-704D-8A1F-7836B7353FCF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="41.33203125" customWidth="1"/>
+    <col min="2" max="2" width="40" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" customWidth="1"/>
+    <col min="11" max="11" width="59.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="26">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="F2" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1252</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="2">
+        <v>129</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="F5" s="26"/>
+      <c r="G5" s="25"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1175</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="25">
+        <f>_xlfn.NORM.INV((G4/100),G2,G3)</f>
+        <v>17.773471879963388</v>
+      </c>
+      <c r="K6" s="27">
+        <f>_xlfn.NORM.DIST(0.39, 19, 1, TRUE)</f>
+        <v>1.3330875347022931E-77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="2">
+        <f xml:space="preserve"> (B6 - B3) / B4</f>
+        <v>-0.5968992248062015</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1400</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="2">
+        <f>(B9-B3) / B4</f>
+        <v>1.1472868217054264</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="2">
+        <f>_xlfn.NORM.DIST(B6,B3,B4,TRUE)</f>
+        <v>0.27528733243802045</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="2">
+        <f>_xlfn.NORM.DIST(B10,B3,B4,TRUE)</f>
+        <v>1.5595941023036459E-22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="B15" s="2">
+        <f>B13-B12</f>
+        <v>-0.27528733243802045</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1175</v>
+      </c>
+      <c r="C17">
+        <f>(B17-B3) / B4</f>
+        <v>-0.5968992248062015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="2">
+        <f xml:space="preserve"> 1 -_xlfn.NORM.DIST(1175, B3, B4, TRUE)</f>
+        <v>0.7247126675619795</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="25">
+        <v>2.2800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="25">
+        <v>0.47720000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="25">
+        <f>(0.5 - B28) + B27</f>
+        <v>4.5599999999999988E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2762,7 +3120,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="12">
         <f>_xlfn.BINOM.DIST(B$2, B$3, B$4, FALSE)</f>
@@ -2771,7 +3129,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="12">
         <f>_xlfn.BINOM.DIST(B$2 - 1, B$3, B$4, TRUE)</f>
@@ -2780,7 +3138,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="12">
         <f>_xlfn.BINOM.DIST(B$2, B$3, B$4, TRUE)</f>
@@ -2789,7 +3147,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="12">
         <f xml:space="preserve"> 1 - B9</f>
@@ -2798,7 +3156,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <f>1 - _xlfn.BINOM.DIST(B$2 - 1, B$3, B$4, FALSE)</f>
@@ -2834,17 +3192,17 @@
     </row>
     <row r="18" spans="1:1" ht="17">
       <c r="A18" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="17">
       <c r="A19" s="15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="17">
       <c r="A20" s="15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2922,44 +3280,124 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7883183-3309-E141-80C9-0F546E3ED993}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A6:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1">
-        <v>7</v>
-      </c>
-      <c r="B1">
-        <f>37/38</f>
-        <v>0.97368421052631582</v>
-      </c>
-      <c r="C1">
-        <f>A1*B1</f>
-        <v>6.8157894736842106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>-245</v>
-      </c>
-      <c r="B2">
-        <f>1/38</f>
-        <v>2.6315789473684209E-2</v>
-      </c>
-      <c r="C2">
-        <f>A2*B2</f>
-        <v>-6.447368421052631</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="C3">
-        <f>SUM(C1:C2)</f>
-        <v>0.36842105263157965</v>
+    <row r="6" spans="1:4">
+      <c r="C6" s="31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="C7" s="30">
+        <f>SUM(C10:C17)</f>
+        <v>1.6335</v>
+      </c>
+      <c r="D7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="7">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0.1663</v>
+      </c>
+      <c r="C10">
+        <f>A10*B10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="7">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:C17" si="0">A11*B11</f>
+        <v>0.34200000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="7">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>0.27660000000000001</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0.55320000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>0.14960000000000001</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0.44880000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0.152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>2.75E-2</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0.13750000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2969,103 +3407,413 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD5251E-A9B7-7F4B-A78E-2F9C7E161BB7}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17">
+    <row r="1" spans="1:8" ht="17">
       <c r="A1" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17">
+      <c r="A2" s="15" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17">
-      <c r="A2" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17">
+    <row r="3" spans="1:8" ht="17">
       <c r="A3" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17">
       <c r="A5" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17">
+      <c r="A6" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="33">
+        <v>0.12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="B7" s="2"/>
+      <c r="G7" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17">
+      <c r="A8" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="33">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8">
+        <f>H6*H7</f>
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17">
+      <c r="A9" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17">
+      <c r="A10" s="21" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="17">
-      <c r="A6" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="17">
-      <c r="A7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="20">
+      <c r="B10" s="33">
+        <v>1.68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10">
+        <f>B6*B8</f>
+        <v>1.68</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17">
-      <c r="A8" s="21" t="s">
+    <row r="11" spans="1:8" ht="26">
+      <c r="A11" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="17">
-      <c r="A9" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="20">
-        <f>B6*B8</f>
+      <c r="B11" s="2"/>
+      <c r="G11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17">
+      <c r="A12" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="33">
+        <f>_xlfn.POISSON.DIST(B9,B10, FALSE)</f>
+        <v>5.8198054157415332E-3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17">
+      <c r="A13" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="33">
+        <f>_xlfn.POISSON.DIST(B9 - 1, B10, TRUE)</f>
+        <v>0.99242454151988369</v>
+      </c>
+      <c r="G13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="17">
+      <c r="A14" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="33">
+        <f>1 - B13</f>
+        <v>7.575458480116315E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="17">
+      <c r="A16" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17">
+      <c r="A17" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17">
+      <c r="A18" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="16">
+        <f>B16</f>
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <f>_xlfn.POISSON.DIST(A19, B$10, FALSE)</f>
+        <v>6.1860176612899005E-2</v>
+      </c>
+      <c r="C19" t="str">
+        <f>IF(A19&gt;B$17,"ERASE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="16">
+        <f>A19+1</f>
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ref="B20:B26" si="0">_xlfn.POISSON.DIST(A20, B$10, FALSE)</f>
+        <v>2.0785019341934056E-2</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" ref="C20:C26" si="1">IF(A20&gt;B$17,"ERASE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="16">
+        <f t="shared" ref="A21:A26" si="2">A20+1</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="26">
-      <c r="A11" s="24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="17">
-      <c r="A12" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="20">
-        <f>_xlfn.POISSON.DIST(B7,B9, FALSE)</f>
-        <v>0.16062314104798003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="17">
-      <c r="A13" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="20">
-        <f>_xlfn.POISSON.DIST(B7 - 1, B9, TRUE)</f>
-        <v>0.44567964136461113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="17">
-      <c r="A14" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="20">
-        <f>1 - B13</f>
-        <v>0.55432035863538887</v>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>5.8198054157415332E-3</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="16">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>1.3967532997779695E-3</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="16">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>2.9331819295337359E-4</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="1"/>
+        <v>ERASE</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="16">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>5.4752729351296345E-5</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="1"/>
+        <v>ERASE</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="16">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>9.1984585310177959E-6</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="1"/>
+        <v>ERASE</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="16">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>1.4048554847372632E-6</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="1"/>
+        <v>ERASE</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" s="20">
+        <f>SUMIF(C19:C26,"",B19:B26)</f>
+        <v>8.9861754670352567E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41">
+        <v>106</v>
+      </c>
+      <c r="E41">
+        <f>_xlfn.POISSON.DIST(6, 7.2, FALSE)</f>
+        <v>0.14445820444290103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>0.34905660379999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="20">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" s="20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49">
+        <f>B47*B48</f>
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52">
+        <f>_xlfn.POISSON.DIST(B51, B49, FALSE)</f>
+        <v>0.13372702354142837</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>109</v>
+      </c>
+      <c r="B53">
+        <f>_xlfn.POISSON.DIST(B51 - 1, B49, TRUE)</f>
+        <v>0.56894123888215242</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54">
+        <f xml:space="preserve"> 1 - B53</f>
+        <v>0.43105876111784758</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56">
+        <f>_xlfn.POISSON.DIST(1, 7.2, FALSE)</f>
+        <v>5.3754178203120903E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57">
+        <f xml:space="preserve"> 1 - A56</f>
+        <v>0.99462458217968786</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B197D298-ED68-BB49-99FA-0C7491034B92}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Normal distribution neg/pos z-score formula
</commit_message>
<xml_diff>
--- a/Midterm Excel Sheet.xlsx
+++ b/Midterm Excel Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanninoa/Desktop/Business-Stats-Excel-Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2FE2ED-D55D-D345-9581-29434AFA7836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7FE551-DBE2-334A-BFBF-6528D706A46F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" activeTab="5" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" activeTab="1" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
   </bookViews>
   <sheets>
     <sheet name="Random Variable x" sheetId="1" r:id="rId1"/>
@@ -2845,8 +2845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C96CE9-B77B-704D-8A1F-7836B7353FCF}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3042,7 +3042,11 @@
         <v>81</v>
       </c>
       <c r="B27" s="25">
-        <v>2.2800000000000001E-2</v>
+        <v>-2.61</v>
+      </c>
+      <c r="C27">
+        <f>_xlfn.NORM.DIST(B27, 0, 1, TRUE)</f>
+        <v>4.5271111329673241E-3</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -3050,7 +3054,11 @@
         <v>82</v>
       </c>
       <c r="B28" s="25">
-        <v>0.47720000000000001</v>
+        <v>1.61</v>
+      </c>
+      <c r="C28">
+        <f>1 - _xlfn.NORM.DIST(B28, 0, 1, TRUE)</f>
+        <v>5.3698928148119718E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -3058,8 +3066,8 @@
         <v>83</v>
       </c>
       <c r="B29" s="25">
-        <f>(0.5 - B28) + B27</f>
-        <v>4.5599999999999988E-2</v>
+        <f>SUM(C27:C28)</f>
+        <v>5.8226039281087043E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3409,7 +3417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD5251E-A9B7-7F4B-A78E-2F9C7E161BB7}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add Normal Distribution formulas
</commit_message>
<xml_diff>
--- a/Midterm Excel Sheet.xlsx
+++ b/Midterm Excel Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanninoa/Desktop/Business-Stats-Excel-Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7FE551-DBE2-334A-BFBF-6528D706A46F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3A3623-D9D3-B549-A7F6-93C01C045B4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" activeTab="1" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <sheet name="x &amp; Probability" sheetId="4" r:id="rId4"/>
     <sheet name="Expected Value" sheetId="5" r:id="rId5"/>
     <sheet name="Poisson" sheetId="3" r:id="rId6"/>
-    <sheet name="Poisson v2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="163">
   <si>
     <t>x</t>
   </si>
@@ -369,6 +368,165 @@
   </si>
   <si>
     <t>Fewer than X</t>
+  </si>
+  <si>
+    <t>Negative Z-score</t>
+  </si>
+  <si>
+    <t>Positive Z-score</t>
+  </si>
+  <si>
+    <t>Middle X%</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>% -&gt; Proportion</t>
+  </si>
+  <si>
+    <t>Area in each tail</t>
+  </si>
+  <si>
+    <t>lower-tail z-score</t>
+  </si>
+  <si>
+    <t>upper-tail z-score</t>
+  </si>
+  <si>
+    <t>Ex: The mean incubation time of fertilized eggs is 19 days. Suppose the incubation times are approximately normally distributed with a standard deviation of 1 day. Determine the 11th percentile for incubation times.</t>
+  </si>
+  <si>
+    <t>X1 (area to the left of the %precentile)</t>
+  </si>
+  <si>
+    <t>x2(area of left + percentile)</t>
+  </si>
+  <si>
+    <t>Proportion of Percentile</t>
+  </si>
+  <si>
+    <t>Zsub1</t>
+  </si>
+  <si>
+    <t>Zsub2</t>
+  </si>
+  <si>
+    <t>(1 - alpha)</t>
+  </si>
+  <si>
+    <t>z-score</t>
+  </si>
+  <si>
+    <t>Simple Z-score to area</t>
+  </si>
+  <si>
+    <t>α</t>
+  </si>
+  <si>
+    <t>Zα</t>
+  </si>
+  <si>
+    <t>Area (1 - α)</t>
+  </si>
+  <si>
+    <t>Normal Distribution on variable X w/ Mean and SD</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>P(x &lt;= val)</t>
+  </si>
+  <si>
+    <t>Answer (xth percentile)</t>
+  </si>
+  <si>
+    <t>Probability of a Normal Random Variable</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>upper</t>
+  </si>
+  <si>
+    <t>P(lower &lt;= x &lt;= upper)</t>
+  </si>
+  <si>
+    <t>p(x &lt; lower)</t>
+  </si>
+  <si>
+    <t>(Make sure to change values for certain individual questions)</t>
+  </si>
+  <si>
+    <t>p (x &gt; upper)</t>
+  </si>
+  <si>
+    <t>Percentile (change lower bound)</t>
+  </si>
+  <si>
+    <t>Middle X% w/ Mean &amp; SD</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Proportion</t>
+  </si>
+  <si>
+    <t>X (Answer)</t>
+  </si>
+  <si>
+    <t>Middle %</t>
+  </si>
+  <si>
+    <t>middle Proportion</t>
+  </si>
+  <si>
+    <t>X1 (lower-bound)</t>
+  </si>
+  <si>
+    <t>X2 (upper-bound)</t>
+  </si>
+  <si>
+    <t>IQR</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Determine the # of items that make up the middle % (Make sure to change percentile)</t>
+  </si>
+  <si>
+    <t>Time Requred, mean, SD, x</t>
+  </si>
+  <si>
+    <t>x (minutes)</t>
+  </si>
+  <si>
+    <t>Percent(x &gt; time)</t>
+  </si>
+  <si>
+    <t>​for later: (b) If the automotive center does not want to give the discount to more than 55% of its​ customers, how long should it make the guaranteed time​ limit?</t>
+  </si>
+  <si>
+    <t>Calculate Z-score</t>
+  </si>
+  <si>
+    <t>Score A</t>
+  </si>
+  <si>
+    <t>Score B</t>
+  </si>
+  <si>
+    <t>Z-score</t>
+  </si>
+  <si>
+    <t>Find val of Zα</t>
   </si>
 </sst>
 </file>
@@ -381,7 +539,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.000000000000000000000_);_(* \(#,##0.000000000000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="215" formatCode="0.0000000000000000000000000000000000000000000000000000E+00"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -462,6 +620,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF7030A0"/>
@@ -471,19 +636,35 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue Light"/>
+      <color rgb="FFBD00C7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -500,12 +681,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -559,18 +781,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="215" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -579,6 +793,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="215" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2843,232 +3109,702 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C96CE9-B77B-704D-8A1F-7836B7353FCF}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:AG33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="41.33203125" customWidth="1"/>
     <col min="2" max="2" width="40" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" customWidth="1"/>
-    <col min="11" max="11" width="59.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="36.33203125" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" customWidth="1"/>
+    <col min="24" max="24" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26">
-      <c r="A1" t="s">
+    <row r="1" spans="1:33" ht="26">
+      <c r="A1" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="D1" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="E1" s="2"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="F2" s="26" t="s">
+      <c r="J1" s="46"/>
+      <c r="N1" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="O1" s="33"/>
+      <c r="Q1" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="R1" s="33"/>
+      <c r="T1" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="X1" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y1" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
+      <c r="A2" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="E2" s="2"/>
+      <c r="H2" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="47"/>
+      <c r="N2" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="O2" s="33">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="33">
+        <v>19</v>
+      </c>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="X2" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y2" s="51">
+        <v>0.18</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC2">
+        <v>-1.72</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
+      <c r="A3" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="37">
+        <v>1252</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1252</v>
+      </c>
+      <c r="H3" s="33"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="47"/>
+      <c r="N3" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="O3" s="33">
+        <f>O2/100</f>
+        <v>0.39</v>
+      </c>
+      <c r="Q3" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="R3" s="33">
+        <v>3</v>
+      </c>
+      <c r="T3" s="33"/>
+      <c r="U3" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="V3" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="X3" s="36"/>
+      <c r="Y3" s="51"/>
+      <c r="AF3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33">
+      <c r="A4" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="37">
+        <v>129</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2">
+        <v>129</v>
+      </c>
+      <c r="H4" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="25">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
+      <c r="I4" s="43">
+        <v>1262</v>
+      </c>
+      <c r="J4" s="47"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="Q4" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="R4" s="33">
+        <v>20</v>
+      </c>
+      <c r="T4" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="U4" s="33">
+        <v>25</v>
+      </c>
+      <c r="V4" s="33">
+        <v>1229</v>
+      </c>
+      <c r="X4" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y4" s="51">
+        <f xml:space="preserve"> 1 - Y2</f>
+        <v>0.82000000000000006</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC4">
+        <f>_xlfn.NORM.S.DIST(AC2, TRUE)</f>
+        <v>4.2716220791328911E-2</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>131</v>
+      </c>
+      <c r="AG4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33">
+      <c r="A5" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="37">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="H5" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="44">
+        <v>118</v>
+      </c>
+      <c r="J5" s="47"/>
+      <c r="N5" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="O5" s="33">
+        <f xml:space="preserve"> (1 - O3) / 2</f>
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="T5" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="U5" s="33">
+        <v>21.4</v>
+      </c>
+      <c r="V5" s="33">
+        <v>1026</v>
+      </c>
+      <c r="X5" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y5" s="51">
+        <f>_xlfn.NORM.INV(Y4,0, 1)</f>
+        <v>0.91536508784281367</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33">
+      <c r="A6" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="37">
+        <v>1225</v>
+      </c>
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1100</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="44">
+        <v>97</v>
+      </c>
+      <c r="J6" s="47"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="33"/>
+      <c r="Q6" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="R6" s="33">
+        <f>(1 - _xlfn.NORM.DIST(R4,R2,R3, TRUE)) * 100</f>
+        <v>36.944134018176356</v>
+      </c>
+      <c r="T6" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="U6" s="33">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="V6" s="33">
+        <v>203</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>132</v>
+      </c>
+      <c r="AG6">
+        <f>_xlfn.NORM.DIST(AG2,AG3,AG4, TRUE)</f>
+        <v>0.42074029056089696</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33">
+      <c r="A7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="2">
+        <f xml:space="preserve"> (E6 - E3) / E4</f>
+        <v>-1.1782945736434109</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="I7" s="44">
+        <f>I6/100</f>
+        <v>0.97</v>
+      </c>
+      <c r="J7" s="47"/>
+      <c r="N7" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="O7" s="33">
+        <f>_xlfn.NORM.DIST(O5, 0, 1, TRUE)</f>
+        <v>0.61981692384016507</v>
+      </c>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33">
+        <f>NORMINV(0.07,19,2.5)</f>
+        <v>15.310522429552075</v>
+      </c>
+      <c r="T7" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="U7" s="33">
+        <f>(U4-U5)/U6</f>
+        <v>0.70588235294117685</v>
+      </c>
+      <c r="V7" s="33">
+        <f>(V4-V5)/V6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33">
+      <c r="A8" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="37">
+        <f>_xlfn.NORM.DIST(B6, B3, B4, TRUE) - _xlfn.NORM.DIST(B5, B3, B4, TRUE)</f>
+        <v>0.39172524132251257</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="47"/>
+      <c r="N8" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="O8" s="33">
+        <f>_xlfn.NORM.DIST(O5, 0, 1, TRUE)</f>
+        <v>0.61981692384016507</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" ht="19">
+      <c r="A9" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="37">
+        <f>_xlfn.NORM.DIST(B5,B3,B4,TRUE)</f>
+        <v>2.5380876893736339E-2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1400</v>
+      </c>
+      <c r="H9" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="I9" s="50">
+        <f>_xlfn.NORM.INV(($I$6/100),I$4,I$5)</f>
+        <v>1483.9336457618476</v>
+      </c>
+      <c r="J9" s="47"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="Q9" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="R9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" ht="17">
+      <c r="A10" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="37">
+        <f>1 - _xlfn.NORM.DIST(B6, B3, B4, TRUE)</f>
+        <v>0.58289388178375101</v>
+      </c>
+      <c r="D10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="2">
+        <f>(E9-E3) / E4</f>
+        <v>1.1472868217054264</v>
+      </c>
+      <c r="H10" s="33"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="48"/>
+      <c r="N10" s="33">
+        <f>_xlfn.NORM.INV(0.79, 0, 1)</f>
+        <v>0.80642124701824058</v>
+      </c>
+      <c r="O10" s="33"/>
+      <c r="Q10" s="21"/>
+    </row>
+    <row r="11" spans="1:33" ht="17">
+      <c r="A11" s="36"/>
+      <c r="B11" s="37"/>
+      <c r="E11" s="2"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="47"/>
+      <c r="Q11" s="21"/>
+    </row>
+    <row r="12" spans="1:33">
+      <c r="A12" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="37">
+        <f>B9*100</f>
+        <v>2.5380876893736337</v>
+      </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="2">
+        <f>_xlfn.NORM.DIST(E6,E3,E4,TRUE)</f>
+        <v>0.11933959517437347</v>
+      </c>
+      <c r="H12" s="33"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="48"/>
+    </row>
+    <row r="13" spans="1:33">
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="2">
+        <f>_xlfn.NORM.DIST(E10,E3,E4,TRUE)</f>
+        <v>1.5595941023036459E-22</v>
+      </c>
+      <c r="H13" s="33"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="47"/>
+    </row>
+    <row r="14" spans="1:33">
+      <c r="E14" s="2"/>
+      <c r="H14" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="I14" s="41">
+        <f>(1 - I7)/2</f>
+        <v>1.5000000000000013E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33">
+      <c r="E15" s="2">
+        <f>E13-E12</f>
+        <v>-0.11933959517437347</v>
+      </c>
+      <c r="H15" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="I15" s="41">
+        <f>I7+I14</f>
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="N15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33">
+      <c r="E16" s="2"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="41"/>
+      <c r="N16" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="2">
-        <v>1252</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="2">
-        <v>129</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" s="25">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="F5" s="26"/>
-      <c r="G5" s="25"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="O16">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="17" spans="4:15">
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="2">
         <v>1175</v>
       </c>
-      <c r="F6" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="G6" s="25">
-        <f>_xlfn.NORM.INV((G4/100),G2,G3)</f>
-        <v>17.773471879963388</v>
-      </c>
-      <c r="K6" s="27">
-        <f>_xlfn.NORM.DIST(0.39, 19, 1, TRUE)</f>
-        <v>1.3330875347022931E-77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="2">
-        <f xml:space="preserve"> (B6 - B3) / B4</f>
-        <v>-0.5968992248062015</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1400</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="2">
-        <f>(B9-B3) / B4</f>
-        <v>1.1472868217054264</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="2">
-        <f>_xlfn.NORM.DIST(B6,B3,B4,TRUE)</f>
-        <v>0.27528733243802045</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="2">
-        <f>_xlfn.NORM.DIST(B10,B3,B4,TRUE)</f>
-        <v>1.5595941023036459E-22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="B15" s="2">
-        <f>B13-B12</f>
-        <v>-0.27528733243802045</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="2">
-        <v>1175</v>
-      </c>
-      <c r="C17">
-        <f>(B17-B3) / B4</f>
-        <v>-0.5968992248062015</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+      <c r="H17" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="I17" s="41">
+        <f>NORMINV(I14, 0, 1)</f>
+        <v>-2.1700903775845601</v>
+      </c>
+      <c r="N17" t="s">
+        <v>131</v>
+      </c>
+      <c r="O17">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="4:15">
+      <c r="D18" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="2">
-        <f xml:space="preserve"> 1 -_xlfn.NORM.DIST(1175, B3, B4, TRUE)</f>
+      <c r="E18" s="2">
+        <f xml:space="preserve"> 1 -_xlfn.NORM.DIST(1175, E3, E4, TRUE)</f>
         <v>0.7247126675619795</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="B19" s="2" t="s">
+      <c r="H18" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="I18" s="41">
+        <f>NORMINV(I15, 0, 1)</f>
+        <v>2.1700903775845601</v>
+      </c>
+      <c r="N18" t="s">
+        <v>143</v>
+      </c>
+      <c r="O18">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="4:15">
+      <c r="E19" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="N19" t="s">
+        <v>144</v>
+      </c>
+      <c r="O19">
+        <f>O18/100</f>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="4:15">
+      <c r="D20" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
+      <c r="E20" s="2"/>
+      <c r="H20" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+    </row>
+    <row r="21" spans="4:15">
+      <c r="D21" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
+      <c r="E21" s="2"/>
+      <c r="H21" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="I21" s="32">
+        <f>I4 + (I17)*I5</f>
+        <v>1005.9293354450219</v>
+      </c>
+      <c r="N21" t="s">
+        <v>146</v>
+      </c>
+      <c r="O21">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="4:15">
+      <c r="E22" s="2"/>
+      <c r="H22" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="I22" s="32">
+        <f>I4+(I18*I5)</f>
+        <v>1518.0706645549781</v>
+      </c>
+      <c r="N22" t="s">
+        <v>147</v>
+      </c>
+      <c r="O22">
+        <f>O21/100</f>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="23" spans="4:15">
+      <c r="D23" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
+      <c r="E23" s="2"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+    </row>
+    <row r="24" spans="4:15">
+      <c r="E24" s="2"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+    </row>
+    <row r="25" spans="4:15">
+      <c r="E25" s="2"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+    </row>
+    <row r="26" spans="4:15">
+      <c r="D26" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
+      <c r="E26" s="2"/>
+      <c r="H26" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="I26" s="32">
+        <f>I28-I27</f>
+        <v>159.17958104627542</v>
+      </c>
+    </row>
+    <row r="27" spans="4:15">
+      <c r="D27" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="25">
+      <c r="E27" s="29">
         <v>-2.61</v>
       </c>
-      <c r="C27">
-        <f>_xlfn.NORM.DIST(B27, 0, 1, TRUE)</f>
+      <c r="H27" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="I27" s="31">
+        <f>_xlfn.NORM.INV((25/100),I$4,I$5)</f>
+        <v>1182.4102094768623</v>
+      </c>
+    </row>
+    <row r="28" spans="4:15">
+      <c r="D28" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="29">
+        <v>1.61</v>
+      </c>
+      <c r="H28" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="I28" s="31">
+        <f>_xlfn.NORM.INV((75/100),I$4,I$5)</f>
+        <v>1341.5897905231377</v>
+      </c>
+    </row>
+    <row r="29" spans="4:15">
+      <c r="D29" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" s="29">
+        <f>_xlfn.NORM.DIST(E27, 0, 1, TRUE)</f>
         <v>4.5271111329673241E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="25">
-        <v>1.61</v>
-      </c>
-      <c r="C28">
-        <f>1 - _xlfn.NORM.DIST(B28, 0, 1, TRUE)</f>
+    <row r="30" spans="4:15">
+      <c r="D30" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" s="29">
+        <f>1 - _xlfn.NORM.DIST(E28, 0, 1, TRUE)</f>
         <v>5.3698928148119718E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="28" t="s">
+    <row r="31" spans="4:15">
+      <c r="D31" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="25">
-        <f>SUM(C27:C28)</f>
+      <c r="E31" s="29">
+        <f>SUM(E29:E30)</f>
         <v>5.8226039281087043E-2</v>
       </c>
+      <c r="N31" t="s">
+        <v>145</v>
+      </c>
+      <c r="O31">
+        <f>NORMINV(0.28,1264,116)</f>
+        <v>1196.390385156539</v>
+      </c>
+    </row>
+    <row r="32" spans="4:15">
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3297,12 +4033,12 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="6" spans="1:4">
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="27" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="C7" s="30">
+      <c r="C7" s="26">
         <f>SUM(C10:C17)</f>
         <v>1.6335</v>
       </c>
@@ -3417,7 +4153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD5251E-A9B7-7F4B-A78E-2F9C7E161BB7}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
@@ -3455,7 +4191,7 @@
       <c r="A6" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="29">
         <v>0.12</v>
       </c>
       <c r="G6" t="s">
@@ -3478,7 +4214,7 @@
       <c r="A8" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="29">
         <v>14</v>
       </c>
       <c r="G8" t="s">
@@ -3493,7 +4229,7 @@
       <c r="A9" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="29">
         <v>6</v>
       </c>
     </row>
@@ -3501,7 +4237,7 @@
       <c r="A10" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="29">
         <v>1.68</v>
       </c>
       <c r="C10" t="s">
@@ -3531,7 +4267,7 @@
       <c r="A12" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12" s="29">
         <f>_xlfn.POISSON.DIST(B9,B10, FALSE)</f>
         <v>5.8198054157415332E-3</v>
       </c>
@@ -3543,7 +4279,7 @@
       <c r="A13" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="29">
         <f>_xlfn.POISSON.DIST(B9 - 1, B10, TRUE)</f>
         <v>0.99242454151988369</v>
       </c>
@@ -3555,7 +4291,7 @@
       <c r="A14" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="29">
         <f>1 - B13</f>
         <v>7.575458480116315E-3</v>
       </c>
@@ -3694,7 +4430,7 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="25" t="s">
         <v>97</v>
       </c>
       <c r="B27" s="20">
@@ -3703,7 +4439,7 @@
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="28" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3812,16 +4548,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B197D298-ED68-BB49-99FA-0C7491034B92}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Norm Dist functions
</commit_message>
<xml_diff>
--- a/Midterm Excel Sheet.xlsx
+++ b/Midterm Excel Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanninoa/Desktop/Business-Stats-Excel-Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3A3623-D9D3-B549-A7F6-93C01C045B4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A05C66-6DB8-384F-9130-62FB7AD2AB3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" activeTab="1" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="165">
   <si>
     <t>x</t>
   </si>
@@ -527,6 +527,12 @@
   </si>
   <si>
     <t>Find val of Zα</t>
+  </si>
+  <si>
+    <t>MOVE THIS^^^^^</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIND OUT HOW TO DO Z SCORE </t>
   </si>
 </sst>
 </file>
@@ -794,9 +800,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -845,6 +848,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3109,10 +3115,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C96CE9-B77B-704D-8A1F-7836B7353FCF}">
-  <dimension ref="A1:AG33"/>
+  <dimension ref="A1:AI34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3121,690 +3127,712 @@
     <col min="2" max="2" width="40" style="2" customWidth="1"/>
     <col min="4" max="4" width="41.33203125" customWidth="1"/>
     <col min="5" max="5" width="22.5" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
-    <col min="8" max="8" width="36.33203125" customWidth="1"/>
+    <col min="6" max="6" width="3.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="40.83203125" customWidth="1"/>
+    <col min="10" max="10" width="35.5" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="16" max="16" width="24.6640625" customWidth="1"/>
     <col min="17" max="17" width="14.6640625" customWidth="1"/>
     <col min="24" max="24" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="26">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:35" ht="26">
+      <c r="A1" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="D1" t="s">
+      <c r="B1" s="34"/>
+      <c r="D1" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="38" t="s">
+      <c r="E1" s="34"/>
+      <c r="G1" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="34"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="46"/>
-      <c r="N1" s="32" t="s">
+      <c r="L1" s="45"/>
+      <c r="P1" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="O1" s="33"/>
-      <c r="Q1" s="33" t="s">
+      <c r="Q1" s="32"/>
+      <c r="S1" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="R1" s="33"/>
-      <c r="T1" s="33" t="s">
+      <c r="T1" s="32"/>
+      <c r="V1" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="X1" s="33" t="s">
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Z1" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="Y1" s="33" t="s">
+      <c r="AA1" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AE1" s="32"/>
+      <c r="AH1" s="32" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="2" spans="1:33">
-      <c r="A2" s="36" t="s">
+      <c r="AI1" s="32"/>
+    </row>
+    <row r="2" spans="1:35">
+      <c r="A2" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="E2" s="2"/>
-      <c r="H2" s="33" t="s">
+      <c r="B2" s="34"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="34"/>
+      <c r="G2" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="36">
+        <v>-0.89</v>
+      </c>
+      <c r="J2" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="K2" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="47"/>
-      <c r="N2" s="33" t="s">
+      <c r="L2" s="46"/>
+      <c r="P2" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="O2" s="33">
+      <c r="Q2" s="32">
         <v>39</v>
       </c>
-      <c r="Q2" s="33" t="s">
+      <c r="S2" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="33">
-        <v>19</v>
-      </c>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="X2" s="36" t="s">
+      <c r="T2" s="32">
+        <v>50</v>
+      </c>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Z2" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="Y2" s="51">
+      <c r="AA2" s="50">
         <v>0.18</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="AC2">
+      <c r="AE2" s="32">
         <v>-1.72</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="AG2">
+      <c r="AI2" s="32">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
-      <c r="A3" s="36" t="s">
+    <row r="3" spans="1:35">
+      <c r="A3" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="36">
+        <v>50</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="34">
         <v>1252</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="36">
+        <v>1.88</v>
+      </c>
+      <c r="J3" s="32"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="46"/>
+      <c r="P3" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q3" s="32">
+        <f>Q2/100</f>
+        <v>0.39</v>
+      </c>
+      <c r="S3" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="T3" s="32">
+        <v>7</v>
+      </c>
+      <c r="V3" s="32"/>
+      <c r="W3" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="X3" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z3" s="35"/>
+      <c r="AA3" s="50"/>
+      <c r="AD3" s="32"/>
+      <c r="AE3" s="32"/>
+      <c r="AH3" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="2">
-        <v>1252</v>
-      </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="47"/>
-      <c r="N3" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="O3" s="33">
-        <f>O2/100</f>
-        <v>0.39</v>
-      </c>
-      <c r="Q3" s="33" t="s">
+      <c r="AI3" s="32">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35">
+      <c r="A4" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="36">
+        <v>7</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="34">
+        <v>129</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" s="36">
+        <f>_xlfn.NORM.DIST(H2, 0, 1, TRUE)</f>
+        <v>0.18673294303717258</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" s="42">
+        <v>49</v>
+      </c>
+      <c r="L4" s="46"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="S4" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="T4" s="32">
+        <v>41</v>
+      </c>
+      <c r="V4" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="W4" s="32">
+        <v>25</v>
+      </c>
+      <c r="X4" s="32">
+        <v>1156</v>
+      </c>
+      <c r="Z4" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA4" s="50">
+        <f xml:space="preserve"> 1 - AA2</f>
+        <v>0.82000000000000006</v>
+      </c>
+      <c r="AD4" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE4" s="32">
+        <f>_xlfn.NORM.S.DIST(AE2, TRUE)</f>
+        <v>4.2716220791328911E-2</v>
+      </c>
+      <c r="AH4" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="R3" s="33">
-        <v>3</v>
-      </c>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="V3" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="X3" s="36"/>
-      <c r="Y3" s="51"/>
-      <c r="AF3" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG3">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33">
-      <c r="A4" s="36" t="s">
+      <c r="AI4" s="32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35">
+      <c r="A5" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="36">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="34"/>
+      <c r="G5" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="36">
+        <f>1 - _xlfn.NORM.DIST(H3, 0, 1, TRUE)</f>
+        <v>3.0054038961199736E-2</v>
+      </c>
+      <c r="J5" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="37">
-        <v>129</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="2">
-        <v>129</v>
-      </c>
-      <c r="H4" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" s="43">
-        <v>1262</v>
-      </c>
-      <c r="J4" s="47"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="Q4" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="R4" s="33">
-        <v>20</v>
-      </c>
-      <c r="T4" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="U4" s="33">
-        <v>25</v>
-      </c>
-      <c r="V4" s="33">
-        <v>1229</v>
-      </c>
-      <c r="X4" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y4" s="51">
-        <f xml:space="preserve"> 1 - Y2</f>
-        <v>0.82000000000000006</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC4">
-        <f>_xlfn.NORM.S.DIST(AC2, TRUE)</f>
-        <v>4.2716220791328911E-2</v>
-      </c>
-      <c r="AF4" t="s">
+      <c r="K5" s="43">
+        <v>5</v>
+      </c>
+      <c r="L5" s="46"/>
+      <c r="P5" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q5" s="32">
+        <f xml:space="preserve"> (1 - Q3) / 2</f>
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+      <c r="V5" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="W5" s="32">
+        <v>21.3</v>
+      </c>
+      <c r="X5" s="32">
+        <v>1037</v>
+      </c>
+      <c r="Z5" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA5" s="50">
+        <f>_xlfn.NORM.INV(AA4,0, 1)</f>
+        <v>0.91536508784281367</v>
+      </c>
+      <c r="AH5" s="32"/>
+      <c r="AI5" s="32"/>
+    </row>
+    <row r="6" spans="1:35">
+      <c r="A6" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="36">
+        <v>41</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="34">
+        <v>1100</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="36">
+        <f>SUM(H4:H5)</f>
+        <v>0.21678698199837232</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="K6" s="43">
+        <v>15</v>
+      </c>
+      <c r="L6" s="46"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="32"/>
+      <c r="S6" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="T6" s="32">
+        <f>(1 - _xlfn.NORM.DIST(T4,T2,T3, TRUE)) * 100</f>
+        <v>90.072860315666901</v>
+      </c>
+      <c r="V6" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="AG4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33">
-      <c r="A5" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="B5" s="37">
-        <v>1000</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="H5" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="44">
-        <v>118</v>
-      </c>
-      <c r="J5" s="47"/>
-      <c r="N5" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="O5" s="33">
-        <f xml:space="preserve"> (1 - O3) / 2</f>
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
-      <c r="T5" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="U5" s="33">
-        <v>21.4</v>
-      </c>
-      <c r="V5" s="33">
-        <v>1026</v>
-      </c>
-      <c r="X5" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y5" s="51">
-        <f>_xlfn.NORM.INV(Y4,0, 1)</f>
-        <v>0.91536508784281367</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33">
-      <c r="A6" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="B6" s="37">
-        <v>1225</v>
-      </c>
-      <c r="D6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1100</v>
-      </c>
-      <c r="H6" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="I6" s="44">
-        <v>97</v>
-      </c>
-      <c r="J6" s="47"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="33"/>
-      <c r="Q6" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="R6" s="33">
-        <f>(1 - _xlfn.NORM.DIST(R4,R2,R3, TRUE)) * 100</f>
-        <v>36.944134018176356</v>
-      </c>
-      <c r="T6" s="33" t="s">
-        <v>131</v>
-      </c>
-      <c r="U6" s="33">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="V6" s="33">
-        <v>203</v>
-      </c>
-      <c r="AF6" t="s">
+      <c r="W6" s="32">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="X6" s="32">
+        <v>201</v>
+      </c>
+      <c r="AH6" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="AG6">
-        <f>_xlfn.NORM.DIST(AG2,AG3,AG4, TRUE)</f>
+      <c r="AI6" s="32">
+        <f>_xlfn.NORM.DIST(AI2,AI3,AI4, TRUE)</f>
         <v>0.42074029056089696</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
-      <c r="A7" s="36"/>
-      <c r="B7" s="37"/>
-      <c r="D7" t="s">
+    <row r="7" spans="1:35">
+      <c r="A7" s="35"/>
+      <c r="B7" s="36"/>
+      <c r="D7" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="34">
         <f xml:space="preserve"> (E6 - E3) / E4</f>
         <v>-1.1782945736434109</v>
       </c>
-      <c r="H7" s="39" t="s">
+      <c r="J7" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="I7" s="44">
-        <f>I6/100</f>
-        <v>0.97</v>
-      </c>
-      <c r="J7" s="47"/>
-      <c r="N7" s="33" t="s">
+      <c r="K7" s="43">
+        <f>K6/100</f>
+        <v>0.15</v>
+      </c>
+      <c r="L7" s="46"/>
+      <c r="P7" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="O7" s="33">
-        <f>_xlfn.NORM.DIST(O5, 0, 1, TRUE)</f>
+      <c r="Q7" s="32">
+        <f>_xlfn.NORM.DIST(Q5, 0, 1, TRUE)</f>
         <v>0.61981692384016507</v>
       </c>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33">
+      <c r="S7" s="32"/>
+      <c r="T7" s="32">
         <f>NORMINV(0.07,19,2.5)</f>
         <v>15.310522429552075</v>
       </c>
-      <c r="T7" s="33" t="s">
+      <c r="V7" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="U7" s="33">
-        <f>(U4-U5)/U6</f>
-        <v>0.70588235294117685</v>
-      </c>
-      <c r="V7" s="33">
-        <f>(V4-V5)/V6</f>
+      <c r="W7" s="32">
+        <f>(W4-W5)/W6</f>
+        <v>0.80434782608695643</v>
+      </c>
+      <c r="X7" s="32">
+        <f>(X4-X5)/X6</f>
+        <v>0.59203980099502485</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35">
+      <c r="A8" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="36">
+        <f>_xlfn.NORM.DIST(B6, B3, B4, TRUE) - _xlfn.NORM.DIST(B5, B3, B4, TRUE)</f>
+        <v>-0.90072860315666903</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" s="34"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="46"/>
+      <c r="P8" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q8" s="32">
+        <f>_xlfn.NORM.DIST(Q5, 0, 1, TRUE)</f>
+        <v>0.61981692384016507</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="19">
+      <c r="A9" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="36">
+        <f>_xlfn.NORM.DIST(B5,B3,B4,TRUE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:33">
-      <c r="A8" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" s="37">
-        <f>_xlfn.NORM.DIST(B6, B3, B4, TRUE) - _xlfn.NORM.DIST(B5, B3, B4, TRUE)</f>
-        <v>0.39172524132251257</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="47"/>
-      <c r="N8" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="O8" s="33">
-        <f>_xlfn.NORM.DIST(O5, 0, 1, TRUE)</f>
-        <v>0.61981692384016507</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" ht="19">
-      <c r="A9" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="B9" s="37">
-        <f>_xlfn.NORM.DIST(B5,B3,B4,TRUE)</f>
-        <v>2.5380876893736339E-2</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="D9" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="34">
         <v>1400</v>
       </c>
-      <c r="H9" s="49" t="s">
+      <c r="J9" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="I9" s="50">
-        <f>_xlfn.NORM.INV(($I$6/100),I$4,I$5)</f>
-        <v>1483.9336457618476</v>
-      </c>
-      <c r="J9" s="47"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="Q9" s="21" t="s">
+      <c r="K9" s="49">
+        <f>_xlfn.NORM.INV(($K$6/100),K$4,K$5)</f>
+        <v>43.81783305253105</v>
+      </c>
+      <c r="L9" s="46"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="S9" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="17">
-      <c r="A10" s="36" t="s">
+    <row r="10" spans="1:35" ht="17">
+      <c r="A10" s="35" t="s">
         <v>140</v>
       </c>
-      <c r="B10" s="37">
+      <c r="B10" s="36">
         <f>1 - _xlfn.NORM.DIST(B6, B3, B4, TRUE)</f>
-        <v>0.58289388178375101</v>
-      </c>
-      <c r="D10" t="s">
+        <v>0.90072860315666903</v>
+      </c>
+      <c r="D10" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="34">
         <f>(E9-E3) / E4</f>
         <v>1.1472868217054264</v>
       </c>
-      <c r="H10" s="33"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="48"/>
-      <c r="N10" s="33">
+      <c r="J10" s="32"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="47"/>
+      <c r="P10" s="35">
         <f>_xlfn.NORM.INV(0.79, 0, 1)</f>
         <v>0.80642124701824058</v>
       </c>
-      <c r="O10" s="33"/>
-      <c r="Q10" s="21"/>
-    </row>
-    <row r="11" spans="1:33" ht="17">
-      <c r="A11" s="36"/>
-      <c r="B11" s="37"/>
-      <c r="E11" s="2"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="47"/>
-      <c r="Q11" s="21"/>
-    </row>
-    <row r="12" spans="1:33">
-      <c r="A12" s="36" t="s">
+      <c r="Q10" s="32"/>
+      <c r="S10" s="21"/>
+    </row>
+    <row r="11" spans="1:35" ht="17">
+      <c r="A11" s="35"/>
+      <c r="B11" s="36"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="34"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="46"/>
+      <c r="S11" s="21"/>
+    </row>
+    <row r="12" spans="1:35">
+      <c r="A12" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="B12" s="37">
+      <c r="B12" s="36">
         <f>B9*100</f>
-        <v>2.5380876893736337</v>
-      </c>
-      <c r="D12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="34">
         <f>_xlfn.NORM.DIST(E6,E3,E4,TRUE)</f>
         <v>0.11933959517437347</v>
       </c>
-      <c r="H12" s="33"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="48"/>
-    </row>
-    <row r="13" spans="1:33">
-      <c r="D13" t="s">
+      <c r="J12" s="32"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="47"/>
+    </row>
+    <row r="13" spans="1:35">
+      <c r="D13" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="34">
         <f>_xlfn.NORM.DIST(E10,E3,E4,TRUE)</f>
         <v>1.5595941023036459E-22</v>
       </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="47"/>
-    </row>
-    <row r="14" spans="1:33">
-      <c r="E14" s="2"/>
-      <c r="H14" s="40" t="s">
+      <c r="J13" s="32"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="46"/>
+    </row>
+    <row r="14" spans="1:35">
+      <c r="D14" s="32"/>
+      <c r="E14" s="34"/>
+      <c r="J14" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="I14" s="41">
-        <f>(1 - I7)/2</f>
-        <v>1.5000000000000013E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33">
-      <c r="E15" s="2">
+      <c r="K14" s="40">
+        <f>(1 - K7)/2</f>
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35">
+      <c r="D15" s="32"/>
+      <c r="E15" s="34">
         <f>E13-E12</f>
         <v>-0.11933959517437347</v>
       </c>
-      <c r="H15" s="33" t="s">
+      <c r="J15" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="I15" s="41">
-        <f>I7+I14</f>
-        <v>0.98499999999999999</v>
-      </c>
-      <c r="N15" t="s">
+      <c r="K15" s="40">
+        <f>K7+K14</f>
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="P15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:33">
-      <c r="E16" s="2"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="41"/>
-      <c r="N16" t="s">
+    <row r="16" spans="1:35">
+      <c r="D16" s="32"/>
+      <c r="E16" s="34"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="40"/>
+      <c r="P16" t="s">
         <v>22</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>1264</v>
       </c>
     </row>
-    <row r="17" spans="4:15">
-      <c r="D17" t="s">
+    <row r="17" spans="4:17">
+      <c r="D17" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="34">
         <v>1175</v>
       </c>
-      <c r="H17" s="40" t="s">
+      <c r="J17" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="I17" s="41">
-        <f>NORMINV(I14, 0, 1)</f>
-        <v>-2.1700903775845601</v>
-      </c>
-      <c r="N17" t="s">
+      <c r="K17" s="40">
+        <f>NORMINV(K14, 0, 1)</f>
+        <v>-0.18911842627279254</v>
+      </c>
+      <c r="P17" t="s">
         <v>131</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="4:15">
-      <c r="D18" t="s">
+    <row r="18" spans="4:17">
+      <c r="D18" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="34">
         <f xml:space="preserve"> 1 -_xlfn.NORM.DIST(1175, E3, E4, TRUE)</f>
         <v>0.7247126675619795</v>
       </c>
-      <c r="H18" s="33" t="s">
+      <c r="J18" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="I18" s="41">
-        <f>NORMINV(I15, 0, 1)</f>
-        <v>2.1700903775845601</v>
-      </c>
-      <c r="N18" t="s">
+      <c r="K18" s="40">
+        <f>NORMINV(K15, 0, 1)</f>
+        <v>0.18911842627279243</v>
+      </c>
+      <c r="P18" t="s">
         <v>143</v>
       </c>
-      <c r="O18">
+      <c r="Q18">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="4:15">
-      <c r="E19" s="2" t="s">
+    <row r="19" spans="4:17">
+      <c r="D19" s="32"/>
+      <c r="E19" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="N19" t="s">
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="P19" t="s">
         <v>144</v>
       </c>
-      <c r="O19">
-        <f>O18/100</f>
+      <c r="Q19">
+        <f>Q18/100</f>
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="20" spans="4:15">
-      <c r="D20" t="s">
+    <row r="20" spans="4:17">
+      <c r="D20" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="H20" s="33" t="s">
+      <c r="E20" s="34"/>
+      <c r="J20" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-    </row>
-    <row r="21" spans="4:15">
-      <c r="D21" t="s">
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+    </row>
+    <row r="21" spans="4:17">
+      <c r="D21" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="H21" s="33" t="s">
+      <c r="E21" s="34"/>
+      <c r="J21" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="I21" s="32">
-        <f>I4 + (I17)*I5</f>
-        <v>1005.9293354450219</v>
-      </c>
-      <c r="N21" t="s">
+      <c r="K21" s="31">
+        <f>K4 + (K17)*K5</f>
+        <v>48.054407868636041</v>
+      </c>
+      <c r="P21" t="s">
         <v>146</v>
       </c>
-      <c r="O21">
+      <c r="Q21">
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="4:15">
-      <c r="E22" s="2"/>
-      <c r="H22" s="33" t="s">
+    <row r="22" spans="4:17">
+      <c r="D22" s="32"/>
+      <c r="E22" s="34"/>
+      <c r="J22" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="I22" s="32">
-        <f>I4+(I18*I5)</f>
-        <v>1518.0706645549781</v>
-      </c>
-      <c r="N22" t="s">
+      <c r="K22" s="31">
+        <f>K4+(K18*K5)</f>
+        <v>49.945592131363959</v>
+      </c>
+      <c r="P22" t="s">
         <v>147</v>
       </c>
-      <c r="O22">
-        <f>O21/100</f>
+      <c r="Q22">
+        <f>Q21/100</f>
         <v>0.96</v>
       </c>
     </row>
-    <row r="23" spans="4:15">
-      <c r="D23" t="s">
+    <row r="23" spans="4:17">
+      <c r="D23" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-    </row>
-    <row r="24" spans="4:15">
+      <c r="E23" s="34"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+    </row>
+    <row r="24" spans="4:17">
       <c r="E24" s="2"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-    </row>
-    <row r="25" spans="4:15">
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+    </row>
+    <row r="25" spans="4:17">
       <c r="E25" s="2"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-    </row>
-    <row r="26" spans="4:15">
-      <c r="D26" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="H26" s="35" t="s">
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+    </row>
+    <row r="26" spans="4:17">
+      <c r="J26" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="I26" s="32">
-        <f>I28-I27</f>
-        <v>159.17958104627542</v>
-      </c>
-    </row>
-    <row r="27" spans="4:15">
-      <c r="D27" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="29">
-        <v>-2.61</v>
-      </c>
-      <c r="H27" s="35" t="s">
+      <c r="K26" s="31">
+        <f>K28-K27</f>
+        <v>6.7448975019608213</v>
+      </c>
+    </row>
+    <row r="27" spans="4:17">
+      <c r="J27" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="I27" s="31">
-        <f>_xlfn.NORM.INV((25/100),I$4,I$5)</f>
-        <v>1182.4102094768623</v>
-      </c>
-    </row>
-    <row r="28" spans="4:15">
-      <c r="D28" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E28" s="29">
-        <v>1.61</v>
-      </c>
-      <c r="H28" s="35" t="s">
+      <c r="K27" s="30">
+        <f>_xlfn.NORM.INV((25/100),K$4,K$5)</f>
+        <v>45.627551249019589</v>
+      </c>
+    </row>
+    <row r="28" spans="4:17">
+      <c r="J28" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="I28" s="31">
-        <f>_xlfn.NORM.INV((75/100),I$4,I$5)</f>
-        <v>1341.5897905231377</v>
-      </c>
-    </row>
-    <row r="29" spans="4:15">
-      <c r="D29" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E29" s="29">
-        <f>_xlfn.NORM.DIST(E27, 0, 1, TRUE)</f>
-        <v>4.5271111329673241E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="4:15">
-      <c r="D30" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E30" s="29">
-        <f>1 - _xlfn.NORM.DIST(E28, 0, 1, TRUE)</f>
-        <v>5.3698928148119718E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="4:15">
-      <c r="D31" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" s="29">
-        <f>SUM(E29:E30)</f>
-        <v>5.8226039281087043E-2</v>
-      </c>
-      <c r="N31" t="s">
+      <c r="K28" s="30">
+        <f>_xlfn.NORM.INV((75/100),K$4,K$5)</f>
+        <v>52.372448750980411</v>
+      </c>
+    </row>
+    <row r="31" spans="4:17">
+      <c r="P31" t="s">
         <v>145</v>
       </c>
-      <c r="O31">
+      <c r="Q31">
         <f>NORMINV(0.28,1264,116)</f>
         <v>1196.390385156539</v>
       </c>
     </row>
-    <row r="32" spans="4:15">
+    <row r="32" spans="4:17">
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="5:5">
+    <row r="33" spans="4:5">
+      <c r="D33" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="4:5">
+      <c r="D34" t="s">
+        <v>164</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Sample Proportion (Ch 8) formula sheet
</commit_message>
<xml_diff>
--- a/Midterm Excel Sheet.xlsx
+++ b/Midterm Excel Sheet.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanninoa/Desktop/Business-Stats-Excel-Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A05C66-6DB8-384F-9130-62FB7AD2AB3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAE13EB-71EB-6E4E-95B8-471A2E0A67EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" activeTab="1" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
+    <workbookView xWindow="18760" yWindow="460" windowWidth="16480" windowHeight="18540" activeTab="2" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
   </bookViews>
   <sheets>
     <sheet name="Random Variable x" sheetId="1" r:id="rId1"/>
     <sheet name="Normal Distribution" sheetId="6" r:id="rId2"/>
-    <sheet name="Binomial Probability" sheetId="2" r:id="rId3"/>
-    <sheet name="x &amp; Probability" sheetId="4" r:id="rId4"/>
-    <sheet name="Expected Value" sheetId="5" r:id="rId5"/>
-    <sheet name="Poisson" sheetId="3" r:id="rId6"/>
+    <sheet name="Chapter 8" sheetId="8" r:id="rId3"/>
+    <sheet name="Binomial Probability" sheetId="2" r:id="rId4"/>
+    <sheet name="x &amp; Probability" sheetId="4" r:id="rId5"/>
+    <sheet name="Expected Value" sheetId="5" r:id="rId6"/>
+    <sheet name="Poisson" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="189">
   <si>
     <t>x</t>
   </si>
@@ -529,10 +530,82 @@
     <t>Find val of Zα</t>
   </si>
   <si>
-    <t>MOVE THIS^^^^^</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FIND OUT HOW TO DO Z SCORE </t>
+    <t>X Bar</t>
+  </si>
+  <si>
+    <t>sample size</t>
+  </si>
+  <si>
+    <t>mean x bar</t>
+  </si>
+  <si>
+    <t>x bar SD</t>
+  </si>
+  <si>
+    <t>Central limit theorem states that a sample distribution has a normal distribution shape</t>
+  </si>
+  <si>
+    <t>Between a range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lower bound z-score </t>
+  </si>
+  <si>
+    <t>P(lower-bound &lt; X &lt; upper-bound)</t>
+  </si>
+  <si>
+    <t>sample size (n)</t>
+  </si>
+  <si>
+    <t>Current i val</t>
+  </si>
+  <si>
+    <t>z-score for I (using normal SD)</t>
+  </si>
+  <si>
+    <t>z-score for i (using bar SD)</t>
+  </si>
+  <si>
+    <t>bar P(X &lt; i val)</t>
+  </si>
+  <si>
+    <t>bar P(X &gt; i val)</t>
+  </si>
+  <si>
+    <t>normal P(x &lt; I val)</t>
+  </si>
+  <si>
+    <t>normal P(x &gt; I val)</t>
+  </si>
+  <si>
+    <t>Sample Proportion</t>
+  </si>
+  <si>
+    <t>u sub p = p</t>
+  </si>
+  <si>
+    <t>proportion</t>
+  </si>
+  <si>
+    <t>mean of p</t>
+  </si>
+  <si>
+    <t>sd of p</t>
+  </si>
+  <si>
+    <t>if &gt; 10, then it's approx. normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proportion </t>
+  </si>
+  <si>
+    <t>P(p &gt; num)</t>
+  </si>
+  <si>
+    <t>P(p &lt; num)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">probability that more/less than </t>
   </si>
 </sst>
 </file>
@@ -545,7 +618,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.000000000000000000000_);_(* \(#,##0.000000000000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="215" formatCode="0.0000000000000000000000000000000000000000000000000000E+00"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -655,6 +728,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -733,7 +828,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -822,7 +917,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -851,6 +945,23 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3115,10 +3226,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C96CE9-B77B-704D-8A1F-7836B7353FCF}">
-  <dimension ref="A1:AI34"/>
+  <dimension ref="A1:AI33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3155,7 +3266,7 @@
       <c r="K1" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="45"/>
+      <c r="L1" s="44"/>
       <c r="P1" s="31" t="s">
         <v>112</v>
       </c>
@@ -3200,10 +3311,10 @@
       <c r="J2" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="K2" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="46"/>
+      <c r="L2" s="45"/>
       <c r="P2" s="32" t="s">
         <v>113</v>
       </c>
@@ -3222,7 +3333,7 @@
       <c r="Z2" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="AA2" s="50">
+      <c r="AA2" s="49">
         <v>0.18</v>
       </c>
       <c r="AD2" s="32" t="s">
@@ -3258,8 +3369,8 @@
         <v>1.88</v>
       </c>
       <c r="J3" s="32"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="46"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="45"/>
       <c r="P3" s="32" t="s">
         <v>114</v>
       </c>
@@ -3281,7 +3392,7 @@
         <v>160</v>
       </c>
       <c r="Z3" s="35"/>
-      <c r="AA3" s="50"/>
+      <c r="AA3" s="49"/>
       <c r="AD3" s="32"/>
       <c r="AE3" s="32"/>
       <c r="AH3" s="32" t="s">
@@ -3314,10 +3425,10 @@
       <c r="J4" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="K4" s="42">
+      <c r="K4" s="41">
         <v>49</v>
       </c>
-      <c r="L4" s="46"/>
+      <c r="L4" s="45"/>
       <c r="P4" s="32"/>
       <c r="Q4" s="32"/>
       <c r="S4" s="32" t="s">
@@ -3338,7 +3449,7 @@
       <c r="Z4" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="AA4" s="50">
+      <c r="AA4" s="49">
         <f xml:space="preserve"> 1 - AA2</f>
         <v>0.82000000000000006</v>
       </c>
@@ -3375,10 +3486,10 @@
       <c r="J5" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="43">
+      <c r="K5" s="42">
         <v>5</v>
       </c>
-      <c r="L5" s="46"/>
+      <c r="L5" s="45"/>
       <c r="P5" s="32" t="s">
         <v>115</v>
       </c>
@@ -3400,7 +3511,7 @@
       <c r="Z5" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="AA5" s="50">
+      <c r="AA5" s="49">
         <f>_xlfn.NORM.INV(AA4,0, 1)</f>
         <v>0.91536508784281367</v>
       </c>
@@ -3420,7 +3531,7 @@
       <c r="E6" s="34">
         <v>1100</v>
       </c>
-      <c r="G6" s="51" t="s">
+      <c r="G6" s="50" t="s">
         <v>83</v>
       </c>
       <c r="H6" s="36">
@@ -3430,10 +3541,10 @@
       <c r="J6" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="K6" s="43">
+      <c r="K6" s="42">
         <v>15</v>
       </c>
-      <c r="L6" s="46"/>
+      <c r="L6" s="45"/>
       <c r="P6" s="33"/>
       <c r="Q6" s="32"/>
       <c r="S6" s="32" t="s">
@@ -3473,11 +3584,11 @@
       <c r="J7" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="K7" s="43">
+      <c r="K7" s="42">
         <f>K6/100</f>
         <v>0.15</v>
       </c>
-      <c r="L7" s="46"/>
+      <c r="L7" s="45"/>
       <c r="P7" s="32" t="s">
         <v>116</v>
       </c>
@@ -3513,8 +3624,8 @@
       <c r="D8" s="32"/>
       <c r="E8" s="34"/>
       <c r="J8" s="32"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="46"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="45"/>
       <c r="P8" s="32" t="s">
         <v>117</v>
       </c>
@@ -3537,14 +3648,14 @@
       <c r="E9" s="34">
         <v>1400</v>
       </c>
-      <c r="J9" s="48" t="s">
+      <c r="J9" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="K9" s="49">
+      <c r="K9" s="48">
         <f>_xlfn.NORM.INV(($K$6/100),K$4,K$5)</f>
         <v>43.81783305253105</v>
       </c>
-      <c r="L9" s="46"/>
+      <c r="L9" s="45"/>
       <c r="P9" s="32"/>
       <c r="Q9" s="32"/>
       <c r="S9" s="21" t="s">
@@ -3570,8 +3681,8 @@
         <v>1.1472868217054264</v>
       </c>
       <c r="J10" s="32"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="47"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="46"/>
       <c r="P10" s="35">
         <f>_xlfn.NORM.INV(0.79, 0, 1)</f>
         <v>0.80642124701824058</v>
@@ -3585,8 +3696,8 @@
       <c r="D11" s="32"/>
       <c r="E11" s="34"/>
       <c r="J11" s="32"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="46"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="45"/>
       <c r="S11" s="21"/>
     </row>
     <row r="12" spans="1:35">
@@ -3605,8 +3716,8 @@
         <v>0.11933959517437347</v>
       </c>
       <c r="J12" s="32"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="47"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="46"/>
     </row>
     <row r="13" spans="1:35">
       <c r="D13" s="32" t="s">
@@ -3617,8 +3728,8 @@
         <v>1.5595941023036459E-22</v>
       </c>
       <c r="J13" s="32"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="46"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="45"/>
     </row>
     <row r="14" spans="1:35">
       <c r="D14" s="32"/>
@@ -3626,7 +3737,7 @@
       <c r="J14" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="K14" s="40">
+      <c r="K14" s="49">
         <f>(1 - K7)/2</f>
         <v>0.42499999999999999</v>
       </c>
@@ -3640,7 +3751,7 @@
       <c r="J15" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="K15" s="40">
+      <c r="K15" s="49">
         <f>K7+K14</f>
         <v>0.57499999999999996</v>
       </c>
@@ -3652,7 +3763,7 @@
       <c r="D16" s="32"/>
       <c r="E16" s="34"/>
       <c r="J16" s="32"/>
-      <c r="K16" s="40"/>
+      <c r="K16" s="49"/>
       <c r="P16" t="s">
         <v>22</v>
       </c>
@@ -3670,7 +3781,7 @@
       <c r="J17" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="K17" s="40">
+      <c r="K17" s="49">
         <f>NORMINV(K14, 0, 1)</f>
         <v>-0.18911842627279254</v>
       </c>
@@ -3692,7 +3803,7 @@
       <c r="J18" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="K18" s="40">
+      <c r="K18" s="49">
         <f>NORMINV(K15, 0, 1)</f>
         <v>0.18911842627279243</v>
       </c>
@@ -3709,7 +3820,7 @@
         <v>43</v>
       </c>
       <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
+      <c r="K19" s="35"/>
       <c r="P19" t="s">
         <v>144</v>
       </c>
@@ -3726,7 +3837,7 @@
       <c r="J20" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="K20" s="32"/>
+      <c r="K20" s="35"/>
       <c r="L20" s="32"/>
     </row>
     <row r="21" spans="4:17">
@@ -3737,7 +3848,7 @@
       <c r="J21" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="K21" s="31">
+      <c r="K21" s="51">
         <f>K4 + (K17)*K5</f>
         <v>48.054407868636041</v>
       </c>
@@ -3754,7 +3865,7 @@
       <c r="J22" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="K22" s="31">
+      <c r="K22" s="51">
         <f>K4+(K18*K5)</f>
         <v>49.945592131363959</v>
       </c>
@@ -3772,23 +3883,23 @@
       </c>
       <c r="E23" s="34"/>
       <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
+      <c r="K23" s="35"/>
     </row>
     <row r="24" spans="4:17">
       <c r="E24" s="2"/>
       <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
+      <c r="K24" s="35"/>
     </row>
     <row r="25" spans="4:17">
       <c r="E25" s="2"/>
       <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
+      <c r="K25" s="35"/>
     </row>
     <row r="26" spans="4:17">
       <c r="J26" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="K26" s="31">
+      <c r="K26" s="51">
         <f>K28-K27</f>
         <v>6.7448975019608213</v>
       </c>
@@ -3824,15 +3935,8 @@
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="4:5">
-      <c r="D33" s="10" t="s">
-        <v>163</v>
-      </c>
+      <c r="D33" s="10"/>
       <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="4:5">
-      <c r="D34" t="s">
-        <v>164</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3840,6 +3944,279 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFCA351-70B0-5244-BA65-285CF6942DC3}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="16">
+        <v>43.7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="54">
+        <v>4.2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F3">
+        <f>F2/100</f>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="16">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" s="16"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="52">
+        <f>B2</f>
+        <v>43.7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>182</v>
+      </c>
+      <c r="F6" s="53">
+        <f>F3</f>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="56">
+        <f>B3/SQRT(B4)</f>
+        <v>1.2124355652982142</v>
+      </c>
+      <c r="E7" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="53">
+        <f>SQRT(F6*(1 - F6)/F4)</f>
+        <v>2.8861739379323625E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="16"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B9" s="16">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>184</v>
+      </c>
+      <c r="F9" s="53">
+        <f>(F4*F6)*(1 - F6)</f>
+        <v>74.97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" s="55">
+        <f>(B9-B2)/B3</f>
+        <v>-0.8809523809523816</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="B11" s="57">
+        <f>(B9-B2)/B7</f>
+        <v>-3.0517085657165954</v>
+      </c>
+      <c r="E11" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="E12" t="s">
+        <v>185</v>
+      </c>
+      <c r="F12">
+        <f>F11/100</f>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B13">
+        <f>_xlfn.NORM.S.DIST(B10, TRUE)</f>
+        <v>0.18917179719797161</v>
+      </c>
+      <c r="E13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13">
+        <f>(F12-F6)/F7</f>
+        <v>-2.0788767860257109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14">
+        <f xml:space="preserve"> 1-B13</f>
+        <v>0.81082820280202839</v>
+      </c>
+      <c r="E14" t="s">
+        <v>187</v>
+      </c>
+      <c r="F14" s="53">
+        <f>_xlfn.NORM.S.DIST(F13, TRUE)</f>
+        <v>1.8814338445845531E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="E15" t="s">
+        <v>186</v>
+      </c>
+      <c r="F15" s="53">
+        <f xml:space="preserve"> 1 - F14</f>
+        <v>0.98118566155415443</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16" s="52">
+        <f>_xlfn.NORM.S.DIST(B11, TRUE)</f>
+        <v>1.1377145360498184E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" s="52">
+        <f xml:space="preserve"> 1 -B16</f>
+        <v>0.99886228546395017</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" s="16"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="16">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="16">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23">
+        <f>(B21-B$6)/B$7</f>
+        <v>91.798692801150494</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24">
+        <f>(B22-B$6)/B$7</f>
+        <v>95.922623295362101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B26" s="53">
+        <f>_xlfn.NORM.S.DIST(B24, TRUE) - _xlfn.NORM.S.DIST(B23, TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74F7077-45B6-E742-951B-BF30C929E163}">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -3982,7 +4359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1764C7-EB3F-884D-A423-6A64CF5D743E}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -4050,7 +4427,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7883183-3309-E141-80C9-0F546E3ED993}">
   <dimension ref="A6:D17"/>
   <sheetViews>
@@ -4177,7 +4554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD5251E-A9B7-7F4B-A78E-2F9C7E161BB7}">
   <dimension ref="A1:H57"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add more sample proportional formulas
</commit_message>
<xml_diff>
--- a/Midterm Excel Sheet.xlsx
+++ b/Midterm Excel Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanninoa/Desktop/Business-Stats-Excel-Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAE13EB-71EB-6E4E-95B8-471A2E0A67EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620E4AA2-7345-5E46-8DD2-244D4E8E9FE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18760" yWindow="460" windowWidth="16480" windowHeight="18540" activeTab="2" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
+    <workbookView xWindow="11340" yWindow="660" windowWidth="16480" windowHeight="18540" activeTab="2" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
   </bookViews>
   <sheets>
     <sheet name="Random Variable x" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Chapter 9.1 contents
</commit_message>
<xml_diff>
--- a/Midterm Excel Sheet.xlsx
+++ b/Midterm Excel Sheet.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanninoa/Desktop/Business-Stats-Excel-Sheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/unghour/Desktop/Business-Stats-Excel-Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620E4AA2-7345-5E46-8DD2-244D4E8E9FE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69D39EC-D501-B54A-AE17-63E8C540DE85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11340" yWindow="660" windowWidth="16480" windowHeight="18540" activeTab="2" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
   </bookViews>
   <sheets>
     <sheet name="Random Variable x" sheetId="1" r:id="rId1"/>
     <sheet name="Normal Distribution" sheetId="6" r:id="rId2"/>
-    <sheet name="Chapter 8" sheetId="8" r:id="rId3"/>
-    <sheet name="Binomial Probability" sheetId="2" r:id="rId4"/>
-    <sheet name="x &amp; Probability" sheetId="4" r:id="rId5"/>
-    <sheet name="Expected Value" sheetId="5" r:id="rId6"/>
-    <sheet name="Poisson" sheetId="3" r:id="rId7"/>
+    <sheet name="Chapter 9" sheetId="9" r:id="rId3"/>
+    <sheet name="Chapter 8" sheetId="8" r:id="rId4"/>
+    <sheet name="Binomial Probability" sheetId="2" r:id="rId5"/>
+    <sheet name="x &amp; Probability" sheetId="4" r:id="rId6"/>
+    <sheet name="Expected Value" sheetId="5" r:id="rId7"/>
+    <sheet name="Poisson" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="216">
   <si>
     <t>x</t>
   </si>
@@ -606,17 +607,101 @@
   </si>
   <si>
     <t xml:space="preserve">probability that more/less than </t>
+  </si>
+  <si>
+    <t>between mintues</t>
+  </si>
+  <si>
+    <t>Level of Confidence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">find the population portion </t>
+  </si>
+  <si>
+    <t>level of confidence</t>
+  </si>
+  <si>
+    <t>point estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">margin of error </t>
+  </si>
+  <si>
+    <t xml:space="preserve">upper bound </t>
+  </si>
+  <si>
+    <t>np(1-p) &gt;= 10?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">percent </t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>a/2</t>
+  </si>
+  <si>
+    <t>critical value (z(a/2))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lower bound </t>
+  </si>
+  <si>
+    <t>Find sample size (n)</t>
+  </si>
+  <si>
+    <t>margin of error (estimate) E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample size increse and decrese </t>
+  </si>
+  <si>
+    <t>Confidence level</t>
+  </si>
+  <si>
+    <t>given factor</t>
+  </si>
+  <si>
+    <t>previous estimate (p cap)</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>z of a/2</t>
+  </si>
+  <si>
+    <t>n (prior estimate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increasing the sample size by a factor M results in the margin of error decreasing by a factor of </t>
+  </si>
+  <si>
+    <t>n (no prior estimate)</t>
+  </si>
+  <si>
+    <t>StartFraction 1 Over StartRoot Upper M EndRoot EndFraction1M.</t>
+  </si>
+  <si>
+    <t>ex: 1/3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.000000000000000000000_);_(* \(#,##0.000000000000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="215" formatCode="0.0000000000000000000000000000000000000000000000000000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.0000000000000000000000000000000000000000000000000000E+00"/>
+    <numFmt numFmtId="167" formatCode="0.00000000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
   <fonts count="18">
     <font>
@@ -751,7 +836,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -764,8 +849,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -823,12 +914,107 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -900,7 +1086,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="215" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -963,6 +1149,34 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="9" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3228,8 +3442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C96CE9-B77B-704D-8A1F-7836B7353FCF}">
   <dimension ref="A1:AI33"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="T1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3334,7 +3548,7 @@
         <v>127</v>
       </c>
       <c r="AA2" s="49">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="AD2" s="32" t="s">
         <v>125</v>
@@ -3451,7 +3665,7 @@
       </c>
       <c r="AA4" s="49">
         <f xml:space="preserve"> 1 - AA2</f>
-        <v>0.82000000000000006</v>
+        <v>0.84</v>
       </c>
       <c r="AD4" s="32" t="s">
         <v>79</v>
@@ -3511,9 +3725,9 @@
       <c r="Z5" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="AA5" s="49">
+      <c r="AA5" s="59">
         <f>_xlfn.NORM.INV(AA4,0, 1)</f>
-        <v>0.91536508784281367</v>
+        <v>0.9944578832097497</v>
       </c>
       <c r="AH5" s="32"/>
       <c r="AI5" s="32"/>
@@ -3944,11 +4158,404 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFCA351-70B0-5244-BA65-285CF6942DC3}">
-  <dimension ref="A1:F26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77044CB3-A584-0B47-8E5D-C4DB8D5DE250}">
+  <dimension ref="B3:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="28.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4" s="76" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="77"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="76" t="s">
+        <v>191</v>
+      </c>
+      <c r="I4" s="77"/>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="62" t="s">
+        <v>192</v>
+      </c>
+      <c r="C5" s="63">
+        <v>95</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="63">
+        <v>424</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="62" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="63">
+        <v>47</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="63">
+        <v>2285</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="63">
+        <v>0.113</v>
+      </c>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="62" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="63">
+        <v>3</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="63">
+        <v>0.18555799000000001</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="I7" s="63">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="65">
+        <v>0.44</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="62" t="s">
+        <v>196</v>
+      </c>
+      <c r="F8" s="63">
+        <v>345.32341400000001</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="62" t="s">
+        <v>197</v>
+      </c>
+      <c r="I8" s="63">
+        <v>1200</v>
+      </c>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="65">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="62" t="s">
+        <v>198</v>
+      </c>
+      <c r="F9" s="63">
+        <v>90</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="65">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="66">
+        <v>8.1329999999999996E-3</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="64" t="s">
+        <v>199</v>
+      </c>
+      <c r="I10" s="65">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="62" t="s">
+        <v>200</v>
+      </c>
+      <c r="F11" s="63">
+        <v>0.05</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="65">
+        <v>462</v>
+      </c>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="F12" s="63">
+        <v>1.6448536300000001</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="78" t="s">
+        <v>202</v>
+      </c>
+      <c r="F13" s="79">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="78" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="79">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="76" t="s">
+        <v>203</v>
+      </c>
+      <c r="C15" s="77"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="62" t="s">
+        <v>204</v>
+      </c>
+      <c r="C16" s="63">
+        <v>0.05</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="76" t="s">
+        <v>205</v>
+      </c>
+      <c r="F16" s="77"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="69"/>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="62" t="s">
+        <v>206</v>
+      </c>
+      <c r="C17" s="63">
+        <v>94</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="62" t="s">
+        <v>207</v>
+      </c>
+      <c r="F17" s="63">
+        <v>1</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="70"/>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="62" t="s">
+        <v>208</v>
+      </c>
+      <c r="C18" s="63">
+        <v>0.51</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="63">
+        <v>3</v>
+      </c>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="70"/>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" s="62" t="s">
+        <v>200</v>
+      </c>
+      <c r="C19" s="63">
+        <v>0.03</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="62" t="s">
+        <v>209</v>
+      </c>
+      <c r="F19" s="63">
+        <v>9</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="70"/>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" s="62" t="s">
+        <v>210</v>
+      </c>
+      <c r="C20" s="71">
+        <v>1.8808</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="70"/>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" s="64" t="s">
+        <v>211</v>
+      </c>
+      <c r="C21" s="67">
+        <v>353.59699999999998</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="72" t="s">
+        <v>212</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="73"/>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="64" t="s">
+        <v>213</v>
+      </c>
+      <c r="C22" s="67">
+        <v>353.738</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="74" t="s">
+        <v>214</v>
+      </c>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="75"/>
+      <c r="J22" s="63"/>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="E16:F16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFCA351-70B0-5244-BA65-285CF6942DC3}">
+  <dimension ref="A1:I26"/>
+  <sheetViews>
+    <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3957,7 +4564,7 @@
     <col min="5" max="5" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" s="25" t="s">
         <v>163</v>
       </c>
@@ -3974,41 +4581,41 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9">
       <c r="A2" s="16" t="s">
         <v>91</v>
       </c>
       <c r="B2" s="16">
-        <v>43.7</v>
+        <v>150.9</v>
       </c>
       <c r="E2" t="s">
         <v>113</v>
       </c>
       <c r="F2">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="16" t="s">
         <v>131</v>
       </c>
       <c r="B3" s="54">
-        <v>4.2</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
         <v>181</v>
       </c>
       <c r="F3">
         <f>F2/100</f>
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="16" t="s">
         <v>171</v>
       </c>
       <c r="B4" s="16">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
         <v>164</v>
@@ -4017,206 +4624,236 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:9">
       <c r="B5" s="16"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:9">
       <c r="A6" s="16" t="s">
         <v>165</v>
       </c>
       <c r="B6" s="52">
         <f>B2</f>
-        <v>43.7</v>
+        <v>150.9</v>
       </c>
       <c r="E6" t="s">
         <v>182</v>
       </c>
       <c r="F6" s="53">
         <f>F3</f>
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="16" t="s">
         <v>166</v>
       </c>
       <c r="B7" s="56">
         <f>B3/SQRT(B4)</f>
-        <v>1.2124355652982142</v>
+        <v>5.5780180812082092</v>
       </c>
       <c r="E7" t="s">
         <v>183</v>
       </c>
       <c r="F7" s="53">
         <f>SQRT(F6*(1 - F6)/F4)</f>
-        <v>2.8861739379323625E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>1.2583057392117916E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="B8" s="16"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:9">
       <c r="A9" s="16" t="s">
         <v>172</v>
       </c>
       <c r="B9" s="16">
-        <v>40</v>
+        <v>180</v>
       </c>
       <c r="E9" t="s">
         <v>184</v>
       </c>
       <c r="F9" s="53">
         <f>(F4*F6)*(1 - F6)</f>
-        <v>74.97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>14.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="16" t="s">
         <v>173</v>
       </c>
       <c r="B10" s="55">
         <f>(B9-B2)/B3</f>
-        <v>-0.8809523809523816</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>0.88181818181818161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="16" t="s">
         <v>174</v>
       </c>
       <c r="B11" s="57">
         <f>(B9-B2)/B7</f>
-        <v>-3.0517085657165954</v>
+        <v>5.2169067178242061</v>
       </c>
       <c r="E11" t="s">
         <v>188</v>
       </c>
       <c r="F11">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="E12" t="s">
         <v>185</v>
       </c>
       <c r="F12">
         <f>F11/100</f>
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="16" t="s">
         <v>177</v>
       </c>
       <c r="B13">
         <f>_xlfn.NORM.S.DIST(B10, TRUE)</f>
-        <v>0.18917179719797161</v>
+        <v>0.81106243112708065</v>
       </c>
       <c r="E13" t="s">
         <v>125</v>
       </c>
       <c r="F13">
         <f>(F12-F6)/F7</f>
-        <v>-2.0788767860257109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>11.920791213585396</v>
+      </c>
+      <c r="H13">
+        <v>19</v>
+      </c>
+      <c r="I13">
+        <v>0.79341189999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="58">
         <f xml:space="preserve"> 1-B13</f>
-        <v>0.81082820280202839</v>
+        <v>0.18893756887291935</v>
       </c>
       <c r="E14" t="s">
         <v>187</v>
       </c>
       <c r="F14" s="53">
         <f>_xlfn.NORM.S.DIST(F13, TRUE)</f>
-        <v>1.8814338445845531E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>14</v>
+      </c>
+      <c r="I14">
+        <v>0.70731049999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="E15" t="s">
         <v>186</v>
       </c>
       <c r="F15" s="53">
         <f xml:space="preserve"> 1 - F14</f>
-        <v>0.98118566155415443</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f>I13-I14</f>
+        <v>8.6101399999999995E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="16" t="s">
         <v>175</v>
       </c>
       <c r="B16" s="52">
         <f>_xlfn.NORM.S.DIST(B11, TRUE)</f>
-        <v>1.1377145360498184E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>0.99999990903208769</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="16" t="s">
         <v>176</v>
       </c>
       <c r="B17" s="52">
         <f xml:space="preserve"> 1 -B16</f>
-        <v>0.99886228546395017</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>9.0967912313999477E-8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="25" t="s">
         <v>168</v>
       </c>
       <c r="B20" s="16"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:6">
       <c r="A21" s="16" t="s">
         <v>67</v>
       </c>
       <c r="B21" s="16">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>120</v>
+      </c>
+      <c r="E21">
+        <v>0.174543</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="16" t="s">
         <v>68</v>
       </c>
       <c r="B22" s="16">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>180</v>
+      </c>
+      <c r="E22">
+        <v>0.81106243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="16" t="s">
         <v>169</v>
       </c>
       <c r="B23">
         <f>(B21-B$6)/B$7</f>
-        <v>91.798692801150494</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>-5.539601978720551</v>
+      </c>
+      <c r="E23">
+        <f>E22-E21</f>
+        <v>0.63651943</v>
+      </c>
+      <c r="F23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="16" t="s">
         <v>72</v>
       </c>
       <c r="B24">
         <f>(B22-B$6)/B$7</f>
-        <v>95.922623295362101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>5.2169067178242061</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="16" t="s">
         <v>170</v>
       </c>
       <c r="B26" s="53">
         <f>_xlfn.NORM.S.DIST(B24, TRUE) - _xlfn.NORM.S.DIST(B23, TRUE)</f>
-        <v>0</v>
+        <v>0.99999989387409427</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74F7077-45B6-E742-951B-BF30C929E163}">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -4359,7 +4996,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1764C7-EB3F-884D-A423-6A64CF5D743E}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -4427,7 +5064,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7883183-3309-E141-80C9-0F546E3ED993}">
   <dimension ref="A6:D17"/>
   <sheetViews>
@@ -4554,7 +5191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD5251E-A9B7-7F4B-A78E-2F9C7E161BB7}">
   <dimension ref="A1:H57"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added the formula for 9.1
</commit_message>
<xml_diff>
--- a/Midterm Excel Sheet.xlsx
+++ b/Midterm Excel Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/unghour/Desktop/Business-Stats-Excel-Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69D39EC-D501-B54A-AE17-63E8C540DE85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83FD1DE-2CA8-594F-B75A-97744B2D7ECB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" activeTab="2" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
   </bookViews>
   <sheets>
     <sheet name="Random Variable x" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="215">
   <si>
     <t>x</t>
   </si>
@@ -685,9 +685,6 @@
   </si>
   <si>
     <t>StartFraction 1 Over StartRoot Upper M EndRoot EndFraction1M.</t>
-  </si>
-  <si>
-    <t>ex: 1/3</t>
   </si>
 </sst>
 </file>
@@ -701,9 +698,9 @@
     <numFmt numFmtId="166" formatCode="0.0000000000000000000000000000000000000000000000000000E+00"/>
     <numFmt numFmtId="167" formatCode="0.00000000"/>
     <numFmt numFmtId="168" formatCode="0.000000"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -835,6 +832,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -856,7 +866,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -919,32 +929,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -990,15 +974,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1014,7 +989,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1153,30 +1128,23 @@
     <xf numFmtId="168" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="9" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="19" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4159,10 +4127,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77044CB3-A584-0B47-8E5D-C4DB8D5DE250}">
-  <dimension ref="B3:J23"/>
+  <dimension ref="B2:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4172,379 +4140,415 @@
     <col min="8" max="8" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="2:10">
-      <c r="B4" s="76" t="s">
+    <row r="2" spans="2:11">
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+    </row>
+    <row r="3" spans="2:11">
+      <c r="B3" s="61" t="s">
         <v>190</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="76" t="s">
+      <c r="C3" s="61"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="61" t="s">
         <v>191</v>
       </c>
-      <c r="I4" s="77"/>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="2:10">
+      <c r="I3" s="61"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4" s="62" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" s="62">
+        <v>95</v>
+      </c>
+      <c r="D4" s="60"/>
+      <c r="E4" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="62">
+        <v>424</v>
+      </c>
+      <c r="G4" s="60"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+    </row>
+    <row r="5" spans="2:11">
       <c r="B5" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="C5" s="63">
-        <v>95</v>
-      </c>
-      <c r="D5" s="6"/>
+        <v>193</v>
+      </c>
+      <c r="C5" s="62">
+        <v>47</v>
+      </c>
+      <c r="D5" s="60"/>
       <c r="E5" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="63">
-        <v>424</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="2:10">
+        <v>20</v>
+      </c>
+      <c r="F5" s="62">
+        <v>2285</v>
+      </c>
+      <c r="G5" s="60"/>
+      <c r="H5" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="62">
+        <v>0.113</v>
+      </c>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+    </row>
+    <row r="6" spans="2:11">
       <c r="B6" s="62" t="s">
-        <v>193</v>
-      </c>
-      <c r="C6" s="63">
-        <v>47</v>
-      </c>
-      <c r="D6" s="6"/>
+        <v>194</v>
+      </c>
+      <c r="C6" s="62">
+        <v>3</v>
+      </c>
+      <c r="D6" s="60"/>
       <c r="E6" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="63">
-        <v>2285</v>
-      </c>
-      <c r="G6" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="F6" s="62">
+        <f>F4/F5</f>
+        <v>0.18555798687089717</v>
+      </c>
+      <c r="G6" s="60"/>
       <c r="H6" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="I6" s="62">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="63">
-        <v>0.113</v>
-      </c>
-      <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="62" t="s">
-        <v>194</v>
-      </c>
       <c r="C7" s="63">
+        <f>(C5-C6) / 100</f>
+        <v>0.44</v>
+      </c>
+      <c r="D7" s="60"/>
+      <c r="E7" s="62" t="s">
+        <v>196</v>
+      </c>
+      <c r="F7" s="62">
+        <f>F5*F6*(1-F6)</f>
+        <v>345.32341356673965</v>
+      </c>
+      <c r="G7" s="60"/>
+      <c r="H7" s="62" t="s">
+        <v>197</v>
+      </c>
+      <c r="I7" s="62">
+        <v>1200</v>
+      </c>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="63">
+        <f>(C5+C6)/100</f>
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="60"/>
+      <c r="E8" s="62" t="s">
+        <v>198</v>
+      </c>
+      <c r="F8" s="62">
+        <v>90</v>
+      </c>
+      <c r="G8" s="60"/>
+      <c r="H8" s="63" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="63">
+        <f>(I6+I5)/2</f>
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="64">
+        <f>SQRT((F6*(1-F6))/F5)</f>
+        <v>8.1325512394771204E-3</v>
+      </c>
+      <c r="G9" s="60"/>
+      <c r="H9" s="63" t="s">
+        <v>199</v>
+      </c>
+      <c r="I9" s="63">
+        <f>(I6-I5)/2</f>
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="62" t="s">
+        <v>200</v>
+      </c>
+      <c r="F10" s="62">
+        <f>((100-F8) /2)/100</f>
+        <v>0.05</v>
+      </c>
+      <c r="G10" s="60"/>
+      <c r="H10" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="63">
+        <f>I7*I8</f>
+        <v>462</v>
+      </c>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="F11" s="62">
+        <f>_xlfn.NORM.INV((1-F10),0,1)</f>
+        <v>1.6448536269514715</v>
+      </c>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="63" t="s">
+        <v>202</v>
+      </c>
+      <c r="F12" s="65">
+        <f>F6-F$11*F9</f>
+        <v>0.17218113046827455</v>
+      </c>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+    </row>
+    <row r="13" spans="2:11">
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="65">
+        <f>F6+F$11*F9</f>
+        <v>0.19893484327351979</v>
+      </c>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+    </row>
+    <row r="14" spans="2:11">
+      <c r="B14" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="C14" s="61"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+    </row>
+    <row r="15" spans="2:11">
+      <c r="B15" s="62" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="62">
+        <v>0.05</v>
+      </c>
+      <c r="D15" s="60"/>
+      <c r="E15" s="61" t="s">
+        <v>205</v>
+      </c>
+      <c r="F15" s="61"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="60"/>
+    </row>
+    <row r="16" spans="2:11">
+      <c r="B16" s="62" t="s">
+        <v>206</v>
+      </c>
+      <c r="C16" s="62">
+        <v>94</v>
+      </c>
+      <c r="D16" s="60"/>
+      <c r="E16" s="62" t="s">
+        <v>207</v>
+      </c>
+      <c r="F16" s="62">
+        <v>1</v>
+      </c>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="60"/>
+    </row>
+    <row r="17" spans="2:11">
+      <c r="B17" s="62" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" s="62">
+        <v>0.51</v>
+      </c>
+      <c r="D17" s="60"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62">
         <v>3</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="62" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="63">
-        <v>0.18555799000000001</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="62" t="s">
-        <v>195</v>
-      </c>
-      <c r="I7" s="63">
-        <v>0.65700000000000003</v>
-      </c>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="65">
-        <v>0.44</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="62" t="s">
-        <v>196</v>
-      </c>
-      <c r="F8" s="63">
-        <v>345.32341400000001</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="62" t="s">
-        <v>197</v>
-      </c>
-      <c r="I8" s="63">
-        <v>1200</v>
-      </c>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="B9" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="65">
-        <v>0.5</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="62" t="s">
-        <v>198</v>
-      </c>
-      <c r="F9" s="63">
-        <v>90</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="64" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="65">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="62" t="s">
-        <v>131</v>
-      </c>
-      <c r="F10" s="66">
-        <v>8.1329999999999996E-3</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="64" t="s">
-        <v>199</v>
-      </c>
-      <c r="I10" s="65">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="62" t="s">
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="69"/>
+      <c r="K17" s="60"/>
+    </row>
+    <row r="18" spans="2:11">
+      <c r="B18" s="62" t="s">
         <v>200</v>
       </c>
-      <c r="F11" s="63">
-        <v>0.05</v>
-      </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" s="65">
-        <v>462</v>
-      </c>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="62" t="s">
-        <v>201</v>
-      </c>
-      <c r="F12" s="63">
-        <v>1.6448536300000001</v>
-      </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="2:10">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="78" t="s">
-        <v>202</v>
-      </c>
-      <c r="F13" s="79">
-        <v>0.17199999999999999</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="78" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="79">
-        <v>0.19900000000000001</v>
-      </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="2:10">
-      <c r="B15" s="76" t="s">
-        <v>203</v>
-      </c>
-      <c r="C15" s="77"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="2:10">
-      <c r="B16" s="62" t="s">
-        <v>204</v>
-      </c>
-      <c r="C16" s="63">
-        <v>0.05</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="76" t="s">
-        <v>205</v>
-      </c>
-      <c r="F16" s="77"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="69"/>
-    </row>
-    <row r="17" spans="2:10">
-      <c r="B17" s="62" t="s">
-        <v>206</v>
-      </c>
-      <c r="C17" s="63">
-        <v>94</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="62" t="s">
-        <v>207</v>
-      </c>
-      <c r="F17" s="63">
-        <v>1</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="70"/>
-    </row>
-    <row r="18" spans="2:10">
-      <c r="B18" s="62" t="s">
-        <v>208</v>
-      </c>
-      <c r="C18" s="63">
-        <v>0.51</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="63">
-        <v>3</v>
-      </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="70"/>
-    </row>
-    <row r="19" spans="2:10">
+      <c r="C18" s="62">
+        <f>((100-C16)/100)/2</f>
+        <v>0.03</v>
+      </c>
+      <c r="D18" s="60"/>
+      <c r="E18" s="62" t="s">
+        <v>209</v>
+      </c>
+      <c r="F18" s="62">
+        <f>F17^2</f>
+        <v>9</v>
+      </c>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="60"/>
+    </row>
+    <row r="19" spans="2:11">
       <c r="B19" s="62" t="s">
-        <v>200</v>
-      </c>
-      <c r="C19" s="63">
-        <v>0.03</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="62" t="s">
-        <v>209</v>
-      </c>
-      <c r="F19" s="63">
-        <v>9</v>
-      </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="70"/>
-    </row>
-    <row r="20" spans="2:10">
-      <c r="B20" s="62" t="s">
         <v>210</v>
       </c>
-      <c r="C20" s="71">
-        <v>1.8808</v>
-      </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="70"/>
-    </row>
-    <row r="21" spans="2:10">
-      <c r="B21" s="64" t="s">
+      <c r="C19" s="70">
+        <f>_xlfn.NORM.INV(1-C18,0,1)</f>
+        <v>1.8807936081512504</v>
+      </c>
+      <c r="D19" s="60"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="60"/>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="B20" s="63" t="s">
         <v>211</v>
       </c>
-      <c r="C21" s="67">
-        <v>353.59699999999998</v>
-      </c>
-      <c r="D21" s="6"/>
+      <c r="C20" s="65">
+        <f xml:space="preserve"> C17*(1-C17)*((C19/C15)^2)</f>
+        <v>353.59696426240129</v>
+      </c>
+      <c r="D20" s="60"/>
+      <c r="E20" s="71" t="s">
+        <v>212</v>
+      </c>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="69"/>
+      <c r="K20" s="60"/>
+    </row>
+    <row r="21" spans="2:11">
+      <c r="B21" s="63" t="s">
+        <v>213</v>
+      </c>
+      <c r="C21" s="65">
+        <f>0.25*((C19/C15)^2)</f>
+        <v>353.7384596462598</v>
+      </c>
+      <c r="D21" s="60"/>
       <c r="E21" s="72" t="s">
-        <v>212</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="73"/>
-    </row>
-    <row r="22" spans="2:10">
-      <c r="B22" s="64" t="s">
-        <v>213</v>
-      </c>
-      <c r="C22" s="67">
-        <v>353.738</v>
-      </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="74" t="s">
         <v>214</v>
       </c>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="75"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="63"/>
-    </row>
-    <row r="23" spans="2:10">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="73"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="60"/>
+    </row>
+    <row r="22" spans="2:11">
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added the formulas to find t-values
</commit_message>
<xml_diff>
--- a/Midterm Excel Sheet.xlsx
+++ b/Midterm Excel Sheet.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/unghour/Desktop/Business-Stats-Excel-Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83FD1DE-2CA8-594F-B75A-97744B2D7ECB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E554ADD-F480-A44C-B80A-F1D1B1EC541D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" activeTab="2" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" activeTab="3" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
   </bookViews>
   <sheets>
     <sheet name="Random Variable x" sheetId="1" r:id="rId1"/>
     <sheet name="Normal Distribution" sheetId="6" r:id="rId2"/>
     <sheet name="Chapter 9" sheetId="9" r:id="rId3"/>
-    <sheet name="Chapter 8" sheetId="8" r:id="rId4"/>
-    <sheet name="Binomial Probability" sheetId="2" r:id="rId5"/>
-    <sheet name="x &amp; Probability" sheetId="4" r:id="rId6"/>
-    <sheet name="Expected Value" sheetId="5" r:id="rId7"/>
-    <sheet name="Poisson" sheetId="3" r:id="rId8"/>
+    <sheet name="t-values" sheetId="10" r:id="rId4"/>
+    <sheet name="Chapter 8" sheetId="8" r:id="rId5"/>
+    <sheet name="Binomial Probability" sheetId="2" r:id="rId6"/>
+    <sheet name="x &amp; Probability" sheetId="4" r:id="rId7"/>
+    <sheet name="Expected Value" sheetId="5" r:id="rId8"/>
+    <sheet name="Poisson" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="236">
   <si>
     <t>x</t>
   </si>
@@ -685,6 +686,69 @@
   </si>
   <si>
     <t>StartFraction 1 Over StartRoot Upper M EndRoot EndFraction1M.</t>
+  </si>
+  <si>
+    <t>Find the t-value</t>
+  </si>
+  <si>
+    <t>Upper and Lower Bound</t>
+  </si>
+  <si>
+    <t>Determine population mean and margin of error</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>df (degree of freedom)</t>
+  </si>
+  <si>
+    <t>standard deviation</t>
+  </si>
+  <si>
+    <t>t-value (left)</t>
+  </si>
+  <si>
+    <t>confidence level (CI)</t>
+  </si>
+  <si>
+    <t>t-value (right)</t>
+  </si>
+  <si>
+    <t>Margin of Error</t>
+  </si>
+  <si>
+    <t>t-valvue</t>
+  </si>
+  <si>
+    <t>(a/2)</t>
+  </si>
+  <si>
+    <t>t-value from %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use summary to determine the point estimate of the population mean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean </t>
+  </si>
+  <si>
+    <t>Find n</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comfidence level (%) </t>
+  </si>
+  <si>
+    <t>(then you can use the 'Upper and Lower Bound' to compute by changing the standard deviation,…)</t>
+  </si>
+  <si>
+    <t>(round up to one more value ex: 48 then should be 49)</t>
   </si>
 </sst>
 </file>
@@ -700,7 +764,7 @@
     <numFmt numFmtId="168" formatCode="0.000000"/>
     <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -845,8 +909,29 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -865,8 +950,26 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -984,12 +1087,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1129,9 +1245,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1145,6 +1258,60 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4129,7 +4296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77044CB3-A584-0B47-8E5D-C4DB8D5DE250}">
   <dimension ref="B2:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -4153,136 +4320,136 @@
       <c r="K2" s="60"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="74" t="s">
         <v>190</v>
       </c>
-      <c r="C3" s="61"/>
+      <c r="C3" s="74"/>
       <c r="D3" s="60"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="61" t="s">
+      <c r="H3" s="74" t="s">
         <v>191</v>
       </c>
-      <c r="I3" s="61"/>
+      <c r="I3" s="74"/>
       <c r="J3" s="60"/>
       <c r="K3" s="60"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="61" t="s">
         <v>192</v>
       </c>
-      <c r="C4" s="62">
+      <c r="C4" s="61">
         <v>95</v>
       </c>
       <c r="D4" s="60"/>
-      <c r="E4" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="62">
+      <c r="E4" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="61">
         <v>424</v>
       </c>
       <c r="G4" s="60"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
       <c r="J4" s="60"/>
       <c r="K4" s="60"/>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="61" t="s">
         <v>193</v>
       </c>
-      <c r="C5" s="62">
+      <c r="C5" s="61">
         <v>47</v>
       </c>
       <c r="D5" s="60"/>
-      <c r="E5" s="62" t="s">
+      <c r="E5" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="62">
+      <c r="F5" s="61">
         <v>2285</v>
       </c>
       <c r="G5" s="60"/>
-      <c r="H5" s="62" t="s">
+      <c r="H5" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="62">
+      <c r="I5" s="61">
         <v>0.113</v>
       </c>
       <c r="J5" s="60"/>
       <c r="K5" s="60"/>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="61" t="s">
         <v>194</v>
       </c>
-      <c r="C6" s="62">
+      <c r="C6" s="61">
         <v>3</v>
       </c>
       <c r="D6" s="60"/>
-      <c r="E6" s="62" t="s">
+      <c r="E6" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="62">
+      <c r="F6" s="61">
         <f>F4/F5</f>
         <v>0.18555798687089717</v>
       </c>
       <c r="G6" s="60"/>
-      <c r="H6" s="62" t="s">
+      <c r="H6" s="61" t="s">
         <v>195</v>
       </c>
-      <c r="I6" s="62">
+      <c r="I6" s="61">
         <v>0.65700000000000003</v>
       </c>
       <c r="J6" s="60"/>
       <c r="K6" s="60"/>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="63">
+      <c r="C7" s="62">
         <f>(C5-C6) / 100</f>
         <v>0.44</v>
       </c>
       <c r="D7" s="60"/>
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="61" t="s">
         <v>196</v>
       </c>
-      <c r="F7" s="62">
+      <c r="F7" s="61">
         <f>F5*F6*(1-F6)</f>
         <v>345.32341356673965</v>
       </c>
       <c r="G7" s="60"/>
-      <c r="H7" s="62" t="s">
+      <c r="H7" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="I7" s="62">
+      <c r="I7" s="61">
         <v>1200</v>
       </c>
       <c r="J7" s="60"/>
       <c r="K7" s="60"/>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="63">
+      <c r="C8" s="62">
         <f>(C5+C6)/100</f>
         <v>0.5</v>
       </c>
       <c r="D8" s="60"/>
-      <c r="E8" s="62" t="s">
+      <c r="E8" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="F8" s="62">
+      <c r="F8" s="61">
         <v>90</v>
       </c>
       <c r="G8" s="60"/>
-      <c r="H8" s="63" t="s">
+      <c r="H8" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="63">
+      <c r="I8" s="62">
         <f>(I6+I5)/2</f>
         <v>0.38500000000000001</v>
       </c>
@@ -4293,18 +4460,18 @@
       <c r="B9" s="60"/>
       <c r="C9" s="60"/>
       <c r="D9" s="60"/>
-      <c r="E9" s="62" t="s">
+      <c r="E9" s="61" t="s">
         <v>131</v>
       </c>
-      <c r="F9" s="64">
+      <c r="F9" s="63">
         <f>SQRT((F6*(1-F6))/F5)</f>
         <v>8.1325512394771204E-3</v>
       </c>
       <c r="G9" s="60"/>
-      <c r="H9" s="63" t="s">
+      <c r="H9" s="62" t="s">
         <v>199</v>
       </c>
-      <c r="I9" s="63">
+      <c r="I9" s="62">
         <f>(I6-I5)/2</f>
         <v>0.27200000000000002</v>
       </c>
@@ -4315,18 +4482,18 @@
       <c r="B10" s="60"/>
       <c r="C10" s="60"/>
       <c r="D10" s="60"/>
-      <c r="E10" s="62" t="s">
+      <c r="E10" s="61" t="s">
         <v>200</v>
       </c>
-      <c r="F10" s="62">
+      <c r="F10" s="61">
         <f>((100-F8) /2)/100</f>
         <v>0.05</v>
       </c>
       <c r="G10" s="60"/>
-      <c r="H10" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" s="63">
+      <c r="H10" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="62">
         <f>I7*I8</f>
         <v>462</v>
       </c>
@@ -4337,10 +4504,10 @@
       <c r="B11" s="60"/>
       <c r="C11" s="60"/>
       <c r="D11" s="60"/>
-      <c r="E11" s="62" t="s">
+      <c r="E11" s="61" t="s">
         <v>201</v>
       </c>
-      <c r="F11" s="62">
+      <c r="F11" s="61">
         <f>_xlfn.NORM.INV((1-F10),0,1)</f>
         <v>1.6448536269514715</v>
       </c>
@@ -4354,10 +4521,10 @@
       <c r="B12" s="60"/>
       <c r="C12" s="60"/>
       <c r="D12" s="60"/>
-      <c r="E12" s="63" t="s">
+      <c r="E12" s="62" t="s">
         <v>202</v>
       </c>
-      <c r="F12" s="65">
+      <c r="F12" s="64">
         <f>F6-F$11*F9</f>
         <v>0.17218113046827455</v>
       </c>
@@ -4371,10 +4538,10 @@
       <c r="B13" s="60"/>
       <c r="C13" s="60"/>
       <c r="D13" s="60"/>
-      <c r="E13" s="66" t="s">
+      <c r="E13" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="65">
+      <c r="F13" s="64">
         <f>F6+F$11*F9</f>
         <v>0.19893484327351979</v>
       </c>
@@ -4385,10 +4552,10 @@
       <c r="K13" s="60"/>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="74" t="s">
         <v>203</v>
       </c>
-      <c r="C14" s="61"/>
+      <c r="C14" s="74"/>
       <c r="D14" s="60"/>
       <c r="E14" s="60"/>
       <c r="F14" s="60"/>
@@ -4399,136 +4566,136 @@
       <c r="K14" s="60"/>
     </row>
     <row r="15" spans="2:11">
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="C15" s="62">
+      <c r="C15" s="61">
         <v>0.05</v>
       </c>
       <c r="D15" s="60"/>
-      <c r="E15" s="61" t="s">
+      <c r="E15" s="74" t="s">
         <v>205</v>
       </c>
-      <c r="F15" s="61"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="68"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="67"/>
       <c r="K15" s="60"/>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="61" t="s">
         <v>206</v>
       </c>
-      <c r="C16" s="62">
+      <c r="C16" s="61">
         <v>94</v>
       </c>
       <c r="D16" s="60"/>
-      <c r="E16" s="62" t="s">
+      <c r="E16" s="61" t="s">
         <v>207</v>
       </c>
-      <c r="F16" s="62">
+      <c r="F16" s="61">
         <v>1</v>
       </c>
       <c r="G16" s="60"/>
       <c r="H16" s="60"/>
       <c r="I16" s="60"/>
-      <c r="J16" s="69"/>
+      <c r="J16" s="68"/>
       <c r="K16" s="60"/>
     </row>
     <row r="17" spans="2:11">
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="61" t="s">
         <v>208</v>
       </c>
-      <c r="C17" s="62">
+      <c r="C17" s="61">
         <v>0.51</v>
       </c>
       <c r="D17" s="60"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62">
+      <c r="E17" s="61"/>
+      <c r="F17" s="61">
         <v>3</v>
       </c>
       <c r="G17" s="60"/>
       <c r="H17" s="60"/>
       <c r="I17" s="60"/>
-      <c r="J17" s="69"/>
+      <c r="J17" s="68"/>
       <c r="K17" s="60"/>
     </row>
     <row r="18" spans="2:11">
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="61" t="s">
         <v>200</v>
       </c>
-      <c r="C18" s="62">
+      <c r="C18" s="61">
         <f>((100-C16)/100)/2</f>
         <v>0.03</v>
       </c>
       <c r="D18" s="60"/>
-      <c r="E18" s="62" t="s">
+      <c r="E18" s="61" t="s">
         <v>209</v>
       </c>
-      <c r="F18" s="62">
+      <c r="F18" s="61">
         <f>F17^2</f>
         <v>9</v>
       </c>
       <c r="G18" s="60"/>
       <c r="H18" s="60"/>
       <c r="I18" s="60"/>
-      <c r="J18" s="69"/>
+      <c r="J18" s="68"/>
       <c r="K18" s="60"/>
     </row>
     <row r="19" spans="2:11">
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="61" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="70">
+      <c r="C19" s="69">
         <f>_xlfn.NORM.INV(1-C18,0,1)</f>
         <v>1.8807936081512504</v>
       </c>
       <c r="D19" s="60"/>
-      <c r="E19" s="71"/>
+      <c r="E19" s="70"/>
       <c r="F19" s="60"/>
       <c r="G19" s="60"/>
       <c r="H19" s="60"/>
       <c r="I19" s="60"/>
-      <c r="J19" s="69"/>
+      <c r="J19" s="68"/>
       <c r="K19" s="60"/>
     </row>
     <row r="20" spans="2:11">
-      <c r="B20" s="63" t="s">
+      <c r="B20" s="62" t="s">
         <v>211</v>
       </c>
-      <c r="C20" s="65">
+      <c r="C20" s="64">
         <f xml:space="preserve"> C17*(1-C17)*((C19/C15)^2)</f>
         <v>353.59696426240129</v>
       </c>
       <c r="D20" s="60"/>
-      <c r="E20" s="71" t="s">
+      <c r="E20" s="70" t="s">
         <v>212</v>
       </c>
       <c r="F20" s="60"/>
       <c r="G20" s="60"/>
       <c r="H20" s="60"/>
       <c r="I20" s="60"/>
-      <c r="J20" s="69"/>
+      <c r="J20" s="68"/>
       <c r="K20" s="60"/>
     </row>
     <row r="21" spans="2:11">
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="62" t="s">
         <v>213</v>
       </c>
-      <c r="C21" s="65">
+      <c r="C21" s="64">
         <f>0.25*((C19/C15)^2)</f>
         <v>353.7384596462598</v>
       </c>
       <c r="D21" s="60"/>
-      <c r="E21" s="72" t="s">
+      <c r="E21" s="71" t="s">
         <v>214</v>
       </c>
-      <c r="F21" s="73"/>
-      <c r="G21" s="73"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="73"/>
-      <c r="J21" s="74"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="73"/>
       <c r="K21" s="60"/>
     </row>
     <row r="22" spans="2:11">
@@ -4555,6 +4722,335 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7934B88-A85A-EB42-B4EC-BEBEC08109DD}">
+  <dimension ref="B4:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:10">
+      <c r="B4" s="77" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="77"/>
+      <c r="E4" s="77" t="s">
+        <v>216</v>
+      </c>
+      <c r="F4" s="77"/>
+      <c r="H4" s="77" t="s">
+        <v>217</v>
+      </c>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="78"/>
+      <c r="C5" s="79"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="75" t="s">
+        <v>218</v>
+      </c>
+      <c r="C6" s="75">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="E6" s="80" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="81">
+        <v>120.7</v>
+      </c>
+      <c r="H6" s="75" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="32">
+        <v>20</v>
+      </c>
+      <c r="J6" s="32"/>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="76" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="76">
+        <v>25</v>
+      </c>
+      <c r="E7" s="82" t="s">
+        <v>220</v>
+      </c>
+      <c r="F7" s="83">
+        <v>12.4</v>
+      </c>
+      <c r="H7" s="75" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="32">
+        <v>30</v>
+      </c>
+      <c r="J7" s="32"/>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="84" t="s">
+        <v>221</v>
+      </c>
+      <c r="C8" s="85">
+        <f>_xlfn.T.INV(C6,C7)</f>
+        <v>1.5917851223801218</v>
+      </c>
+      <c r="E8" s="86" t="s">
+        <v>222</v>
+      </c>
+      <c r="F8" s="87">
+        <v>99</v>
+      </c>
+      <c r="H8" s="75"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="84" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9" s="85">
+        <f>ABS(C8)</f>
+        <v>1.5917851223801218</v>
+      </c>
+      <c r="E9" s="88" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="89">
+        <v>40</v>
+      </c>
+      <c r="H9" s="90" t="s">
+        <v>91</v>
+      </c>
+      <c r="I9" s="91">
+        <f>(I6+I7)/2</f>
+        <v>25</v>
+      </c>
+      <c r="J9" s="32"/>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="E10" s="75" t="s">
+        <v>200</v>
+      </c>
+      <c r="F10" s="32">
+        <f>((100-F8)/100 )/2</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H10" s="90" t="s">
+        <v>224</v>
+      </c>
+      <c r="I10" s="91">
+        <f>I7-I9</f>
+        <v>5</v>
+      </c>
+      <c r="J10" s="32"/>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="75" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="75">
+        <v>80</v>
+      </c>
+      <c r="E11" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="F11" s="32">
+        <f>ABS(_xlfn.T.INV(F10,F9-1))</f>
+        <v>2.7079131835176615</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="75" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" s="75">
+        <v>14</v>
+      </c>
+      <c r="E12" s="84" t="s">
+        <v>202</v>
+      </c>
+      <c r="F12" s="92" t="e">
+        <f>F$30- (F$35*(F$31/SQRT(F$33)))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="75" t="s">
+        <v>226</v>
+      </c>
+      <c r="C13" s="75">
+        <f>((100-C11)/100)/2</f>
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="84" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="92" t="e">
+        <f>F$30 +(F$35*(F$31/SQRT(F$33)))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="84" t="s">
+        <v>227</v>
+      </c>
+      <c r="C14" s="85">
+        <f>ABS(_xlfn.T.INV(C13,C12))</f>
+        <v>1.3450303744546506</v>
+      </c>
+      <c r="H14" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="H16" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="I16" s="32">
+        <v>23.86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="77" t="s">
+        <v>230</v>
+      </c>
+      <c r="C17" s="77"/>
+      <c r="H17" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="I17" s="32">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="H18" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="I18" s="32">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="75" t="s">
+        <v>199</v>
+      </c>
+      <c r="C19" s="75">
+        <v>4</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" s="32">
+        <v>23.803999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="75" t="s">
+        <v>233</v>
+      </c>
+      <c r="C20" s="75">
+        <v>99</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20" s="32">
+        <v>23.916</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="75" t="s">
+        <v>231</v>
+      </c>
+      <c r="C21" s="75">
+        <v>15.4</v>
+      </c>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
+      <c r="H22" s="91" t="s">
+        <v>199</v>
+      </c>
+      <c r="I22" s="91">
+        <f>I20-I16</f>
+        <v>5.6000000000000938E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="75" t="s">
+        <v>200</v>
+      </c>
+      <c r="C23" s="75">
+        <f>((100-C20)/100 )/2</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H23" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="75" t="s">
+        <v>210</v>
+      </c>
+      <c r="C24" s="93">
+        <f>_xlfn.NORM.INV(1-C23,0,1)</f>
+        <v>2.5758293035488999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="94" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="95">
+        <f>((C24*C21)/C19)^2</f>
+        <v>98.345754868636917</v>
+      </c>
+      <c r="D26" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="B17:C17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFCA351-70B0-5244-BA65-285CF6942DC3}">
   <dimension ref="A1:I26"/>
   <sheetViews>
@@ -4857,7 +5353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74F7077-45B6-E742-951B-BF30C929E163}">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -5000,7 +5496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1764C7-EB3F-884D-A423-6A64CF5D743E}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -5068,7 +5564,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7883183-3309-E141-80C9-0F546E3ED993}">
   <dimension ref="A6:D17"/>
   <sheetViews>
@@ -5195,7 +5691,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD5251E-A9B7-7F4B-A78E-2F9C7E161BB7}">
   <dimension ref="A1:H57"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added Population and Mean Porportion (Chapter 10)
</commit_message>
<xml_diff>
--- a/Midterm Excel Sheet.xlsx
+++ b/Midterm Excel Sheet.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/unghour/Desktop/Business-Stats-Excel-Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E554ADD-F480-A44C-B80A-F1D1B1EC541D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF7E276-F47E-A84C-BA7F-693501488E85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" activeTab="3" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" activeTab="1" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
   </bookViews>
   <sheets>
     <sheet name="Random Variable x" sheetId="1" r:id="rId1"/>
-    <sheet name="Normal Distribution" sheetId="6" r:id="rId2"/>
-    <sheet name="Chapter 9" sheetId="9" r:id="rId3"/>
-    <sheet name="t-values" sheetId="10" r:id="rId4"/>
-    <sheet name="Chapter 8" sheetId="8" r:id="rId5"/>
-    <sheet name="Binomial Probability" sheetId="2" r:id="rId6"/>
-    <sheet name="x &amp; Probability" sheetId="4" r:id="rId7"/>
-    <sheet name="Expected Value" sheetId="5" r:id="rId8"/>
-    <sheet name="Poisson" sheetId="3" r:id="rId9"/>
+    <sheet name="Chpater 10" sheetId="11" r:id="rId2"/>
+    <sheet name="Normal Distribution" sheetId="6" r:id="rId3"/>
+    <sheet name="Chapter 9" sheetId="9" r:id="rId4"/>
+    <sheet name="t-values" sheetId="10" r:id="rId5"/>
+    <sheet name="Chapter 8" sheetId="8" r:id="rId6"/>
+    <sheet name="Binomial Probability" sheetId="2" r:id="rId7"/>
+    <sheet name="x &amp; Probability" sheetId="4" r:id="rId8"/>
+    <sheet name="Expected Value" sheetId="5" r:id="rId9"/>
+    <sheet name="Poisson" sheetId="3" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,8 +41,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="268">
   <si>
     <t>x</t>
   </si>
@@ -749,13 +772,109 @@
   </si>
   <si>
     <t>(round up to one more value ex: 48 then should be 49)</t>
+  </si>
+  <si>
+    <t>Population Proportion (Left-Tailed Test)</t>
+  </si>
+  <si>
+    <t>Population Proportion (Two-Tailed Test)</t>
+  </si>
+  <si>
+    <t>p-zero %</t>
+  </si>
+  <si>
+    <t>keyword</t>
+  </si>
+  <si>
+    <t>"is given"</t>
+  </si>
+  <si>
+    <t>"can assume to be"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">np(1-p) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">np(1-p) &gt;= 10? </t>
+  </si>
+  <si>
+    <t>p-cap</t>
+  </si>
+  <si>
+    <t>z-zero</t>
+  </si>
+  <si>
+    <t>(do not round up)</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p&gt;a? </t>
+  </si>
+  <si>
+    <t>Find Lower and Upper Bound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If np(1-p) &lt; 10 </t>
+  </si>
+  <si>
+    <t>p-zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p-zero </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change this -&gt;***new x value </t>
+  </si>
+  <si>
+    <t>np-zero(1-p-zero) &gt;= 10</t>
+  </si>
+  <si>
+    <t>z-value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p-cap </t>
+  </si>
+  <si>
+    <t>p (less than x)</t>
+  </si>
+  <si>
+    <t>P-value( &gt;= )</t>
+  </si>
+  <si>
+    <t>round up ex:  0.45 -&gt; 0.46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P-value ( &lt;= ) </t>
+  </si>
+  <si>
+    <t>means (u)</t>
+  </si>
+  <si>
+    <t>x-bar (sample mean)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s </t>
+  </si>
+  <si>
+    <t>Is (n &gt;= 30)?</t>
+  </si>
+  <si>
+    <t>t-zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P-value </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reject null hypothesis? </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="9">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.000000000000000000000_);_(* \(#,##0.000000000000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -763,8 +882,10 @@
     <numFmt numFmtId="167" formatCode="0.00000000"/>
     <numFmt numFmtId="168" formatCode="0.000000"/>
     <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="28">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -930,8 +1051,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -968,8 +1124,56 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1100,12 +1304,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1258,17 +1497,11 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1312,6 +1545,92 @@
     <xf numFmtId="164" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="1" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1634,7 +1953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E068083-BD50-CB42-8AAE-F1525497B3A5}">
   <dimension ref="A1:AN226"/>
   <sheetViews>
-    <sheetView zoomScale="82" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView zoomScale="131" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -3573,12 +3892,950 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD5251E-A9B7-7F4B-A78E-2F9C7E161BB7}">
+  <dimension ref="A1:H57"/>
+  <sheetViews>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="17">
+      <c r="A1" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17">
+      <c r="A2" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17">
+      <c r="A3" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17">
+      <c r="A5" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17">
+      <c r="A6" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="29">
+        <v>0.12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="B7" s="2"/>
+      <c r="G7" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17">
+      <c r="A8" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="29">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8">
+        <f>H6*H7</f>
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17">
+      <c r="A9" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17">
+      <c r="A10" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="29">
+        <v>1.68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10">
+        <f>B6*B8</f>
+        <v>1.68</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="26">
+      <c r="A11" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="G11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17">
+      <c r="A12" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="29">
+        <f>_xlfn.POISSON.DIST(B9,B10, FALSE)</f>
+        <v>5.8198054157415332E-3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17">
+      <c r="A13" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="29">
+        <f>_xlfn.POISSON.DIST(B9 - 1, B10, TRUE)</f>
+        <v>0.99242454151988369</v>
+      </c>
+      <c r="G13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="17">
+      <c r="A14" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="29">
+        <f>1 - B13</f>
+        <v>7.575458480116315E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="17">
+      <c r="A16" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17">
+      <c r="A17" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17">
+      <c r="A18" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="16">
+        <f>B16</f>
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <f>_xlfn.POISSON.DIST(A19, B$10, FALSE)</f>
+        <v>6.1860176612899005E-2</v>
+      </c>
+      <c r="C19" t="str">
+        <f>IF(A19&gt;B$17,"ERASE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="16">
+        <f>A19+1</f>
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ref="B20:B26" si="0">_xlfn.POISSON.DIST(A20, B$10, FALSE)</f>
+        <v>2.0785019341934056E-2</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" ref="C20:C26" si="1">IF(A20&gt;B$17,"ERASE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="16">
+        <f t="shared" ref="A21:A26" si="2">A20+1</f>
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>5.8198054157415332E-3</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="16">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>1.3967532997779695E-3</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="16">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>2.9331819295337359E-4</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="1"/>
+        <v>ERASE</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="16">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>5.4752729351296345E-5</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="1"/>
+        <v>ERASE</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="16">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>9.1984585310177959E-6</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="1"/>
+        <v>ERASE</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="16">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>1.4048554847372632E-6</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="1"/>
+        <v>ERASE</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" s="20">
+        <f>SUMIF(C19:C26,"",B19:B26)</f>
+        <v>8.9861754670352567E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41">
+        <v>106</v>
+      </c>
+      <c r="E41">
+        <f>_xlfn.POISSON.DIST(6, 7.2, FALSE)</f>
+        <v>0.14445820444290103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>0.34905660379999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="20">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" s="20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49">
+        <f>B47*B48</f>
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52">
+        <f>_xlfn.POISSON.DIST(B51, B49, FALSE)</f>
+        <v>0.13372702354142837</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>109</v>
+      </c>
+      <c r="B53">
+        <f>_xlfn.POISSON.DIST(B51 - 1, B49, TRUE)</f>
+        <v>0.56894123888215242</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54">
+        <f xml:space="preserve"> 1 - B53</f>
+        <v>0.43105876111784758</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56">
+        <f>_xlfn.POISSON.DIST(1, 7.2, FALSE)</f>
+        <v>5.3754178203120903E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57">
+        <f xml:space="preserve"> 1 - A56</f>
+        <v>0.99462458217968786</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5B9FCC-C544-FD4E-85A9-D1AE64548C87}">
+  <dimension ref="B3:G59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7">
+      <c r="B3" s="96">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="95" t="s">
+        <v>236</v>
+      </c>
+      <c r="C5" s="95"/>
+      <c r="F5" s="95" t="s">
+        <v>237</v>
+      </c>
+      <c r="G5" s="95"/>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="76"/>
+      <c r="C6" s="97"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="97"/>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="84" t="s">
+        <v>238</v>
+      </c>
+      <c r="C7" s="85">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="84" t="s">
+        <v>238</v>
+      </c>
+      <c r="G7" s="85">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="78" t="s">
+        <v>197</v>
+      </c>
+      <c r="C8" s="79">
+        <v>1447</v>
+      </c>
+      <c r="F8" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="87">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="87">
+        <v>740</v>
+      </c>
+      <c r="F9" s="98" t="s">
+        <v>197</v>
+      </c>
+      <c r="G9" s="99">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="100" t="s">
+        <v>218</v>
+      </c>
+      <c r="C10" s="101">
+        <v>0.1</v>
+      </c>
+      <c r="F10" s="100" t="s">
+        <v>218</v>
+      </c>
+      <c r="G10" s="101">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="74" t="s">
+        <v>239</v>
+      </c>
+      <c r="C11" s="74" t="s">
+        <v>240</v>
+      </c>
+      <c r="F11" s="74" t="s">
+        <v>239</v>
+      </c>
+      <c r="G11" s="74" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="102" t="s">
+        <v>242</v>
+      </c>
+      <c r="C13" s="103">
+        <f>C8*C7*(1-C7)</f>
+        <v>361.75</v>
+      </c>
+      <c r="F13" s="102" t="s">
+        <v>242</v>
+      </c>
+      <c r="G13" s="104">
+        <f>G9*G7*(1-G7)</f>
+        <v>4.7328999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="82" t="s">
+        <v>243</v>
+      </c>
+      <c r="C14" s="105" t="b">
+        <f>IF(C13&gt;=10, TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="82" t="s">
+        <v>243</v>
+      </c>
+      <c r="G14" s="82" t="b">
+        <f>IF(G13&gt;=10, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="74"/>
+      <c r="C15" s="32"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="32"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="106" t="s">
+        <v>244</v>
+      </c>
+      <c r="C16" s="107">
+        <f>C9/C8</f>
+        <v>0.51140290255701448</v>
+      </c>
+      <c r="F16" s="74" t="s">
+        <v>244</v>
+      </c>
+      <c r="G16" s="32">
+        <f>G8/G9</f>
+        <v>0.68421052631578949</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="40"/>
+      <c r="C17" s="108"/>
+      <c r="F17" s="109" t="s">
+        <v>245</v>
+      </c>
+      <c r="G17" s="110">
+        <f>(G16-G7)/SQRT((G7*(1-G7))/G9)</f>
+        <v>1.3468026309736418</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="109" t="s">
+        <v>245</v>
+      </c>
+      <c r="C18" s="111">
+        <f>(C16-C7)/SQRT((C7*(1-C7))/C8)</f>
+        <v>0.86752035639687086</v>
+      </c>
+      <c r="D18" t="s">
+        <v>246</v>
+      </c>
+      <c r="F18" s="74"/>
+      <c r="G18" s="32"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="74"/>
+      <c r="C19" s="32"/>
+      <c r="F19" s="112" t="s">
+        <v>247</v>
+      </c>
+      <c r="G19" s="113">
+        <f>TDIST(ABS(G17),G9-1,2)</f>
+        <v>0.19475749775710713</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="112" t="s">
+        <v>247</v>
+      </c>
+      <c r="C20" s="114">
+        <f>TDIST(ABS(C18),C8-1,1)</f>
+        <v>0.1929004515737997</v>
+      </c>
+      <c r="F20" s="115" t="s">
+        <v>248</v>
+      </c>
+      <c r="G20" s="116" t="str">
+        <f>IF(G19&gt;G10, "P &gt; a", "P &lt; a")</f>
+        <v>P &gt; a</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="115" t="s">
+        <v>248</v>
+      </c>
+      <c r="C21" s="116" t="str">
+        <f>IF(C20&gt;C10, "P &gt; a", "P &lt; a")</f>
+        <v>P &gt; a</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="95" t="s">
+        <v>249</v>
+      </c>
+      <c r="C24" s="95"/>
+      <c r="F24" s="117" t="s">
+        <v>250</v>
+      </c>
+      <c r="G24" s="117"/>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="85">
+        <v>26</v>
+      </c>
+      <c r="F26" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="119">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="120" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="120">
+        <v>50</v>
+      </c>
+      <c r="F27" s="118" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="119">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="79" t="s">
+        <v>251</v>
+      </c>
+      <c r="C28" s="79">
+        <v>0.5</v>
+      </c>
+      <c r="F28" s="118" t="s">
+        <v>252</v>
+      </c>
+      <c r="G28" s="119">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="121" t="s">
+        <v>198</v>
+      </c>
+      <c r="C29" s="121">
+        <v>0.3886</v>
+      </c>
+      <c r="F29" s="118" t="s">
+        <v>253</v>
+      </c>
+      <c r="G29" s="119">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="40"/>
+      <c r="C30" s="108"/>
+      <c r="F30" s="122"/>
+      <c r="G30" s="123"/>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="C31" s="32">
+        <f>C27*(C28/100)*(1-(C28/100))</f>
+        <v>0.24875</v>
+      </c>
+      <c r="F31" s="124" t="s">
+        <v>254</v>
+      </c>
+      <c r="G31" s="125">
+        <f>G27*(G28/100)*(1-(G28/100))</f>
+        <v>11.764800000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="32"/>
+      <c r="C32" s="126"/>
+      <c r="F32" s="127" t="s">
+        <v>196</v>
+      </c>
+      <c r="G32" s="127" t="e" cm="1">
+        <f t="array" ref="G32">IF(G31 &gt;= 10, TURE, FALSE)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="C33" s="32">
+        <f>((100-C29) /2)/100</f>
+        <v>0.49805700000000003</v>
+      </c>
+      <c r="F33" s="128"/>
+      <c r="G33" s="97"/>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="C34" s="32">
+        <f>_xlfn.NORM.INV((1-C33),0,1)</f>
+        <v>4.87039799247672E-3</v>
+      </c>
+      <c r="F34" s="74" t="s">
+        <v>244</v>
+      </c>
+      <c r="G34" s="32">
+        <f>G26/G27</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" s="122"/>
+      <c r="C35" s="123"/>
+      <c r="F35" s="74" t="s">
+        <v>255</v>
+      </c>
+      <c r="G35" s="32"/>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="129" t="s">
+        <v>256</v>
+      </c>
+      <c r="C36" s="129">
+        <f>C26/C27</f>
+        <v>0.52</v>
+      </c>
+      <c r="F36" s="74"/>
+      <c r="G36" s="130"/>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" s="131"/>
+      <c r="C37" s="132"/>
+      <c r="F37" s="74" t="s">
+        <v>257</v>
+      </c>
+      <c r="G37" s="130">
+        <f>_xlfn.BINOM.DIST(G29-1,G27,G28/100,TRUE)</f>
+        <v>0.99964533162387259</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="105" t="s">
+        <v>202</v>
+      </c>
+      <c r="C38" s="133">
+        <f>C36-(C34*SQRT((C36*(1-C36))/C27))</f>
+        <v>0.51965588647685279</v>
+      </c>
+      <c r="F38" s="134" t="s">
+        <v>258</v>
+      </c>
+      <c r="G38" s="135">
+        <f>1-G37</f>
+        <v>3.5466837612740942E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" s="105" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="133">
+        <f>C36+(C34*SQRT((C36*(1-C36))/C27))</f>
+        <v>0.52034411352314724</v>
+      </c>
+      <c r="D39" t="s">
+        <v>259</v>
+      </c>
+      <c r="F39" s="136" t="s">
+        <v>260</v>
+      </c>
+      <c r="G39" s="137">
+        <f>_xlfn.BINOM.DIST(G29,G27,G28/100,TRUE)</f>
+        <v>0.99989936814098268</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="B44" s="96">
+        <v>10.3</v>
+      </c>
+      <c r="C44" s="96"/>
+      <c r="D44" s="96"/>
+      <c r="E44" s="96"/>
+      <c r="F44" s="96"/>
+      <c r="G44" s="96"/>
+    </row>
+    <row r="48" spans="2:7">
+      <c r="B48" s="101" t="s">
+        <v>261</v>
+      </c>
+      <c r="C48" s="101">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" s="101" t="s">
+        <v>262</v>
+      </c>
+      <c r="C49" s="101">
+        <v>1.681</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50" s="101" t="s">
+        <v>263</v>
+      </c>
+      <c r="C50">
+        <v>4.8053000000000002E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" s="101" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="101">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" s="101" t="s">
+        <v>218</v>
+      </c>
+      <c r="C52" s="101">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53" s="32"/>
+      <c r="C53" s="32"/>
+    </row>
+    <row r="54" spans="2:3">
+      <c r="B54" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="C54" s="138" t="str">
+        <f>IF(C51&gt;=30, "Yes", "No")</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="B56" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="C56" s="139">
+        <f>(C49-C48)/ (C50/SQRT(C51))</f>
+        <v>0.72089185173415637</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57" s="140" t="s">
+        <v>266</v>
+      </c>
+      <c r="C57" s="135">
+        <f>TDIST(ABS(C56),C51-1,1)</f>
+        <v>0.24300745710152599</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3">
+      <c r="B59" s="141" t="s">
+        <v>267</v>
+      </c>
+      <c r="C59" s="138" t="str">
+        <f>IF(C57&gt;C52, "Do not reject", "Reject")</f>
+        <v>Do not reject</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B44:G44"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C96CE9-B77B-704D-8A1F-7836B7353FCF}">
   <dimension ref="A1:AI33"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="AA5" sqref="AA5"/>
+    <sheetView topLeftCell="E1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3683,7 +4940,7 @@
         <v>127</v>
       </c>
       <c r="AA2" s="49">
-        <v>0.16</v>
+        <v>0.08</v>
       </c>
       <c r="AD2" s="32" t="s">
         <v>125</v>
@@ -3800,7 +5057,7 @@
       </c>
       <c r="AA4" s="49">
         <f xml:space="preserve"> 1 - AA2</f>
-        <v>0.84</v>
+        <v>0.92</v>
       </c>
       <c r="AD4" s="32" t="s">
         <v>79</v>
@@ -3862,7 +5119,7 @@
       </c>
       <c r="AA5" s="59">
         <f>_xlfn.NORM.INV(AA4,0, 1)</f>
-        <v>0.9944578832097497</v>
+        <v>1.4050715603096329</v>
       </c>
       <c r="AH5" s="32"/>
       <c r="AI5" s="32"/>
@@ -4292,7 +5549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77044CB3-A584-0B47-8E5D-C4DB8D5DE250}">
   <dimension ref="B2:K22"/>
   <sheetViews>
@@ -4320,18 +5577,18 @@
       <c r="K2" s="60"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="94" t="s">
         <v>190</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="94"/>
       <c r="D3" s="60"/>
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="74" t="s">
+      <c r="H3" s="94" t="s">
         <v>191</v>
       </c>
-      <c r="I3" s="74"/>
+      <c r="I3" s="94"/>
       <c r="J3" s="60"/>
       <c r="K3" s="60"/>
     </row>
@@ -4552,10 +5809,10 @@
       <c r="K13" s="60"/>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" s="74" t="s">
+      <c r="B14" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="C14" s="74"/>
+      <c r="C14" s="94"/>
       <c r="D14" s="60"/>
       <c r="E14" s="60"/>
       <c r="F14" s="60"/>
@@ -4573,10 +5830,10 @@
         <v>0.05</v>
       </c>
       <c r="D15" s="60"/>
-      <c r="E15" s="74" t="s">
+      <c r="E15" s="94" t="s">
         <v>205</v>
       </c>
-      <c r="F15" s="74"/>
+      <c r="F15" s="94"/>
       <c r="G15" s="66"/>
       <c r="H15" s="66"/>
       <c r="I15" s="66"/>
@@ -4721,12 +5978,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7934B88-A85A-EB42-B4EC-BEBEC08109DD}">
   <dimension ref="B4:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A3" zoomScale="160" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4740,23 +5997,23 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:10">
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="95" t="s">
         <v>215</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="E4" s="77" t="s">
+      <c r="C4" s="95"/>
+      <c r="E4" s="95" t="s">
         <v>216</v>
       </c>
-      <c r="F4" s="77"/>
-      <c r="H4" s="77" t="s">
+      <c r="F4" s="95"/>
+      <c r="H4" s="95" t="s">
         <v>217</v>
       </c>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
     </row>
     <row r="5" spans="2:10">
-      <c r="B5" s="78"/>
-      <c r="C5" s="79"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="77"/>
       <c r="E5" s="32"/>
       <c r="F5" s="32"/>
       <c r="H5" s="32"/>
@@ -4764,19 +6021,19 @@
       <c r="J5" s="32"/>
     </row>
     <row r="6" spans="2:10">
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="74" t="s">
         <v>218</v>
       </c>
-      <c r="C6" s="75">
+      <c r="C6" s="74">
         <v>0.93799999999999994</v>
       </c>
-      <c r="E6" s="80" t="s">
+      <c r="E6" s="78" t="s">
         <v>91</v>
       </c>
-      <c r="F6" s="81">
-        <v>120.7</v>
-      </c>
-      <c r="H6" s="75" t="s">
+      <c r="F6" s="79">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="H6" s="74" t="s">
         <v>67</v>
       </c>
       <c r="I6" s="32">
@@ -4785,19 +6042,19 @@
       <c r="J6" s="32"/>
     </row>
     <row r="7" spans="2:10">
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="75" t="s">
         <v>219</v>
       </c>
-      <c r="C7" s="76">
+      <c r="C7" s="75">
         <v>25</v>
       </c>
-      <c r="E7" s="82" t="s">
+      <c r="E7" s="80" t="s">
         <v>220</v>
       </c>
-      <c r="F7" s="83">
-        <v>12.4</v>
-      </c>
-      <c r="H7" s="75" t="s">
+      <c r="F7" s="81">
+        <v>5.8</v>
+      </c>
+      <c r="H7" s="74" t="s">
         <v>68</v>
       </c>
       <c r="I7" s="32">
@@ -4806,116 +6063,116 @@
       <c r="J7" s="32"/>
     </row>
     <row r="8" spans="2:10">
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="82" t="s">
         <v>221</v>
       </c>
-      <c r="C8" s="85">
+      <c r="C8" s="83">
         <f>_xlfn.T.INV(C6,C7)</f>
         <v>1.5917851223801218</v>
       </c>
-      <c r="E8" s="86" t="s">
+      <c r="E8" s="84" t="s">
         <v>222</v>
       </c>
-      <c r="F8" s="87">
-        <v>99</v>
-      </c>
-      <c r="H8" s="75"/>
+      <c r="F8" s="85">
+        <v>90</v>
+      </c>
+      <c r="H8" s="74"/>
       <c r="I8" s="32"/>
       <c r="J8" s="32"/>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="82" t="s">
         <v>223</v>
       </c>
-      <c r="C9" s="85">
+      <c r="C9" s="83">
         <f>ABS(C8)</f>
         <v>1.5917851223801218</v>
       </c>
-      <c r="E9" s="88" t="s">
+      <c r="E9" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="89">
-        <v>40</v>
-      </c>
-      <c r="H9" s="90" t="s">
+      <c r="F9" s="87">
+        <v>22</v>
+      </c>
+      <c r="H9" s="88" t="s">
         <v>91</v>
       </c>
-      <c r="I9" s="91">
+      <c r="I9" s="89">
         <f>(I6+I7)/2</f>
         <v>25</v>
       </c>
       <c r="J9" s="32"/>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="E10" s="75" t="s">
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="E10" s="74" t="s">
         <v>200</v>
       </c>
       <c r="F10" s="32">
         <f>((100-F8)/100 )/2</f>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="H10" s="90" t="s">
+        <v>0.05</v>
+      </c>
+      <c r="H10" s="88" t="s">
         <v>224</v>
       </c>
-      <c r="I10" s="91">
+      <c r="I10" s="89">
         <f>I7-I9</f>
         <v>5</v>
       </c>
       <c r="J10" s="32"/>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="75">
+      <c r="C11" s="74">
         <v>80</v>
       </c>
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="74" t="s">
         <v>225</v>
       </c>
       <c r="F11" s="32">
         <f>ABS(_xlfn.T.INV(F10,F9-1))</f>
-        <v>2.7079131835176615</v>
+        <v>1.7207429028118781</v>
       </c>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" s="75" t="s">
+      <c r="B12" s="74" t="s">
         <v>219</v>
       </c>
-      <c r="C12" s="75">
+      <c r="C12" s="74">
         <v>14</v>
       </c>
-      <c r="E12" s="84" t="s">
+      <c r="E12" s="82" t="s">
         <v>202</v>
       </c>
-      <c r="F12" s="92" t="e">
-        <f>F$30- (F$35*(F$31/SQRT(F$33)))</f>
-        <v>#DIV/0!</v>
+      <c r="F12" s="90">
+        <f>F6-(F11*(F7/SQRT(F9)))</f>
+        <v>17.472191006648718</v>
       </c>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="74" t="s">
         <v>226</v>
       </c>
-      <c r="C13" s="75">
+      <c r="C13" s="74">
         <f>((100-C11)/100)/2</f>
         <v>0.1</v>
       </c>
-      <c r="E13" s="84" t="s">
+      <c r="E13" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="92" t="e">
-        <f>F$30 +(F$35*(F$31/SQRT(F$33)))</f>
-        <v>#DIV/0!</v>
+      <c r="F13" s="90">
+        <f>F6+ (F11*(F7/SQRT(F9)))</f>
+        <v>21.727808993351285</v>
       </c>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="84" t="s">
+      <c r="B14" s="82" t="s">
         <v>227</v>
       </c>
-      <c r="C14" s="85">
+      <c r="C14" s="83">
         <f>ABS(_xlfn.T.INV(C13,C12))</f>
         <v>1.3450303744546506</v>
       </c>
@@ -4932,10 +6189,10 @@
       </c>
     </row>
     <row r="17" spans="2:9">
-      <c r="B17" s="77" t="s">
+      <c r="B17" s="95" t="s">
         <v>230</v>
       </c>
-      <c r="C17" s="77"/>
+      <c r="C17" s="95"/>
       <c r="H17" s="32" t="s">
         <v>231</v>
       </c>
@@ -4954,10 +6211,10 @@
       </c>
     </row>
     <row r="19" spans="2:9">
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="74" t="s">
         <v>199</v>
       </c>
-      <c r="C19" s="75">
+      <c r="C19" s="74">
         <v>4</v>
       </c>
       <c r="H19" s="32" t="s">
@@ -4968,10 +6225,10 @@
       </c>
     </row>
     <row r="20" spans="2:9">
-      <c r="B20" s="75" t="s">
+      <c r="B20" s="74" t="s">
         <v>233</v>
       </c>
-      <c r="C20" s="75">
+      <c r="C20" s="74">
         <v>99</v>
       </c>
       <c r="H20" s="32" t="s">
@@ -4982,31 +6239,31 @@
       </c>
     </row>
     <row r="21" spans="2:9">
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="74" t="s">
         <v>231</v>
       </c>
-      <c r="C21" s="75">
+      <c r="C21" s="74">
         <v>15.4</v>
       </c>
       <c r="H21" s="32"/>
       <c r="I21" s="32"/>
     </row>
     <row r="22" spans="2:9">
-      <c r="B22" s="75"/>
-      <c r="C22" s="75"/>
-      <c r="H22" s="91" t="s">
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
+      <c r="H22" s="89" t="s">
         <v>199</v>
       </c>
-      <c r="I22" s="91">
+      <c r="I22" s="89">
         <f>I20-I16</f>
         <v>5.6000000000000938E-2</v>
       </c>
     </row>
     <row r="23" spans="2:9">
-      <c r="B23" s="75" t="s">
+      <c r="B23" s="74" t="s">
         <v>200</v>
       </c>
-      <c r="C23" s="75">
+      <c r="C23" s="74">
         <f>((100-C20)/100 )/2</f>
         <v>5.0000000000000001E-3</v>
       </c>
@@ -5015,23 +6272,23 @@
       </c>
     </row>
     <row r="24" spans="2:9">
-      <c r="B24" s="75" t="s">
+      <c r="B24" s="74" t="s">
         <v>210</v>
       </c>
-      <c r="C24" s="93">
+      <c r="C24" s="91">
         <f>_xlfn.NORM.INV(1-C23,0,1)</f>
         <v>2.5758293035488999</v>
       </c>
     </row>
     <row r="25" spans="2:9">
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="74"/>
     </row>
     <row r="26" spans="2:9">
-      <c r="B26" s="94" t="s">
+      <c r="B26" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="95">
+      <c r="C26" s="93">
         <f>((C24*C21)/C19)^2</f>
         <v>98.345754868636917</v>
       </c>
@@ -5050,7 +6307,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFCA351-70B0-5244-BA65-285CF6942DC3}">
   <dimension ref="A1:I26"/>
   <sheetViews>
@@ -5353,7 +6610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74F7077-45B6-E742-951B-BF30C929E163}">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -5496,7 +6753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1764C7-EB3F-884D-A423-6A64CF5D743E}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -5564,7 +6821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7883183-3309-E141-80C9-0F546E3ED993}">
   <dimension ref="A6:D17"/>
   <sheetViews>
@@ -5689,405 +6946,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD5251E-A9B7-7F4B-A78E-2F9C7E161BB7}">
-  <dimension ref="A1:H57"/>
-  <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="17">
-      <c r="A1" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="17">
-      <c r="A2" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="17">
-      <c r="A3" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="17">
-      <c r="A5" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="17">
-      <c r="A6" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="29">
-        <v>0.12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>101</v>
-      </c>
-      <c r="H6">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="B7" s="2"/>
-      <c r="G7" t="s">
-        <v>102</v>
-      </c>
-      <c r="H7">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="17">
-      <c r="A8" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="29">
-        <v>14</v>
-      </c>
-      <c r="G8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H8">
-        <f>H6*H7</f>
-        <v>1.68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="17">
-      <c r="A9" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="29">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="17">
-      <c r="A10" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="29">
-        <v>1.68</v>
-      </c>
-      <c r="C10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10">
-        <f>B6*B8</f>
-        <v>1.68</v>
-      </c>
-      <c r="G10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="26">
-      <c r="A11" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="G11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="17">
-      <c r="A12" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="29">
-        <f>_xlfn.POISSON.DIST(B9,B10, FALSE)</f>
-        <v>5.8198054157415332E-3</v>
-      </c>
-      <c r="G12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="17">
-      <c r="A13" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="29">
-        <f>_xlfn.POISSON.DIST(B9 - 1, B10, TRUE)</f>
-        <v>0.99242454151988369</v>
-      </c>
-      <c r="G13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="17">
-      <c r="A14" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" s="29">
-        <f>1 - B13</f>
-        <v>7.575458480116315E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="17">
-      <c r="A16" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17">
-      <c r="A17" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17">
-      <c r="A18" s="21" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="16">
-        <f>B16</f>
-        <v>4</v>
-      </c>
-      <c r="B19">
-        <f>_xlfn.POISSON.DIST(A19, B$10, FALSE)</f>
-        <v>6.1860176612899005E-2</v>
-      </c>
-      <c r="C19" t="str">
-        <f>IF(A19&gt;B$17,"ERASE","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="16">
-        <f>A19+1</f>
-        <v>5</v>
-      </c>
-      <c r="B20">
-        <f t="shared" ref="B20:B26" si="0">_xlfn.POISSON.DIST(A20, B$10, FALSE)</f>
-        <v>2.0785019341934056E-2</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" ref="C20:C26" si="1">IF(A20&gt;B$17,"ERASE","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="16">
-        <f t="shared" ref="A21:A26" si="2">A20+1</f>
-        <v>6</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>5.8198054157415332E-3</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="16">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>1.3967532997779695E-3</v>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="16">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>2.9331819295337359E-4</v>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" si="1"/>
-        <v>ERASE</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="16">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>5.4752729351296345E-5</v>
-      </c>
-      <c r="C24" t="str">
-        <f t="shared" si="1"/>
-        <v>ERASE</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="16">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>9.1984585310177959E-6</v>
-      </c>
-      <c r="C25" t="str">
-        <f t="shared" si="1"/>
-        <v>ERASE</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="16">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>1.4048554847372632E-6</v>
-      </c>
-      <c r="C26" t="str">
-        <f t="shared" si="1"/>
-        <v>ERASE</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" s="20">
-        <f>SUMIF(C19:C26,"",B19:B26)</f>
-        <v>8.9861754670352567E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" t="s">
-        <v>90</v>
-      </c>
-      <c r="B41">
-        <v>106</v>
-      </c>
-      <c r="E41">
-        <f>_xlfn.POISSON.DIST(6, 7.2, FALSE)</f>
-        <v>0.14445820444290103</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42">
-        <v>0.34905660379999998</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" t="s">
-        <v>107</v>
-      </c>
-      <c r="B47" s="20">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" t="s">
-        <v>108</v>
-      </c>
-      <c r="B48" s="20">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
-        <v>91</v>
-      </c>
-      <c r="B49">
-        <f>B47*B48</f>
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
-        <v>92</v>
-      </c>
-      <c r="B52">
-        <f>_xlfn.POISSON.DIST(B51, B49, FALSE)</f>
-        <v>0.13372702354142837</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
-        <v>109</v>
-      </c>
-      <c r="B53">
-        <f>_xlfn.POISSON.DIST(B51 - 1, B49, TRUE)</f>
-        <v>0.56894123888215242</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
-        <v>94</v>
-      </c>
-      <c r="B54">
-        <f xml:space="preserve"> 1 - B53</f>
-        <v>0.43105876111784758</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56">
-        <f>_xlfn.POISSON.DIST(1, 7.2, FALSE)</f>
-        <v>5.3754178203120903E-3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57">
-        <f xml:space="preserve"> 1 - A56</f>
-        <v>0.99462458217968786</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Histogram and Quartile Range sheets
</commit_message>
<xml_diff>
--- a/Midterm Excel Sheet.xlsx
+++ b/Midterm Excel Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/unghour/Desktop/Business-Stats-Excel-Sheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanninoa/Desktop/updated stats/clean/Statistics-Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF7E276-F47E-A84C-BA7F-693501488E85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36C0BE3-E04B-FA4E-A3A4-FA588BED62EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" activeTab="1" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
+    <workbookView xWindow="1160" yWindow="1080" windowWidth="15640" windowHeight="18740" activeTab="7" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
   </bookViews>
   <sheets>
     <sheet name="Random Variable x" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,13 @@
     <sheet name="Normal Distribution" sheetId="6" r:id="rId3"/>
     <sheet name="Chapter 9" sheetId="9" r:id="rId4"/>
     <sheet name="t-values" sheetId="10" r:id="rId5"/>
-    <sheet name="Chapter 8" sheetId="8" r:id="rId6"/>
-    <sheet name="Binomial Probability" sheetId="2" r:id="rId7"/>
-    <sheet name="x &amp; Probability" sheetId="4" r:id="rId8"/>
-    <sheet name="Expected Value" sheetId="5" r:id="rId9"/>
-    <sheet name="Poisson" sheetId="3" r:id="rId10"/>
+    <sheet name="Histogram" sheetId="13" r:id="rId6"/>
+    <sheet name="Quartiles" sheetId="12" r:id="rId7"/>
+    <sheet name="Chapter 8" sheetId="8" r:id="rId8"/>
+    <sheet name="Binomial Probability" sheetId="2" r:id="rId9"/>
+    <sheet name="x &amp; Probability" sheetId="4" r:id="rId10"/>
+    <sheet name="Expected Value" sheetId="5" r:id="rId11"/>
+    <sheet name="Poisson" sheetId="3" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,30 +43,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="294">
   <si>
     <t>x</t>
   </si>
@@ -789,9 +769,6 @@
     <t>"is given"</t>
   </si>
   <si>
-    <t>"can assume to be"</t>
-  </si>
-  <si>
     <t xml:space="preserve">np(1-p) </t>
   </si>
   <si>
@@ -868,6 +845,177 @@
   </si>
   <si>
     <t xml:space="preserve">Reject null hypothesis? </t>
+  </si>
+  <si>
+    <t>A​ p-value is the probability of observing the actual​ result, a sample​ mean, for​ example, or something more unusual just by chance if the null hypothesis is true.</t>
+  </si>
+  <si>
+    <t>Type I Error: Rejecting null hypothesis (Hsub0) when Hsub0 is true</t>
+  </si>
+  <si>
+    <t>Type II Error: Rejecting Hsub1 when Hsub1 is true. Or not rejecting Hsub0 when Hsub1 is true</t>
+  </si>
+  <si>
+    <t>α = P(type I error) = P(rejecting Hsub0 when Hsub0 is true)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">β </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF4D4D4F"/>
+        <rFont val="STIXGeneral-Regular"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF4D4D4F"/>
+        <rFont val="STIXGeneral-Italic"/>
+      </rPr>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF4D4D4F"/>
+        <rFont val="STIXGeneral-Regular"/>
+      </rPr>
+      <t xml:space="preserve">(Type II error) = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF4D4D4F"/>
+        <rFont val="STIXGeneral-Italic"/>
+      </rPr>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF4D4D4F"/>
+        <rFont val="STIXGeneral-Regular"/>
+      </rPr>
+      <t>(not rejecting </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF4D4D4F"/>
+        <rFont val="STIXGeneral-Italic"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF4D4D4F"/>
+        <rFont val="STIXGeneral-Regular"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF4D4D4F"/>
+        <rFont val="STIXGeneral-Regular"/>
+      </rPr>
+      <t>when </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF4D4D4F"/>
+        <rFont val="STIXGeneral-Italic"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF4D4D4F"/>
+        <rFont val="STIXGeneral-Regular"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF4D4D4F"/>
+        <rFont val="STIXGeneral-Regular"/>
+      </rPr>
+      <t>is true)</t>
+    </r>
+  </si>
+  <si>
+    <t>level of significance alpha</t>
+  </si>
+  <si>
+    <t>IF P-VALUE is less than alpha, reject the null hypothesis</t>
+  </si>
+  <si>
+    <t>percent (integer)</t>
+  </si>
+  <si>
+    <t>IF P-Value is &gt; alpha, do not reject as there is not enough evdence</t>
+  </si>
+  <si>
+    <t>if P &gt; A, don't reject.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A​ P-value is the probability of observing a sample statistic as extreme or more extreme than the one observed under the assumption that the statement in the null hypothesis is true. </t>
+  </si>
+  <si>
+    <t>p value = .19</t>
+  </si>
+  <si>
+    <t>If the​ P-value for a particular test statistic is 0.19​, she expects results at least as extreme as the test statistic in about 19 of 100 samples if the null hypothesis is true.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">since the event is not unusual, don't reject </t>
+  </si>
+  <si>
+    <t>Statistical significance means that the result observed in a sample is unusual when the null hypothesis is assumed to be true.</t>
+  </si>
+  <si>
+    <t>if the interval (lower, upper) contains the proportion stated in the null hypothesis, there is insufficient evidence toward a changed result</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>^ change the &lt; and &gt; string values</t>
+  </si>
+  <si>
+    <t>Relative Freq</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Class upperbound</t>
+  </si>
+  <si>
+    <t>Class lowerbound</t>
+  </si>
+  <si>
+    <t>width?</t>
+  </si>
+  <si>
+    <t>How many classes?</t>
   </si>
 </sst>
 </file>
@@ -885,7 +1033,7 @@
     <numFmt numFmtId="170" formatCode="0.0"/>
     <numFmt numFmtId="171" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="33">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1085,6 +1233,34 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF4D4D4F"/>
+      <name val="STIXGeneral-Italic"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF4D4D4F"/>
+      <name val="Myriad"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF4D4D4F"/>
+      <name val="STIXGeneral-Regular"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF4D4D4F"/>
+      <name val="STIXGeneral-Regular"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="15">
@@ -1344,7 +1520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1545,15 +1721,6 @@
     <xf numFmtId="164" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1592,9 +1759,6 @@
     <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1631,6 +1795,22 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1652,6 +1832,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1154356</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>12699</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{719618EF-0FFD-3942-B8FE-2053D58DB334}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6805856" y="13030200"/>
+          <a:ext cx="3849443" cy="1765300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3893,6 +4122,201 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1764C7-EB3F-884D-A423-6A64CF5D743E}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="23">
+        <v>150</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="19">
+        <f>B2*B3</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="23">
+        <v>0.42</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="19">
+        <f>SQRT((B2*B3)*(1-B3))</f>
+        <v>6.044832503882966</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="C6" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7883183-3309-E141-80C9-0F546E3ED993}">
+  <dimension ref="A6:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="6" spans="1:4">
+      <c r="C6" s="27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="C7" s="26">
+        <f>SUM(C10:C17)</f>
+        <v>1.6335</v>
+      </c>
+      <c r="D7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="7">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0.1663</v>
+      </c>
+      <c r="C10">
+        <f>A10*B10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="7">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:C17" si="0">A11*B11</f>
+        <v>0.34200000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="7">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>0.27660000000000001</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0.55320000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>0.14960000000000001</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0.44880000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0.152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>2.75E-2</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0.13750000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD5251E-A9B7-7F4B-A78E-2F9C7E161BB7}">
   <dimension ref="A1:H57"/>
   <sheetViews>
@@ -4295,14 +4719,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5B9FCC-C544-FD4E-85A9-D1AE64548C87}">
-  <dimension ref="B3:G59"/>
+  <dimension ref="A3:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView topLeftCell="A35" zoomScale="58" workbookViewId="0">
+      <selection activeCell="O53" sqref="O53:Y78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" customWidth="1"/>
@@ -4310,43 +4735,43 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7">
-      <c r="B3" s="96">
+      <c r="B3" s="140">
         <v>10.199999999999999</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
+      <c r="F3" s="140"/>
+      <c r="G3" s="140"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="141" t="s">
         <v>236</v>
       </c>
-      <c r="C5" s="95"/>
-      <c r="F5" s="95" t="s">
+      <c r="C5" s="141"/>
+      <c r="F5" s="141" t="s">
         <v>237</v>
       </c>
-      <c r="G5" s="95"/>
+      <c r="G5" s="141"/>
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="76"/>
-      <c r="C6" s="97"/>
+      <c r="C6" s="94"/>
       <c r="F6" s="76"/>
-      <c r="G6" s="97"/>
+      <c r="G6" s="94"/>
     </row>
     <row r="7" spans="2:7">
       <c r="B7" s="84" t="s">
         <v>238</v>
       </c>
       <c r="C7" s="85">
-        <v>0.5</v>
+        <v>0.48</v>
       </c>
       <c r="F7" s="84" t="s">
         <v>238</v>
       </c>
       <c r="G7" s="85">
-        <v>0.53</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="8" spans="2:7">
@@ -4354,13 +4779,13 @@
         <v>197</v>
       </c>
       <c r="C8" s="79">
-        <v>1447</v>
+        <v>2000</v>
       </c>
       <c r="F8" s="86" t="s">
         <v>0</v>
       </c>
       <c r="G8" s="87">
-        <v>13</v>
+        <v>409</v>
       </c>
     </row>
     <row r="9" spans="2:7">
@@ -4368,27 +4793,27 @@
         <v>0</v>
       </c>
       <c r="C9" s="87">
-        <v>740</v>
-      </c>
-      <c r="F9" s="98" t="s">
+        <v>982</v>
+      </c>
+      <c r="F9" s="95" t="s">
         <v>197</v>
       </c>
-      <c r="G9" s="99">
-        <v>19</v>
+      <c r="G9" s="96">
+        <v>700</v>
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="100" t="s">
+      <c r="B10" s="97" t="s">
         <v>218</v>
       </c>
-      <c r="C10" s="101">
+      <c r="C10" s="98">
         <v>0.1</v>
       </c>
-      <c r="F10" s="100" t="s">
+      <c r="F10" s="97" t="s">
         <v>218</v>
       </c>
-      <c r="G10" s="101">
-        <v>2.5000000000000001E-2</v>
+      <c r="G10" s="98">
+        <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="2:7">
@@ -4401,8 +4826,8 @@
       <c r="F11" s="74" t="s">
         <v>239</v>
       </c>
-      <c r="G11" s="74" t="s">
-        <v>241</v>
+      <c r="G11" s="74">
+        <v>0.01</v>
       </c>
     </row>
     <row r="12" spans="2:7">
@@ -4412,35 +4837,35 @@
       <c r="G12" s="32"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="102" t="s">
-        <v>242</v>
-      </c>
-      <c r="C13" s="103">
+      <c r="B13" s="99" t="s">
+        <v>241</v>
+      </c>
+      <c r="C13" s="100">
         <f>C8*C7*(1-C7)</f>
-        <v>361.75</v>
-      </c>
-      <c r="F13" s="102" t="s">
-        <v>242</v>
-      </c>
-      <c r="G13" s="104">
+        <v>499.20000000000005</v>
+      </c>
+      <c r="F13" s="99" t="s">
+        <v>241</v>
+      </c>
+      <c r="G13" s="101">
         <f>G9*G7*(1-G7)</f>
-        <v>4.7328999999999999</v>
+        <v>170.52</v>
       </c>
     </row>
     <row r="14" spans="2:7">
       <c r="B14" s="82" t="s">
-        <v>243</v>
-      </c>
-      <c r="C14" s="105" t="b">
+        <v>242</v>
+      </c>
+      <c r="C14" s="102" t="b">
         <f>IF(C13&gt;=10, TRUE, FALSE)</f>
         <v>1</v>
       </c>
       <c r="F14" s="82" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G14" s="82" t="b">
         <f>IF(G13&gt;=10, TRUE, FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:7">
@@ -4450,383 +4875,427 @@
       <c r="G15" s="32"/>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="106" t="s">
-        <v>244</v>
-      </c>
-      <c r="C16" s="107">
+      <c r="B16" s="103" t="s">
+        <v>243</v>
+      </c>
+      <c r="C16" s="104">
         <f>C9/C8</f>
-        <v>0.51140290255701448</v>
+        <v>0.49099999999999999</v>
       </c>
       <c r="F16" s="74" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G16" s="32">
         <f>G8/G9</f>
-        <v>0.68421052631578949</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7">
+        <v>0.5842857142857143</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
       <c r="B17" s="40"/>
-      <c r="C17" s="108"/>
-      <c r="F17" s="109" t="s">
+      <c r="C17" s="105"/>
+      <c r="F17" s="106" t="s">
+        <v>244</v>
+      </c>
+      <c r="G17" s="107">
+        <f>(G16-G7)/SQRT((G7*(1-G7))/G9)</f>
+        <v>0.22973840032238738</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="B18" s="106" t="s">
+        <v>244</v>
+      </c>
+      <c r="C18" s="108">
+        <f>(C16-C7)/SQRT((C7*(1-C7))/C8)</f>
+        <v>0.98465795180422111</v>
+      </c>
+      <c r="D18" t="s">
         <v>245</v>
-      </c>
-      <c r="G17" s="110">
-        <f>(G16-G7)/SQRT((G7*(1-G7))/G9)</f>
-        <v>1.3468026309736418</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="109" t="s">
-        <v>245</v>
-      </c>
-      <c r="C18" s="111">
-        <f>(C16-C7)/SQRT((C7*(1-C7))/C8)</f>
-        <v>0.86752035639687086</v>
-      </c>
-      <c r="D18" t="s">
-        <v>246</v>
       </c>
       <c r="F18" s="74"/>
       <c r="G18" s="32"/>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:12">
       <c r="B19" s="74"/>
       <c r="C19" s="32"/>
-      <c r="F19" s="112" t="s">
+      <c r="F19" s="109" t="s">
+        <v>246</v>
+      </c>
+      <c r="G19" s="110">
+        <f>TDIST(ABS(G17),G9-1,2)</f>
+        <v>0.81836226346609831</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12">
+      <c r="B20" s="109" t="s">
+        <v>246</v>
+      </c>
+      <c r="C20" s="111">
+        <f>TDIST(ABS(C18),C8-1,1)</f>
+        <v>0.16245563671949209</v>
+      </c>
+      <c r="F20" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="G19" s="113">
-        <f>TDIST(ABS(G17),G9-1,2)</f>
-        <v>0.19475749775710713</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="112" t="s">
-        <v>247</v>
-      </c>
-      <c r="C20" s="114">
-        <f>TDIST(ABS(C18),C8-1,1)</f>
-        <v>0.1929004515737997</v>
-      </c>
-      <c r="F20" s="115" t="s">
-        <v>248</v>
-      </c>
-      <c r="G20" s="116" t="str">
+      <c r="G20" s="113" t="str">
         <f>IF(G19&gt;G10, "P &gt; a", "P &lt; a")</f>
         <v>P &gt; a</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="115" t="s">
-        <v>248</v>
-      </c>
-      <c r="C21" s="116" t="str">
+    <row r="21" spans="2:12">
+      <c r="B21" s="112" t="s">
+        <v>247</v>
+      </c>
+      <c r="C21" s="113" t="str">
         <f>IF(C20&gt;C10, "P &gt; a", "P &lt; a")</f>
         <v>P &gt; a</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="95" t="s">
+    <row r="22" spans="2:12">
+      <c r="D22" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="B24" s="141" t="s">
+        <v>248</v>
+      </c>
+      <c r="C24" s="141"/>
+      <c r="F24" s="142" t="s">
         <v>249</v>
       </c>
-      <c r="C24" s="95"/>
-      <c r="F24" s="117" t="s">
-        <v>250</v>
-      </c>
-      <c r="G24" s="117"/>
-    </row>
-    <row r="25" spans="2:7">
+      <c r="G24" s="142"/>
+    </row>
+    <row r="25" spans="2:12">
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
       <c r="F25" s="32"/>
       <c r="G25" s="32"/>
-    </row>
-    <row r="26" spans="2:7">
+      <c r="K25" s="98" t="s">
+        <v>260</v>
+      </c>
+      <c r="L25" s="98">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12">
       <c r="B26" s="85" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="85">
-        <v>26</v>
-      </c>
-      <c r="F26" s="118" t="s">
-        <v>0</v>
-      </c>
-      <c r="G26" s="119">
+        <v>494</v>
+      </c>
+      <c r="F26" s="114" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="115">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="B27" s="120" t="s">
+      <c r="K26" s="98" t="s">
+        <v>261</v>
+      </c>
+      <c r="L26" s="98">
+        <v>105.2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12">
+      <c r="B27" s="116" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="120">
-        <v>50</v>
-      </c>
-      <c r="F27" s="118" t="s">
+      <c r="C27" s="116">
+        <v>1195</v>
+      </c>
+      <c r="F27" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="G27" s="119">
+      <c r="G27" s="115">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="2:7">
+      <c r="K27" s="98" t="s">
+        <v>262</v>
+      </c>
+      <c r="L27">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12">
       <c r="B28" s="79" t="s">
+        <v>250</v>
+      </c>
+      <c r="C28" s="79">
+        <v>0.4</v>
+      </c>
+      <c r="F28" s="114" t="s">
         <v>251</v>
       </c>
-      <c r="C28" s="79">
-        <v>0.5</v>
-      </c>
-      <c r="F28" s="118" t="s">
+      <c r="G28" s="115">
+        <v>57</v>
+      </c>
+      <c r="K28" s="98" t="s">
+        <v>20</v>
+      </c>
+      <c r="L28" s="98">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12">
+      <c r="B29" s="117" t="s">
+        <v>274</v>
+      </c>
+      <c r="C29" s="117">
+        <v>99</v>
+      </c>
+      <c r="F29" s="114" t="s">
         <v>252</v>
       </c>
-      <c r="G28" s="119">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="B29" s="121" t="s">
-        <v>198</v>
-      </c>
-      <c r="C29" s="121">
-        <v>0.3886</v>
-      </c>
-      <c r="F29" s="118" t="s">
-        <v>253</v>
-      </c>
-      <c r="G29" s="119">
+      <c r="G29" s="115">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="2:7">
+      <c r="K29" s="98" t="s">
+        <v>218</v>
+      </c>
+      <c r="L29" s="98">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12">
       <c r="B30" s="40"/>
-      <c r="C30" s="108"/>
-      <c r="F30" s="122"/>
-      <c r="G30" s="123"/>
-    </row>
-    <row r="31" spans="2:7">
+      <c r="C30" s="105"/>
+      <c r="F30" s="118"/>
+      <c r="G30" s="119"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+    </row>
+    <row r="31" spans="2:12">
       <c r="B31" s="32" t="s">
         <v>196</v>
       </c>
       <c r="C31" s="32">
         <f>C27*(C28/100)*(1-(C28/100))</f>
-        <v>0.24875</v>
-      </c>
-      <c r="F31" s="124" t="s">
-        <v>254</v>
-      </c>
-      <c r="G31" s="125">
+        <v>4.7608800000000002</v>
+      </c>
+      <c r="F31" s="120" t="s">
+        <v>253</v>
+      </c>
+      <c r="G31" s="121">
         <f>G27*(G28/100)*(1-(G28/100))</f>
         <v>11.764800000000001</v>
       </c>
-    </row>
-    <row r="32" spans="2:7">
+      <c r="K31" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="L31" s="134" t="str">
+        <f>IF(L28&gt;=30, "Yes", "No")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12">
       <c r="B32" s="32"/>
-      <c r="C32" s="126"/>
-      <c r="F32" s="127" t="s">
+      <c r="C32" s="122"/>
+      <c r="F32" s="123" t="s">
         <v>196</v>
       </c>
-      <c r="G32" s="127" t="e" cm="1">
-        <f t="array" ref="G32">IF(G31 &gt;= 10, TURE, FALSE)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7">
+      <c r="G32" s="123" t="b">
+        <f>IF(G31 &gt;= 10, TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+    </row>
+    <row r="33" spans="2:12">
       <c r="B33" s="32" t="s">
         <v>200</v>
       </c>
       <c r="C33" s="32">
         <f>((100-C29) /2)/100</f>
-        <v>0.49805700000000003</v>
-      </c>
-      <c r="F33" s="128"/>
-      <c r="G33" s="97"/>
-    </row>
-    <row r="34" spans="2:7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F33" s="124"/>
+      <c r="G33" s="94"/>
+      <c r="K33" s="135" t="s">
+        <v>264</v>
+      </c>
+      <c r="L33" s="135">
+        <f>(L26-L25)/ (L27/SQRT(L28))</f>
+        <v>1.5086095259518884</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12">
       <c r="B34" s="32" t="s">
         <v>201</v>
       </c>
       <c r="C34" s="32">
         <f>_xlfn.NORM.INV((1-C33),0,1)</f>
-        <v>4.87039799247672E-3</v>
+        <v>2.5758293035488999</v>
       </c>
       <c r="F34" s="74" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G34" s="32">
         <f>G26/G27</f>
         <v>0.27083333333333331</v>
       </c>
-    </row>
-    <row r="35" spans="2:7">
-      <c r="B35" s="122"/>
-      <c r="C35" s="123"/>
+      <c r="K34" s="136" t="s">
+        <v>265</v>
+      </c>
+      <c r="L34" s="131">
+        <f>TDIST(ABS(L33),L28-1,1)</f>
+        <v>6.9728940266272882E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12">
+      <c r="B35" s="118"/>
+      <c r="C35" s="119"/>
       <c r="F35" s="74" t="s">
+        <v>254</v>
+      </c>
+      <c r="G35" s="32"/>
+    </row>
+    <row r="36" spans="2:12">
+      <c r="B36" s="125" t="s">
         <v>255</v>
       </c>
-      <c r="G35" s="32"/>
-    </row>
-    <row r="36" spans="2:7">
-      <c r="B36" s="129" t="s">
+      <c r="C36" s="125">
+        <f>C26/C27</f>
+        <v>0.41338912133891215</v>
+      </c>
+      <c r="F36" s="74"/>
+      <c r="G36" s="126"/>
+      <c r="K36" s="137" t="s">
+        <v>266</v>
+      </c>
+      <c r="L36" s="134" t="str">
+        <f>IF(L34&gt;L29, "Do not reject", "Reject")</f>
+        <v>Reject</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12">
+      <c r="B37" s="127"/>
+      <c r="C37" s="128"/>
+      <c r="F37" s="74" t="s">
         <v>256</v>
       </c>
-      <c r="C36" s="129">
-        <f>C26/C27</f>
-        <v>0.52</v>
-      </c>
-      <c r="F36" s="74"/>
-      <c r="G36" s="130"/>
-    </row>
-    <row r="37" spans="2:7">
-      <c r="B37" s="131"/>
-      <c r="C37" s="132"/>
-      <c r="F37" s="74" t="s">
-        <v>257</v>
-      </c>
-      <c r="G37" s="130">
+      <c r="G37" s="126">
         <f>_xlfn.BINOM.DIST(G29-1,G27,G28/100,TRUE)</f>
         <v>0.99964533162387259</v>
       </c>
     </row>
-    <row r="38" spans="2:7">
-      <c r="B38" s="105" t="s">
+    <row r="38" spans="2:12">
+      <c r="B38" s="102" t="s">
         <v>202</v>
       </c>
-      <c r="C38" s="133">
+      <c r="C38" s="129">
         <f>C36-(C34*SQRT((C36*(1-C36))/C27))</f>
-        <v>0.51965588647685279</v>
-      </c>
-      <c r="F38" s="134" t="s">
-        <v>258</v>
-      </c>
-      <c r="G38" s="135">
+        <v>0.37669574247190074</v>
+      </c>
+      <c r="F38" s="130" t="s">
+        <v>257</v>
+      </c>
+      <c r="G38" s="131">
         <f>1-G37</f>
         <v>3.5466837612740942E-4</v>
       </c>
     </row>
-    <row r="39" spans="2:7">
-      <c r="B39" s="105" t="s">
+    <row r="39" spans="2:12">
+      <c r="B39" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="133">
+      <c r="C39" s="129">
         <f>C36+(C34*SQRT((C36*(1-C36))/C27))</f>
-        <v>0.52034411352314724</v>
+        <v>0.45008250020592355</v>
       </c>
       <c r="D39" t="s">
+        <v>258</v>
+      </c>
+      <c r="F39" s="132" t="s">
         <v>259</v>
       </c>
-      <c r="F39" s="136" t="s">
-        <v>260</v>
-      </c>
-      <c r="G39" s="137">
+      <c r="G39" s="133">
         <f>_xlfn.BINOM.DIST(G29,G27,G28/100,TRUE)</f>
         <v>0.99989936814098268</v>
       </c>
     </row>
-    <row r="44" spans="2:7">
-      <c r="B44" s="96">
-        <v>10.3</v>
-      </c>
-      <c r="C44" s="96"/>
-      <c r="D44" s="96"/>
-      <c r="E44" s="96"/>
-      <c r="F44" s="96"/>
-      <c r="G44" s="96"/>
-    </row>
-    <row r="48" spans="2:7">
-      <c r="B48" s="101" t="s">
-        <v>261</v>
-      </c>
-      <c r="C48" s="101">
-        <v>1.68</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3">
-      <c r="B49" s="101" t="s">
-        <v>262</v>
-      </c>
-      <c r="C49" s="101">
-        <v>1.681</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3">
-      <c r="B50" s="101" t="s">
-        <v>263</v>
-      </c>
-      <c r="C50">
-        <v>4.8053000000000002E-3</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3">
-      <c r="B51" s="101" t="s">
-        <v>20</v>
-      </c>
-      <c r="C51" s="101">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3">
-      <c r="B52" s="101" t="s">
-        <v>218</v>
-      </c>
-      <c r="C52" s="101">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3">
-      <c r="B53" s="32"/>
-      <c r="C53" s="32"/>
-    </row>
-    <row r="54" spans="2:3">
-      <c r="B54" s="31" t="s">
-        <v>264</v>
-      </c>
-      <c r="C54" s="138" t="str">
-        <f>IF(C51&gt;=30, "Yes", "No")</f>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3">
-      <c r="B55" s="32"/>
-      <c r="C55" s="32"/>
-    </row>
-    <row r="56" spans="2:3">
-      <c r="B56" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="C56" s="139">
-        <f>(C49-C48)/ (C50/SQRT(C51))</f>
-        <v>0.72089185173415637</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3">
-      <c r="B57" s="140" t="s">
-        <v>266</v>
-      </c>
-      <c r="C57" s="135">
-        <f>TDIST(ABS(C56),C51-1,1)</f>
-        <v>0.24300745710152599</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3">
-      <c r="B59" s="141" t="s">
+    <row r="45" spans="2:12">
+      <c r="B45" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12">
+      <c r="B47" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12">
+      <c r="B48" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="B49" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="B50" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="29">
+      <c r="A52" t="s">
+        <v>272</v>
+      </c>
+      <c r="B52" s="138" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="29">
+      <c r="B53" s="138" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="21">
+      <c r="B55" s="139"/>
+    </row>
+    <row r="61" spans="1:2" ht="17">
+      <c r="B61" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="C59" s="138" t="str">
-        <f>IF(C57&gt;C52, "Do not reject", "Reject")</f>
-        <v>Do not reject</v>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="B62" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" ht="17">
+      <c r="B69" s="15" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="F24:G24"/>
-    <mergeCell ref="B44:G44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5577,18 +6046,18 @@
       <c r="K2" s="60"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="143" t="s">
         <v>190</v>
       </c>
-      <c r="C3" s="94"/>
+      <c r="C3" s="143"/>
       <c r="D3" s="60"/>
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="94" t="s">
+      <c r="H3" s="143" t="s">
         <v>191</v>
       </c>
-      <c r="I3" s="94"/>
+      <c r="I3" s="143"/>
       <c r="J3" s="60"/>
       <c r="K3" s="60"/>
     </row>
@@ -5809,10 +6278,10 @@
       <c r="K13" s="60"/>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" s="94" t="s">
+      <c r="B14" s="143" t="s">
         <v>203</v>
       </c>
-      <c r="C14" s="94"/>
+      <c r="C14" s="143"/>
       <c r="D14" s="60"/>
       <c r="E14" s="60"/>
       <c r="F14" s="60"/>
@@ -5830,10 +6299,10 @@
         <v>0.05</v>
       </c>
       <c r="D15" s="60"/>
-      <c r="E15" s="94" t="s">
+      <c r="E15" s="143" t="s">
         <v>205</v>
       </c>
-      <c r="F15" s="94"/>
+      <c r="F15" s="143"/>
       <c r="G15" s="66"/>
       <c r="H15" s="66"/>
       <c r="I15" s="66"/>
@@ -5997,19 +6466,19 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:10">
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="141" t="s">
         <v>215</v>
       </c>
-      <c r="C4" s="95"/>
-      <c r="E4" s="95" t="s">
+      <c r="C4" s="141"/>
+      <c r="E4" s="141" t="s">
         <v>216</v>
       </c>
-      <c r="F4" s="95"/>
-      <c r="H4" s="95" t="s">
+      <c r="F4" s="141"/>
+      <c r="H4" s="141" t="s">
         <v>217</v>
       </c>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
+      <c r="I4" s="141"/>
+      <c r="J4" s="141"/>
     </row>
     <row r="5" spans="2:10">
       <c r="B5" s="76"/>
@@ -6189,10 +6658,10 @@
       </c>
     </row>
     <row r="17" spans="2:9">
-      <c r="B17" s="95" t="s">
+      <c r="B17" s="141" t="s">
         <v>230</v>
       </c>
-      <c r="C17" s="95"/>
+      <c r="C17" s="141"/>
       <c r="H17" s="32" t="s">
         <v>231</v>
       </c>
@@ -6308,10 +6777,521 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74898097-6201-8D4A-AA45-F89B2A2E7762}">
+  <dimension ref="A2:F27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7">
+        <v>30120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>293</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7">
+        <v>30415</v>
+      </c>
+      <c r="C4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D4">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7">
+        <v>30729</v>
+      </c>
+      <c r="C5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7">
+        <v>32114</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E6" t="s">
+        <v>289</v>
+      </c>
+      <c r="F6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="7">
+        <v>33093</v>
+      </c>
+      <c r="C7">
+        <f>D$5 + D$4*0</f>
+        <v>30000</v>
+      </c>
+      <c r="D7">
+        <f>D$5 + ((D$4 * 1) -1)</f>
+        <v>35999</v>
+      </c>
+      <c r="E7">
+        <f>COUNTIFS(A$3:A$200,"&gt;30000", A$3:A$200,"&lt;35999")</f>
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <f>E7/F14</f>
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="7">
+        <v>33713</v>
+      </c>
+      <c r="C8">
+        <f>D$5 + D$4*1</f>
+        <v>36000</v>
+      </c>
+      <c r="D8">
+        <f>D$5 + ((D$4 * 2) -1)</f>
+        <v>41999</v>
+      </c>
+      <c r="E8">
+        <f>COUNTIFS(A$3:A$200,"&gt;36000", A$3:A$200,"&lt;41999")</f>
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <f>10/F14</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="7">
+        <v>33915</v>
+      </c>
+      <c r="C9">
+        <f>D$5 + D$4*2</f>
+        <v>42000</v>
+      </c>
+      <c r="D9">
+        <f>D$5 + ((D$4 * 3) -1)</f>
+        <v>47999</v>
+      </c>
+      <c r="E9">
+        <f>COUNTIFS(A$3:A$200,"&gt;30000", A$3:A$200,"&lt;35999")</f>
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <f>1/F14</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="7">
+        <v>34184</v>
+      </c>
+      <c r="C10">
+        <f>D$5 + D$4*3</f>
+        <v>48000</v>
+      </c>
+      <c r="D10">
+        <f>D$5 + ((D$4 * 4) -1)</f>
+        <v>53999</v>
+      </c>
+      <c r="E10">
+        <f>COUNTIFS(A$3:A$200,"&gt;30000", A$3:A$200,"&lt;35999")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="7">
+        <v>34676</v>
+      </c>
+      <c r="D11" s="145" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="7">
+        <v>34837</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="7">
+        <v>35214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="7">
+        <v>35576</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="F14">
+        <f>COUNT(A3:A27)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="7">
+        <v>35755</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="7">
+        <v>35976</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="7">
+        <v>36817</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="7">
+        <v>37298</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="7">
+        <v>37764</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="7">
+        <v>38441</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="7">
+        <v>38692</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="7">
+        <v>38878</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="7">
+        <v>39879</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="7">
+        <v>40141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="7">
+        <v>41175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="7">
+        <v>41420</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="7">
+        <v>52591</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A47A757-16BD-0749-9653-C8284C431BBD}">
+  <dimension ref="A2:D42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>0.26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D3">
+        <f>COUNT(A3:A202)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>0.47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4">
+        <f>AVERAGE(A3:A200)</f>
+        <v>5.6750000000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>-0.05</v>
+      </c>
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5">
+        <f>STDEV(A3:A220)</f>
+        <v>0.11958019517011616</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>0.01</v>
+      </c>
+      <c r="C7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="5">
+        <f>QUARTILE(A$3:A$22, 1)</f>
+        <v>-1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>0.26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>283</v>
+      </c>
+      <c r="D8">
+        <f>QUARTILE(A$3:A$22, 2)</f>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>0.06</v>
+      </c>
+      <c r="C9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="144">
+        <f>QUARTILE(A$3:A$22, 3)</f>
+        <v>0.10250000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>-0.15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>-0.11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42">
+        <v>0.03</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFCA351-70B0-5244-BA65-285CF6942DC3}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6610,7 +7590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74F7077-45B6-E742-951B-BF30C929E163}">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -6751,199 +7731,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1764C7-EB3F-884D-A423-6A64CF5D743E}">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="23">
-        <v>150</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="19">
-        <f>B2*B3</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="23">
-        <v>0.42</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="19">
-        <f>SQRT((B2*B3)*(1-B3))</f>
-        <v>6.044832503882966</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="C6" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7883183-3309-E141-80C9-0F546E3ED993}">
-  <dimension ref="A6:D17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="6" spans="1:4">
-      <c r="C6" s="27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="C7" s="26">
-        <f>SUM(C10:C17)</f>
-        <v>1.6335</v>
-      </c>
-      <c r="D7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="7">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>0.1663</v>
-      </c>
-      <c r="C10">
-        <f>A10*B10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="7">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>0.34200000000000003</v>
-      </c>
-      <c r="C11">
-        <f t="shared" ref="C11:C17" si="0">A11*B11</f>
-        <v>0.34200000000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="7">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>0.27660000000000001</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>0.55320000000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>0.14960000000000001</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>0.44880000000000003</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>0.152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <v>5</v>
-      </c>
-      <c r="B15">
-        <v>2.75E-2</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>0.13750000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3">
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add final formulas and notes
</commit_message>
<xml_diff>
--- a/Midterm Excel Sheet.xlsx
+++ b/Midterm Excel Sheet.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanninoa/Desktop/updated stats/clean/Statistics-Sheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanninoa/Desktop/wednesday/Statistics-Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36C0BE3-E04B-FA4E-A3A4-FA588BED62EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504B0DF5-DD22-F843-8072-C13957891763}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1080" windowWidth="15640" windowHeight="18740" activeTab="7" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
+    <workbookView xWindow="20300" yWindow="460" windowWidth="12920" windowHeight="18740" activeTab="1" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
   </bookViews>
   <sheets>
     <sheet name="Random Variable x" sheetId="1" r:id="rId1"/>
     <sheet name="Chpater 10" sheetId="11" r:id="rId2"/>
-    <sheet name="Normal Distribution" sheetId="6" r:id="rId3"/>
+    <sheet name="Normal Distribution - Z-score" sheetId="6" r:id="rId3"/>
     <sheet name="Chapter 9" sheetId="9" r:id="rId4"/>
     <sheet name="t-values" sheetId="10" r:id="rId5"/>
     <sheet name="Histogram" sheetId="13" r:id="rId6"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="367">
   <si>
     <t>x</t>
   </si>
@@ -289,12 +289,6 @@
     <t>If the z-score is positive, add .5 to the table value</t>
   </si>
   <si>
-    <t>Negative Z</t>
-  </si>
-  <si>
-    <t>positive Z</t>
-  </si>
-  <si>
     <t>Result</t>
   </si>
   <si>
@@ -376,12 +370,6 @@
     <t>Fewer than X</t>
   </si>
   <si>
-    <t>Negative Z-score</t>
-  </si>
-  <si>
-    <t>Positive Z-score</t>
-  </si>
-  <si>
     <t>Middle X%</t>
   </si>
   <si>
@@ -505,9 +493,6 @@
     <t>Q3</t>
   </si>
   <si>
-    <t>Determine the # of items that make up the middle % (Make sure to change percentile)</t>
-  </si>
-  <si>
     <t>Time Requred, mean, SD, x</t>
   </si>
   <si>
@@ -520,9 +505,6 @@
     <t>​for later: (b) If the automotive center does not want to give the discount to more than 55% of its​ customers, how long should it make the guaranteed time​ limit?</t>
   </si>
   <si>
-    <t>Calculate Z-score</t>
-  </si>
-  <si>
     <t>Score A</t>
   </si>
   <si>
@@ -562,9 +544,6 @@
     <t>sample size (n)</t>
   </si>
   <si>
-    <t>Current i val</t>
-  </si>
-  <si>
     <t>z-score for I (using normal SD)</t>
   </si>
   <si>
@@ -754,12 +733,6 @@
     <t>(round up to one more value ex: 48 then should be 49)</t>
   </si>
   <si>
-    <t>Population Proportion (Left-Tailed Test)</t>
-  </si>
-  <si>
-    <t>Population Proportion (Two-Tailed Test)</t>
-  </si>
-  <si>
     <t>p-zero %</t>
   </si>
   <si>
@@ -836,9 +809,6 @@
   </si>
   <si>
     <t>Is (n &gt;= 30)?</t>
-  </si>
-  <si>
-    <t>t-zero</t>
   </si>
   <si>
     <t xml:space="preserve">P-value </t>
@@ -1017,12 +987,299 @@
   <si>
     <t>How many classes?</t>
   </si>
+  <si>
+    <t>Of the monthly​ returns, 25% are less than or equal to the first​ quartile, 50% are less than or equal to the second​ quartile, and​ 75% are less than or equal to the third quartile.</t>
+  </si>
+  <si>
+    <t>IQR = Q3 - Q1</t>
+  </si>
+  <si>
+    <t>in R:</t>
+  </si>
+  <si>
+    <t>Lower fence = Q1 − ​1.5(IQR)</t>
+  </si>
+  <si>
+    <t>Upper fence = Q3 + 1.5(IQR)</t>
+  </si>
+  <si>
+    <t>for IQR - use IQR(x) func in R</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Pulse</t>
+  </si>
+  <si>
+    <t>Student 1</t>
+  </si>
+  <si>
+    <t>Student 2</t>
+  </si>
+  <si>
+    <t>Student 3</t>
+  </si>
+  <si>
+    <t>Student 4</t>
+  </si>
+  <si>
+    <t>Student 5</t>
+  </si>
+  <si>
+    <t>Student 6</t>
+  </si>
+  <si>
+    <t>Student 7</t>
+  </si>
+  <si>
+    <t>Student 8</t>
+  </si>
+  <si>
+    <t>Student 9</t>
+  </si>
+  <si>
+    <t>The interquartile range is preferred when the data are skewed or have outliers. An advantage of the standard deviation is that it uses all the observations in its computation.</t>
+  </si>
+  <si>
+    <t>Height distributions for men and women have different centers and​ spreads, making it difficult to compare male and female heights directly.</t>
+  </si>
+  <si>
+    <t>z-score mean</t>
+  </si>
+  <si>
+    <t>sample SD</t>
+  </si>
+  <si>
+    <t>population SD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes: </t>
+  </si>
+  <si>
+    <t>The area under normal curve is 1/2 (0.5)</t>
+  </si>
+  <si>
+    <t>Must be bell-shaped to be normal distribution</t>
+  </si>
+  <si>
+    <t>σ - Population Standard deviation</t>
+  </si>
+  <si>
+    <t> μ - population mean</t>
+  </si>
+  <si>
+    <t> μ bar - sample mean</t>
+  </si>
+  <si>
+    <t>s - sample standard deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inflection points - Q1 and Q3 </t>
+  </si>
+  <si>
+    <t>Normal density function -  the histogram shape resembles a normal​ curve, and the area of each bar is roughly equal to the area under the normal curve for the same region</t>
+  </si>
+  <si>
+    <t>As the mean increases, the graph of the normal curve slides right.</t>
+  </si>
+  <si>
+    <t>As the standard deviation decreases, The graph of the normal curve compresses and becomes steeper.</t>
+  </si>
+  <si>
+    <t>The normal curve is symmetric about its​ mean μ. The normal curve is a symmetric distribution with one​ peak, which means the​ mean, median, and mode are all equal.​ Therefore, the normal curve is symmetric about the​ mean, mu.</t>
+  </si>
+  <si>
+    <t>Left Z</t>
+  </si>
+  <si>
+    <t>Right Z</t>
+  </si>
+  <si>
+    <t>Left Z-score</t>
+  </si>
+  <si>
+    <t>Right Z-score</t>
+  </si>
+  <si>
+    <t>Left is negative</t>
+  </si>
+  <si>
+    <t>right is positive</t>
+  </si>
+  <si>
+    <r>
+      <t>Determine the # of items that make up the middle % (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Make sure to change percentile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Calculate Z-score for 2 different scores</t>
+  </si>
+  <si>
+    <t>Sampling Distribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">μ ofx bar​ </t>
+  </si>
+  <si>
+    <t>σ of x bar</t>
+  </si>
+  <si>
+    <t>samle size</t>
+  </si>
+  <si>
+    <t>The distribution of the sample mean is normally distributed when the random variable X is normally​ distributed, or when the sample size is large​ (at least​ 30).</t>
+  </si>
+  <si>
+    <t>Notice that in this case the distribution of the sample mean is normal and the sample size is small. The sampling distribution of the mean is only normal when the population is normal or the sample size is large.</t>
+  </si>
+  <si>
+    <t>​Thus, the shape of the population must be approximately normal because the sample size is not large.</t>
+  </si>
+  <si>
+    <t>CHECK: A simple random sample of size nequals81 is obtained from a population that is skewed right with mu equals 89 and sigma equals 9.
+​(a) Describe the sampling distribution of x overbar.
+​(b) What is Upper P left parenthesis x overbar greater than 90.15 right parenthesis​?
+​(c) What is Upper P left parenthesis x overbar less than or equals 86.9 right parenthesis​?
+​(d) What is Upper P left parenthesis 87.75 less than x overbar less than 90.65 right parenthesis​?</t>
+  </si>
+  <si>
+    <t>Current val (x &lt;&gt; value)</t>
+  </si>
+  <si>
+    <t>SD bar = SD / SQRT(n)</t>
+  </si>
+  <si>
+    <t>Suppose the lengths of the pregnancies of a certain animal are approximately normally distributed with mean μ=123 days and standard deviation sigma = 11 days.</t>
+  </si>
+  <si>
+    <t>mean of x bar</t>
+  </si>
+  <si>
+    <t>SD of x bar</t>
+  </si>
+  <si>
+    <t>Find the Point Estimate</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Point estimate (mean)</t>
+  </si>
+  <si>
+    <t>in mound shaped histogram, median = mean</t>
+  </si>
+  <si>
+    <t>rght skewed, mean &gt; median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left skewed, mean &lt; median </t>
+  </si>
+  <si>
+    <t>mean is sensitive to large numbers. Median always stays in center of distribution (more robust)</t>
+  </si>
+  <si>
+    <t>binomial variables are discrete</t>
+  </si>
+  <si>
+    <t>Decision Based on P-value: We will reject the null hypothesis at α level of significance if the P-value ≤ αOtherwise, we do not reject the null hypothesis.</t>
+  </si>
+  <si>
+    <t>p-cap (Test statistic value)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x </t>
+  </si>
+  <si>
+    <t>n (sample size)</t>
+  </si>
+  <si>
+    <t>Margin of Error  +/-</t>
+  </si>
+  <si>
+    <t>Guaranteed Time limit is</t>
+  </si>
+  <si>
+    <t>Population proportoin ( two tailed with multiple sample values)</t>
+  </si>
+  <si>
+    <t>mean (x bar)</t>
+  </si>
+  <si>
+    <r>
+      <t>𝜇</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <t>Test Statistic</t>
+  </si>
+  <si>
+    <t>^^ sample deviates _ SD below the mean from what is expected under the null hypothesis</t>
+  </si>
+  <si>
+    <t>Explain the difference between statistical significance and practical significance.</t>
+  </si>
+  <si>
+    <t>Ans: Statistical significance means that the sample statistic is not likely to come from the population whose parameter is stated in the null hypothesis. Practical significance refers to whether the difference between the sample statistic and the parameter stated in the null hypothesis is large enough to be considered important in an application.</t>
+  </si>
+  <si>
+    <t>t-zero (test statistic)</t>
+  </si>
+  <si>
+    <t>Not statistically significantly higher if &gt;= 0.05</t>
+  </si>
+  <si>
+    <t>impact of large samples on the p-value? As n​ increases, the likelihood of rejecting the null hypothesis increases.​ However, large samples tend to overemphasize practically insignificant differences.</t>
+  </si>
+  <si>
+    <t>do not reject if x falls within the bounds</t>
+  </si>
+  <si>
+    <t>simple random samle has to be &lt; 30 to be normally distributed</t>
+  </si>
+  <si>
+    <t>Population Proportion (Two-Tailed Test) !=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population Proportion (Left/Right-Tailed Test) &lt; or &gt; </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.000000000000000000000_);_(* \(#,##0.000000000000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1032,8 +1289,9 @@
     <numFmt numFmtId="169" formatCode="0.000"/>
     <numFmt numFmtId="170" formatCode="0.0"/>
     <numFmt numFmtId="171" formatCode="0.00000"/>
+    <numFmt numFmtId="176" formatCode="0.000000000000000"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="38">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1261,6 +1519,36 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="21"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -1520,7 +1808,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1797,20 +2085,45 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1838,16 +2151,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1154356</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1482804</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>47297</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>12699</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1540637</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>15329</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1870,8 +2183,167 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6805856" y="13030200"/>
-          <a:ext cx="3849443" cy="1765300"/>
+          <a:off x="10044356" y="10097814"/>
+          <a:ext cx="3850757" cy="1763549"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>20158</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>120952</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>120145</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>96422</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FFE3DFA-FF56-434E-8E82-AFAA916E9568}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17054285" y="4152698"/>
+          <a:ext cx="10058400" cy="1588168"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>656167</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>148167</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>694267</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>88901</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D7C5035-54FC-D34D-B45B-E2DBC3E12647}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="656167" y="9313334"/>
+          <a:ext cx="10219267" cy="5232400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DA75547-2610-FD49-A714-D42544222539}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="50800" y="5994400"/>
+          <a:ext cx="5080000" cy="1866900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2182,8 +2654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E068083-BD50-CB42-8AAE-F1525497B3A5}">
   <dimension ref="A1:AN226"/>
   <sheetViews>
-    <sheetView zoomScale="131" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="AL1" zoomScale="75" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4126,7 +4598,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4201,7 +4673,7 @@
   <sheetData>
     <row r="6" spans="1:4">
       <c r="C6" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4210,7 +4682,7 @@
         <v>1.6335</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4224,7 +4696,7 @@
         <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4320,7 +4792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD5251E-A9B7-7F4B-A78E-2F9C7E161BB7}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="85" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
@@ -4348,10 +4820,10 @@
     </row>
     <row r="5" spans="1:8" ht="17">
       <c r="A5" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17">
@@ -4362,7 +4834,7 @@
         <v>0.12</v>
       </c>
       <c r="G6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H6">
         <v>0.12</v>
@@ -4371,7 +4843,7 @@
     <row r="7" spans="1:8">
       <c r="B7" s="2"/>
       <c r="G7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H7">
         <v>14</v>
@@ -4385,7 +4857,7 @@
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H8">
         <f>H6*H7</f>
@@ -4408,7 +4880,7 @@
         <v>1.68</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D10">
         <f>B6*B8</f>
@@ -4427,36 +4899,36 @@
       </c>
       <c r="B11" s="2"/>
       <c r="G11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="17">
       <c r="A12" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B12" s="29">
         <f>_xlfn.POISSON.DIST(B9,B10, FALSE)</f>
         <v>5.8198054157415332E-3</v>
       </c>
       <c r="G12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="17">
       <c r="A13" s="21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B13" s="29">
         <f>_xlfn.POISSON.DIST(B9 - 1, B10, TRUE)</f>
         <v>0.99242454151988369</v>
       </c>
       <c r="G13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17">
       <c r="A14" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B14" s="29">
         <f>1 - B13</f>
@@ -4465,7 +4937,7 @@
     </row>
     <row r="16" spans="1:8" ht="17">
       <c r="A16" s="21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -4473,7 +4945,7 @@
     </row>
     <row r="17" spans="1:3" ht="17">
       <c r="A17" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B17">
         <v>7</v>
@@ -4481,7 +4953,7 @@
     </row>
     <row r="18" spans="1:3" ht="17">
       <c r="A18" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -4598,7 +5070,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B27" s="20">
         <f>SUMIF(C19:C26,"",B19:B26)</f>
@@ -4607,12 +5079,12 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B40">
         <v>37</v>
@@ -4620,7 +5092,7 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B41">
         <v>106</v>
@@ -4637,12 +5109,12 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B47" s="20">
         <v>0.8</v>
@@ -4650,7 +5122,7 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B48" s="20">
         <v>9</v>
@@ -4658,7 +5130,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B49">
         <f>B47*B48</f>
@@ -4675,7 +5147,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B52">
         <f>_xlfn.POISSON.DIST(B51, B49, FALSE)</f>
@@ -4684,7 +5156,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B53">
         <f>_xlfn.POISSON.DIST(B51 - 1, B49, TRUE)</f>
@@ -4693,7 +5165,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B54">
         <f xml:space="preserve"> 1 - B53</f>
@@ -4719,484 +5191,603 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5B9FCC-C544-FD4E-85A9-D1AE64548C87}">
-  <dimension ref="A3:L69"/>
+  <dimension ref="A3:V75"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="58" workbookViewId="0">
-      <selection activeCell="O53" sqref="O53:Y78"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="63" workbookViewId="0">
+      <selection activeCell="U36" sqref="U36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="10" max="10" width="27.83203125" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" customWidth="1"/>
+    <col min="20" max="20" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7">
-      <c r="B3" s="140">
+    <row r="3" spans="2:22">
+      <c r="B3" s="143">
         <v>10.199999999999999</v>
       </c>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
-    </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="141" t="s">
-        <v>236</v>
-      </c>
-      <c r="C5" s="141"/>
-      <c r="F5" s="141" t="s">
-        <v>237</v>
-      </c>
-      <c r="G5" s="141"/>
-    </row>
-    <row r="6" spans="2:7">
+      <c r="C3" s="143"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="143"/>
+      <c r="F3" s="143"/>
+      <c r="G3" s="143"/>
+    </row>
+    <row r="5" spans="2:22">
+      <c r="B5" s="144" t="s">
+        <v>366</v>
+      </c>
+      <c r="C5" s="144"/>
+      <c r="F5" s="144" t="s">
+        <v>365</v>
+      </c>
+      <c r="G5" s="144"/>
+      <c r="J5" s="140" t="s">
+        <v>240</v>
+      </c>
+      <c r="K5" s="140"/>
+      <c r="N5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22">
       <c r="B6" s="76"/>
       <c r="C6" s="94"/>
       <c r="F6" s="76"/>
       <c r="G6" s="94"/>
-    </row>
-    <row r="7" spans="2:7">
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="N6" s="32" t="s">
+        <v>340</v>
+      </c>
+      <c r="O6" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="P6" s="32">
+        <v>400</v>
+      </c>
+      <c r="T6" s="98" t="s">
+        <v>251</v>
+      </c>
+      <c r="U6" s="98">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22">
       <c r="B7" s="84" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C7" s="85">
-        <v>0.48</v>
+        <v>0.1</v>
       </c>
       <c r="F7" s="84" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="G7" s="85">
-        <v>0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7">
+        <v>0.86</v>
+      </c>
+      <c r="J7" s="114" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="115">
+        <v>13</v>
+      </c>
+      <c r="N7" s="32">
+        <v>310</v>
+      </c>
+      <c r="O7" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" s="32">
+        <v>10</v>
+      </c>
+      <c r="T7" s="98" t="s">
+        <v>252</v>
+      </c>
+      <c r="U7" s="98">
+        <v>22.3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22">
       <c r="B8" s="78" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C8" s="79">
-        <v>2000</v>
+        <v>200</v>
       </c>
       <c r="F8" s="86" t="s">
-        <v>0</v>
+        <v>349</v>
       </c>
       <c r="G8" s="87">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7">
+        <v>400</v>
+      </c>
+      <c r="J8" s="114" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="115">
+        <v>48</v>
+      </c>
+      <c r="N8" s="32">
+        <v>311</v>
+      </c>
+      <c r="O8" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="P8" s="32">
+        <f>AVERAGE(N7:N100)</f>
+        <v>365.2</v>
+      </c>
+      <c r="T8" s="98" t="s">
+        <v>253</v>
+      </c>
+      <c r="U8">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22">
       <c r="B9" s="86" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="87">
-        <v>982</v>
+        <v>26</v>
       </c>
       <c r="F9" s="95" t="s">
-        <v>197</v>
+        <v>350</v>
       </c>
       <c r="G9" s="96">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7">
+        <v>10</v>
+      </c>
+      <c r="J9" s="114" t="s">
+        <v>242</v>
+      </c>
+      <c r="K9" s="115">
+        <v>57</v>
+      </c>
+      <c r="N9" s="32">
+        <v>412</v>
+      </c>
+      <c r="O9" s="158" t="s">
+        <v>355</v>
+      </c>
+      <c r="P9" s="32">
+        <f>P6</f>
+        <v>400</v>
+      </c>
+      <c r="T9" s="98" t="s">
+        <v>20</v>
+      </c>
+      <c r="U9" s="98">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22">
       <c r="B10" s="97" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C10" s="98">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F10" s="97" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="G10" s="98">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7">
+        <v>0.05</v>
+      </c>
+      <c r="J10" s="114" t="s">
+        <v>243</v>
+      </c>
+      <c r="K10" s="115">
+        <v>39</v>
+      </c>
+      <c r="N10" s="32">
+        <v>368</v>
+      </c>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="T10" s="98" t="s">
+        <v>211</v>
+      </c>
+      <c r="U10" s="98">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22">
       <c r="B11" s="74" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C11" s="74" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="F11" s="74" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="G11" s="74">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="12" spans="2:7">
+      <c r="J11" s="118"/>
+      <c r="K11" s="119"/>
+      <c r="N11" s="32">
+        <v>447</v>
+      </c>
+      <c r="O11" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="P11" s="32">
+        <f>_xlfn.STDEV.S(N7:N16)</f>
+        <v>48.416709695907549</v>
+      </c>
+      <c r="T11" s="32"/>
+      <c r="U11" s="32"/>
+    </row>
+    <row r="12" spans="2:22">
       <c r="B12" s="32"/>
       <c r="C12" s="32"/>
       <c r="F12" s="32"/>
       <c r="G12" s="32"/>
-    </row>
-    <row r="13" spans="2:7">
+      <c r="J12" s="120" t="s">
+        <v>244</v>
+      </c>
+      <c r="K12" s="121">
+        <f>K8*(K9/100)*(1-(K9/100))</f>
+        <v>11.764800000000001</v>
+      </c>
+      <c r="N12" s="32">
+        <v>376</v>
+      </c>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="T12" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="U12" s="134" t="str">
+        <f>IF(U9&gt;=30, "Yes", "No")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22">
       <c r="B13" s="99" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C13" s="100">
         <f>C8*C7*(1-C7)</f>
-        <v>499.20000000000005</v>
+        <v>18</v>
       </c>
       <c r="F13" s="99" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="G13" s="101">
         <f>G9*G7*(1-G7)</f>
-        <v>170.52</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7">
+        <v>1.204</v>
+      </c>
+      <c r="J13" s="123" t="s">
+        <v>189</v>
+      </c>
+      <c r="K13" s="123" t="b">
+        <f>IF(K12 &gt;= 10, TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="N13" s="32">
+        <v>303</v>
+      </c>
+      <c r="O13" s="156" t="s">
+        <v>356</v>
+      </c>
+      <c r="P13" s="136">
+        <f>(P8-P9)/(P11/SQRT(P7))</f>
+        <v>-2.2729190658563367</v>
+      </c>
+      <c r="T13" s="32"/>
+      <c r="U13" s="32"/>
+    </row>
+    <row r="14" spans="2:22">
       <c r="B14" s="82" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="C14" s="102" t="b">
         <f>IF(C13&gt;=10, TRUE, FALSE)</f>
         <v>1</v>
       </c>
       <c r="F14" s="82" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="G14" s="82" t="b">
         <f>IF(G13&gt;=10, TRUE, FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7">
+        <v>0</v>
+      </c>
+      <c r="J14" s="124"/>
+      <c r="K14" s="94"/>
+      <c r="N14" s="32">
+        <v>410</v>
+      </c>
+      <c r="O14" s="32" t="s">
+        <v>357</v>
+      </c>
+      <c r="P14" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="T14" s="135" t="s">
+        <v>360</v>
+      </c>
+      <c r="U14" s="135">
+        <f>(U7-U6)/ (U8/SQRT(U9))</f>
+        <v>1.2162606385263026</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22">
       <c r="B15" s="74"/>
       <c r="C15" s="32"/>
       <c r="F15" s="74"/>
       <c r="G15" s="32"/>
-    </row>
-    <row r="16" spans="2:7">
+      <c r="J15" s="74" t="s">
+        <v>234</v>
+      </c>
+      <c r="K15" s="32">
+        <f>K7/K8</f>
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="N15" s="32">
+        <v>365</v>
+      </c>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="T15" s="136" t="s">
+        <v>255</v>
+      </c>
+      <c r="U15" s="131">
+        <f>TDIST(ABS(U14),U9-1,1)</f>
+        <v>0.11251867808518326</v>
+      </c>
+      <c r="V15" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22">
       <c r="B16" s="103" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C16" s="104">
         <f>C9/C8</f>
-        <v>0.49099999999999999</v>
+        <v>0.13</v>
       </c>
       <c r="F16" s="74" t="s">
-        <v>243</v>
+        <v>348</v>
       </c>
       <c r="G16" s="32">
         <f>G8/G9</f>
-        <v>0.5842857142857143</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12">
+        <v>40</v>
+      </c>
+      <c r="J16" s="74" t="s">
+        <v>245</v>
+      </c>
+      <c r="K16" s="32"/>
+      <c r="N16" s="32">
+        <v>350</v>
+      </c>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+    </row>
+    <row r="17" spans="2:21">
       <c r="B17" s="40"/>
       <c r="C17" s="105"/>
       <c r="F17" s="106" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="G17" s="107">
         <f>(G16-G7)/SQRT((G7*(1-G7))/G9)</f>
-        <v>0.22973840032238738</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12">
+        <v>356.70367016004735</v>
+      </c>
+      <c r="J17" s="74"/>
+      <c r="K17" s="126"/>
+      <c r="T17" s="137" t="s">
+        <v>256</v>
+      </c>
+      <c r="U17" s="134" t="str">
+        <f>IF(U15&gt;U10, "Do not reject", "Reject")</f>
+        <v>Do not reject</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21">
       <c r="B18" s="106" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C18" s="108">
         <f>(C16-C7)/SQRT((C7*(1-C7))/C8)</f>
-        <v>0.98465795180422111</v>
+        <v>1.4142135623730949</v>
       </c>
       <c r="D18" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="F18" s="74"/>
       <c r="G18" s="32"/>
-    </row>
-    <row r="19" spans="2:12">
+      <c r="J18" s="74" t="s">
+        <v>247</v>
+      </c>
+      <c r="K18" s="126">
+        <f>_xlfn.BINOM.DIST(K10-1,K8,K9/100,TRUE)</f>
+        <v>0.99964533162387259</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21">
       <c r="B19" s="74"/>
       <c r="C19" s="32"/>
       <c r="F19" s="109" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="G19" s="110">
         <f>TDIST(ABS(G17),G9-1,2)</f>
-        <v>0.81836226346609831</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12">
+        <v>5.4447377312745193E-20</v>
+      </c>
+      <c r="J19" s="130" t="s">
+        <v>248</v>
+      </c>
+      <c r="K19" s="131">
+        <f>1-K18</f>
+        <v>3.5466837612740942E-4</v>
+      </c>
+      <c r="T19" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21">
       <c r="B20" s="109" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="C20" s="111">
         <f>TDIST(ABS(C18),C8-1,1)</f>
-        <v>0.16245563671949209</v>
-      </c>
-      <c r="F20" s="112" t="s">
-        <v>247</v>
-      </c>
-      <c r="G20" s="113" t="str">
-        <f>IF(G19&gt;G10, "P &gt; a", "P &lt; a")</f>
-        <v>P &gt; a</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12">
+        <v>7.9430911180115582E-2</v>
+      </c>
+      <c r="F20" s="155" t="s">
+        <v>351</v>
+      </c>
+      <c r="J20" s="132" t="s">
+        <v>250</v>
+      </c>
+      <c r="K20" s="133">
+        <f>_xlfn.BINOM.DIST(K10,K8,K9/100,TRUE)</f>
+        <v>0.99989936814098268</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21">
       <c r="B21" s="112" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C21" s="113" t="str">
         <f>IF(C20&gt;C10, "P &gt; a", "P &lt; a")</f>
         <v>P &gt; a</v>
       </c>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:21">
+      <c r="B22" s="32"/>
+      <c r="C22" s="115" t="str">
+        <f>IF(C21="P &gt; a", "DON'T REJECT", "REJECT")</f>
+        <v>DON'T REJECT</v>
+      </c>
       <c r="D22" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12">
-      <c r="B24" s="141" t="s">
-        <v>248</v>
-      </c>
-      <c r="C24" s="141"/>
-      <c r="F24" s="142" t="s">
-        <v>249</v>
-      </c>
-      <c r="G24" s="142"/>
-    </row>
-    <row r="25" spans="2:12">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21">
+      <c r="B24" s="144" t="s">
+        <v>239</v>
+      </c>
+      <c r="C24" s="144"/>
+    </row>
+    <row r="25" spans="2:21">
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="K25" s="98" t="s">
-        <v>260</v>
-      </c>
-      <c r="L25" s="98">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12">
+      <c r="F25" s="112" t="s">
+        <v>238</v>
+      </c>
+      <c r="G25" s="113" t="str">
+        <f>IF(G19&gt;G10, "P &gt; a", "P &lt; a")</f>
+        <v>P &lt; a</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21">
       <c r="B26" s="85" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="85">
         <v>494</v>
       </c>
-      <c r="F26" s="114" t="s">
-        <v>0</v>
-      </c>
-      <c r="G26" s="115">
-        <v>13</v>
-      </c>
-      <c r="K26" s="98" t="s">
-        <v>261</v>
-      </c>
-      <c r="L26" s="98">
-        <v>105.2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12">
+      <c r="G26" s="115" t="str">
+        <f>IF(G25="P &gt; a", "DON'T REJECT NULL HYPOTHESIS", "REJECT NULL HYPOTHESIS")</f>
+        <v>REJECT NULL HYPOTHESIS</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21">
       <c r="B27" s="116" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="116">
         <v>1195</v>
       </c>
-      <c r="F27" s="114" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="115">
-        <v>48</v>
-      </c>
-      <c r="K27" s="98" t="s">
-        <v>262</v>
-      </c>
-      <c r="L27">
-        <v>21.8</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12">
+    </row>
+    <row r="28" spans="2:21">
       <c r="B28" s="79" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C28" s="79">
         <v>0.4</v>
       </c>
-      <c r="F28" s="114" t="s">
-        <v>251</v>
-      </c>
-      <c r="G28" s="115">
-        <v>57</v>
-      </c>
-      <c r="K28" s="98" t="s">
-        <v>20</v>
-      </c>
-      <c r="L28" s="98">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12">
+    </row>
+    <row r="29" spans="2:21">
       <c r="B29" s="117" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="C29" s="117">
         <v>99</v>
       </c>
-      <c r="F29" s="114" t="s">
-        <v>252</v>
-      </c>
-      <c r="G29" s="115">
-        <v>39</v>
-      </c>
-      <c r="K29" s="98" t="s">
-        <v>218</v>
-      </c>
-      <c r="L29" s="98">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12">
+    </row>
+    <row r="30" spans="2:21">
       <c r="B30" s="40"/>
       <c r="C30" s="105"/>
-      <c r="F30" s="118"/>
-      <c r="G30" s="119"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32"/>
-    </row>
-    <row r="31" spans="2:12">
+    </row>
+    <row r="31" spans="2:21">
       <c r="B31" s="32" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C31" s="32">
         <f>C27*(C28/100)*(1-(C28/100))</f>
         <v>4.7608800000000002</v>
       </c>
-      <c r="F31" s="120" t="s">
-        <v>253</v>
-      </c>
-      <c r="G31" s="121">
-        <f>G27*(G28/100)*(1-(G28/100))</f>
-        <v>11.764800000000001</v>
-      </c>
-      <c r="K31" s="31" t="s">
-        <v>263</v>
-      </c>
-      <c r="L31" s="134" t="str">
-        <f>IF(L28&gt;=30, "Yes", "No")</f>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12">
+    </row>
+    <row r="32" spans="2:21">
       <c r="B32" s="32"/>
       <c r="C32" s="122"/>
-      <c r="F32" s="123" t="s">
-        <v>196</v>
-      </c>
-      <c r="G32" s="123" t="b">
-        <f>IF(G31 &gt;= 10, TRUE, FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-    </row>
-    <row r="33" spans="2:12">
+    </row>
+    <row r="33" spans="2:4">
       <c r="B33" s="32" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C33" s="32">
         <f>((100-C29) /2)/100</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F33" s="124"/>
-      <c r="G33" s="94"/>
-      <c r="K33" s="135" t="s">
-        <v>264</v>
-      </c>
-      <c r="L33" s="135">
-        <f>(L26-L25)/ (L27/SQRT(L28))</f>
-        <v>1.5086095259518884</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12">
+    </row>
+    <row r="34" spans="2:4">
       <c r="B34" s="32" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C34" s="32">
         <f>_xlfn.NORM.INV((1-C33),0,1)</f>
         <v>2.5758293035488999</v>
       </c>
-      <c r="F34" s="74" t="s">
-        <v>243</v>
-      </c>
-      <c r="G34" s="32">
-        <f>G26/G27</f>
-        <v>0.27083333333333331</v>
-      </c>
-      <c r="K34" s="136" t="s">
-        <v>265</v>
-      </c>
-      <c r="L34" s="131">
-        <f>TDIST(ABS(L33),L28-1,1)</f>
-        <v>6.9728940266272882E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12">
+    </row>
+    <row r="35" spans="2:4">
       <c r="B35" s="118"/>
       <c r="C35" s="119"/>
-      <c r="F35" s="74" t="s">
-        <v>254</v>
-      </c>
-      <c r="G35" s="32"/>
-    </row>
-    <row r="36" spans="2:12">
+    </row>
+    <row r="36" spans="2:4">
       <c r="B36" s="125" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="C36" s="125">
         <f>C26/C27</f>
         <v>0.41338912133891215</v>
       </c>
-      <c r="F36" s="74"/>
-      <c r="G36" s="126"/>
-      <c r="K36" s="137" t="s">
-        <v>266</v>
-      </c>
-      <c r="L36" s="134" t="str">
-        <f>IF(L34&gt;L29, "Do not reject", "Reject")</f>
-        <v>Reject</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12">
+    </row>
+    <row r="37" spans="2:4">
       <c r="B37" s="127"/>
       <c r="C37" s="128"/>
-      <c r="F37" s="74" t="s">
-        <v>256</v>
-      </c>
-      <c r="G37" s="126">
-        <f>_xlfn.BINOM.DIST(G29-1,G27,G28/100,TRUE)</f>
-        <v>0.99964533162387259</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12">
+    </row>
+    <row r="38" spans="2:4">
       <c r="B38" s="102" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C38" s="129">
         <f>C36-(C34*SQRT((C36*(1-C36))/C27))</f>
         <v>0.37669574247190074</v>
       </c>
-      <c r="F38" s="130" t="s">
-        <v>257</v>
-      </c>
-      <c r="G38" s="131">
-        <f>1-G37</f>
-        <v>3.5466837612740942E-4</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12">
+    </row>
+    <row r="39" spans="2:4">
       <c r="B39" s="102" t="s">
         <v>68</v>
       </c>
@@ -5205,52 +5796,50 @@
         <v>0.45008250020592355</v>
       </c>
       <c r="D39" t="s">
-        <v>258</v>
-      </c>
-      <c r="F39" s="132" t="s">
-        <v>259</v>
-      </c>
-      <c r="G39" s="133">
-        <f>_xlfn.BINOM.DIST(G29,G27,G28/100,TRUE)</f>
-        <v>0.99989936814098268</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4">
       <c r="B45" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4">
       <c r="B47" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4">
       <c r="B48" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="B49" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="B50" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="29">
       <c r="A52" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="B52" s="138" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="29">
       <c r="B53" s="138" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="21">
@@ -5258,41 +5847,55 @@
     </row>
     <row r="61" spans="1:2" ht="17">
       <c r="B61" s="15" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="B62" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="69" spans="2:2" ht="17">
       <c r="B69" s="15" t="s">
-        <v>281</v>
+        <v>271</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" ht="26">
+      <c r="B72" s="154" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" ht="17">
+      <c r="B74" s="15" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" t="s">
+        <v>359</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="F24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5301,10 +5904,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C96CE9-B77B-704D-8A1F-7836B7353FCF}">
-  <dimension ref="A1:AI33"/>
+  <dimension ref="A1:AI69"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="L1" zoomScale="94" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5321,12 +5924,14 @@
     <col min="14" max="14" width="18" customWidth="1"/>
     <col min="16" max="16" width="24.6640625" customWidth="1"/>
     <col min="17" max="17" width="14.6640625" customWidth="1"/>
+    <col min="19" max="19" width="29" customWidth="1"/>
     <col min="24" max="24" width="13.33203125" customWidth="1"/>
+    <col min="26" max="26" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="26">
       <c r="A1" s="32" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B1" s="34"/>
       <c r="D1" s="32" t="s">
@@ -5334,7 +5939,7 @@
       </c>
       <c r="E1" s="34"/>
       <c r="G1" s="32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H1" s="34"/>
       <c r="J1" s="32"/>
@@ -5343,85 +5948,85 @@
       </c>
       <c r="L1" s="44"/>
       <c r="P1" s="31" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="Q1" s="32"/>
       <c r="S1" s="32" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="T1" s="32"/>
       <c r="V1" s="32" t="s">
-        <v>158</v>
+        <v>325</v>
       </c>
       <c r="W1" s="32"/>
       <c r="X1" s="32"/>
       <c r="Z1" s="32" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="AA1" s="32" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AD1" s="32" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="AE1" s="32"/>
       <c r="AH1" s="32" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="AI1" s="32"/>
     </row>
     <row r="2" spans="1:35">
       <c r="A2" s="35" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B2" s="34"/>
       <c r="D2" s="32"/>
       <c r="E2" s="34"/>
       <c r="G2" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="H2" s="36">
-        <v>-0.89</v>
+        <v>318</v>
+      </c>
+      <c r="H2" s="149">
+        <v>-2</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K2" s="40" t="s">
         <v>43</v>
       </c>
       <c r="L2" s="45"/>
       <c r="P2" s="32" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="Q2" s="32">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="S2" s="32" t="s">
         <v>22</v>
       </c>
       <c r="T2" s="32">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="V2" s="32"/>
       <c r="W2" s="32"/>
       <c r="X2" s="32"/>
       <c r="Z2" s="35" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AA2" s="49">
-        <v>0.08</v>
+        <v>0.25</v>
       </c>
       <c r="AD2" s="32" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AE2" s="32">
-        <v>-1.72</v>
+        <v>0.44</v>
       </c>
       <c r="AH2" s="32" t="s">
         <v>25</v>
       </c>
       <c r="AI2" s="32">
-        <v>45</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:35">
@@ -5429,7 +6034,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="36">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="D3" s="32" t="s">
         <v>22</v>
@@ -5438,33 +6043,33 @@
         <v>1252</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="H3" s="36">
-        <v>1.88</v>
+        <v>319</v>
+      </c>
+      <c r="H3" s="149">
+        <v>2</v>
       </c>
       <c r="J3" s="32"/>
       <c r="K3" s="40"/>
       <c r="L3" s="45"/>
       <c r="P3" s="32" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="Q3" s="32">
         <f>Q2/100</f>
-        <v>0.39</v>
+        <v>0.96</v>
       </c>
       <c r="S3" s="32" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="T3" s="32">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="V3" s="32"/>
       <c r="W3" s="32" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="X3" s="32" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="Z3" s="35"/>
       <c r="AA3" s="49"/>
@@ -5474,7 +6079,7 @@
         <v>22</v>
       </c>
       <c r="AI3" s="32">
-        <v>47</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:35">
@@ -5482,7 +6087,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="36">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>23</v>
@@ -5491,26 +6096,26 @@
         <v>129</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="H4" s="36">
+        <v>320</v>
+      </c>
+      <c r="H4" s="149">
         <f>_xlfn.NORM.DIST(H2, 0, 1, TRUE)</f>
-        <v>0.18673294303717258</v>
+        <v>2.2750131948179191E-2</v>
       </c>
       <c r="J4" s="38" t="s">
         <v>60</v>
       </c>
       <c r="K4" s="41">
-        <v>49</v>
+        <v>1262</v>
       </c>
       <c r="L4" s="45"/>
       <c r="P4" s="32"/>
       <c r="Q4" s="32"/>
       <c r="S4" s="32" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="T4" s="32">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="V4" s="32" t="s">
         <v>0</v>
@@ -5519,86 +6124,86 @@
         <v>25</v>
       </c>
       <c r="X4" s="32">
-        <v>1156</v>
+        <v>1229</v>
       </c>
       <c r="Z4" s="35" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="AA4" s="49">
         <f xml:space="preserve"> 1 - AA2</f>
-        <v>0.92</v>
+        <v>0.75</v>
       </c>
       <c r="AD4" s="32" t="s">
         <v>79</v>
       </c>
       <c r="AE4" s="32">
         <f>_xlfn.NORM.S.DIST(AE2, TRUE)</f>
-        <v>4.2716220791328911E-2</v>
+        <v>0.67003144633940637</v>
       </c>
       <c r="AH4" s="32" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="AI4" s="32">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:35">
       <c r="A5" s="35" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B5" s="36">
-        <v>1000</v>
+        <v>119</v>
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="34"/>
       <c r="G5" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="H5" s="36">
+        <v>321</v>
+      </c>
+      <c r="H5" s="149">
         <f>1 - _xlfn.NORM.DIST(H3, 0, 1, TRUE)</f>
-        <v>3.0054038961199736E-2</v>
+        <v>2.2750131948179209E-2</v>
       </c>
       <c r="J5" s="38" t="s">
         <v>23</v>
       </c>
       <c r="K5" s="42">
-        <v>5</v>
+        <v>118</v>
       </c>
       <c r="L5" s="45"/>
       <c r="P5" s="32" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q5" s="32">
         <f xml:space="preserve"> (1 - Q3) / 2</f>
-        <v>0.30499999999999999</v>
+        <v>2.0000000000000018E-2</v>
       </c>
       <c r="S5" s="32"/>
       <c r="T5" s="32"/>
       <c r="V5" s="32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="W5" s="32">
-        <v>21.3</v>
+        <v>21.4</v>
       </c>
       <c r="X5" s="32">
-        <v>1037</v>
+        <v>1026</v>
       </c>
       <c r="Z5" s="35" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="AA5" s="59">
         <f>_xlfn.NORM.INV(AA4,0, 1)</f>
-        <v>1.4050715603096329</v>
+        <v>0.67448975019608193</v>
       </c>
       <c r="AH5" s="32"/>
       <c r="AI5" s="32"/>
     </row>
     <row r="6" spans="1:35">
       <c r="A6" s="35" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B6" s="36">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>67</v>
@@ -5607,43 +6212,43 @@
         <v>1100</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="H6" s="36">
+        <v>81</v>
+      </c>
+      <c r="H6" s="149">
         <f>SUM(H4:H5)</f>
-        <v>0.21678698199837232</v>
+        <v>4.5500263896358403E-2</v>
       </c>
       <c r="J6" s="38" t="s">
         <v>78</v>
       </c>
       <c r="K6" s="42">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="L6" s="45"/>
       <c r="P6" s="33"/>
       <c r="Q6" s="32"/>
-      <c r="S6" s="32" t="s">
-        <v>156</v>
-      </c>
-      <c r="T6" s="32">
+      <c r="S6" s="157" t="s">
+        <v>151</v>
+      </c>
+      <c r="T6" s="136">
         <f>(1 - _xlfn.NORM.DIST(T4,T2,T3, TRUE)) * 100</f>
-        <v>90.072860315666901</v>
+        <v>4.7790352272814696</v>
       </c>
       <c r="V6" s="32" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="W6" s="32">
-        <v>4.5999999999999996</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="X6" s="32">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="AH6" s="32" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="AI6" s="32">
         <f>_xlfn.NORM.DIST(AI2,AI3,AI4, TRUE)</f>
-        <v>0.42074029056089696</v>
+        <v>0.35806478442778267</v>
       </c>
     </row>
     <row r="7" spans="1:35">
@@ -5657,65 +6262,74 @@
         <v>-1.1782945736434109</v>
       </c>
       <c r="J7" s="38" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K7" s="42">
         <f>K6/100</f>
-        <v>0.15</v>
+        <v>0.97</v>
       </c>
       <c r="L7" s="45"/>
       <c r="P7" s="32" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q7" s="32">
-        <f>_xlfn.NORM.DIST(Q5, 0, 1, TRUE)</f>
-        <v>0.61981692384016507</v>
+        <f>- _xlfn.NORM.DIST(Q5, 0, 1, TRUE)</f>
+        <v>-0.50797831371690205</v>
       </c>
       <c r="S7" s="32"/>
-      <c r="T7" s="32">
-        <f>NORMINV(0.07,19,2.5)</f>
-        <v>15.310522429552075</v>
-      </c>
+      <c r="T7" s="32"/>
       <c r="V7" s="32" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="W7" s="32">
         <f>(W4-W5)/W6</f>
-        <v>0.80434782608695643</v>
+        <v>0.70588235294117685</v>
       </c>
       <c r="X7" s="32">
         <f>(X4-X5)/X6</f>
-        <v>0.59203980099502485</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35">
-      <c r="A8" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" s="36">
-        <f>_xlfn.NORM.DIST(B6, B3, B4, TRUE) - _xlfn.NORM.DIST(B5, B3, B4, TRUE)</f>
-        <v>-0.90072860315666903</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" ht="21" customHeight="1">
+      <c r="A8" s="152" t="s">
+        <v>337</v>
+      </c>
+      <c r="B8" s="2">
+        <f>B3</f>
+        <v>123</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="34"/>
+      <c r="G8" s="150" t="s">
+        <v>322</v>
+      </c>
       <c r="J8" s="32"/>
       <c r="K8" s="40"/>
       <c r="L8" s="45"/>
       <c r="P8" s="32" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="Q8" s="32">
         <f>_xlfn.NORM.DIST(Q5, 0, 1, TRUE)</f>
-        <v>0.61981692384016507</v>
+        <v>0.50797831371690205</v>
+      </c>
+      <c r="S8" s="156" t="s">
+        <v>352</v>
+      </c>
+      <c r="T8" s="136">
+        <f>_xlfn.NORM.INV(0.97, 15, 3)</f>
+        <v>20.642380824453753</v>
+      </c>
+      <c r="AH8" s="151" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="19">
-      <c r="A9" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="B9" s="36">
-        <f>_xlfn.NORM.DIST(B5,B3,B4,TRUE)</f>
-        <v>1</v>
+      <c r="A9" s="152" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2">
+        <v>17</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>68</v>
@@ -5723,30 +6337,34 @@
       <c r="E9" s="34">
         <v>1400</v>
       </c>
+      <c r="G9" s="150" t="s">
+        <v>323</v>
+      </c>
       <c r="J9" s="47" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="K9" s="48">
         <f>_xlfn.NORM.INV(($K$6/100),K$4,K$5)</f>
-        <v>43.81783305253105</v>
+        <v>1483.9336457618476</v>
       </c>
       <c r="L9" s="45"/>
       <c r="P9" s="32"/>
       <c r="Q9" s="32"/>
       <c r="S9" s="21" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="T9" t="s">
         <v>43</v>
       </c>
+      <c r="AH9" s="15"/>
     </row>
     <row r="10" spans="1:35" ht="17">
-      <c r="A10" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="B10" s="36">
-        <f>1 - _xlfn.NORM.DIST(B6, B3, B4, TRUE)</f>
-        <v>0.90072860315666903</v>
+      <c r="A10" s="152" t="s">
+        <v>338</v>
+      </c>
+      <c r="B10" s="2">
+        <f>B4/SQRT(B9)</f>
+        <v>2.6678918753996625</v>
       </c>
       <c r="D10" s="32" t="s">
         <v>72</v>
@@ -5764,25 +6382,17 @@
       </c>
       <c r="Q10" s="32"/>
       <c r="S10" s="21"/>
+      <c r="AH10" s="15"/>
     </row>
     <row r="11" spans="1:35" ht="17">
-      <c r="A11" s="35"/>
-      <c r="B11" s="36"/>
       <c r="D11" s="32"/>
       <c r="E11" s="34"/>
       <c r="J11" s="32"/>
       <c r="K11" s="43"/>
       <c r="L11" s="45"/>
-      <c r="S11" s="21"/>
-    </row>
-    <row r="12" spans="1:35">
-      <c r="A12" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="B12" s="36">
-        <f>B9*100</f>
-        <v>100</v>
-      </c>
+      <c r="AH11" s="15"/>
+    </row>
+    <row r="12" spans="1:35" ht="17">
       <c r="D12" s="32" t="s">
         <v>70</v>
       </c>
@@ -5793,6 +6403,7 @@
       <c r="J12" s="32"/>
       <c r="K12" s="43"/>
       <c r="L12" s="46"/>
+      <c r="AH12" s="15"/>
     </row>
     <row r="13" spans="1:35">
       <c r="D13" s="32" t="s">
@@ -5807,34 +6418,55 @@
       <c r="L13" s="45"/>
     </row>
     <row r="14" spans="1:35">
+      <c r="A14" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="36">
+        <f>_xlfn.NORM.DIST(B6, B3, B4, TRUE) - _xlfn.NORM.DIST(B5, B3, B4, TRUE)</f>
+        <v>0</v>
+      </c>
       <c r="D14" s="32"/>
       <c r="E14" s="34"/>
       <c r="J14" s="39" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="K14" s="49">
         <f>(1 - K7)/2</f>
-        <v>0.42499999999999999</v>
+        <v>1.5000000000000013E-2</v>
       </c>
     </row>
     <row r="15" spans="1:35">
+      <c r="A15" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="36">
+        <f>_xlfn.NORM.DIST(B5,B3,B4,TRUE)</f>
+        <v>0.35806478442778267</v>
+      </c>
       <c r="D15" s="32"/>
       <c r="E15" s="34">
         <f>E13-E12</f>
         <v>-0.11933959517437347</v>
       </c>
       <c r="J15" s="32" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="K15" s="49">
         <f>K7+K14</f>
-        <v>0.57499999999999996</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="P15" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:35">
+      <c r="A16" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="36">
+        <f>1 - _xlfn.NORM.DIST(B6, B3, B4, TRUE)</f>
+        <v>0.64193521557221733</v>
+      </c>
       <c r="D16" s="32"/>
       <c r="E16" s="34"/>
       <c r="J16" s="32"/>
@@ -5846,7 +6478,9 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="17" spans="4:17">
+    <row r="17" spans="1:17">
+      <c r="A17" s="35"/>
+      <c r="B17" s="36"/>
       <c r="D17" s="32" t="s">
         <v>74</v>
       </c>
@@ -5854,20 +6488,27 @@
         <v>1175</v>
       </c>
       <c r="J17" s="39" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K17" s="49">
         <f>NORMINV(K14, 0, 1)</f>
-        <v>-0.18911842627279254</v>
+        <v>-2.1700903775845601</v>
       </c>
       <c r="P17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="Q17">
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="4:17">
+    <row r="18" spans="1:17">
+      <c r="A18" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" s="36">
+        <f>B15*100</f>
+        <v>35.806478442778264</v>
+      </c>
       <c r="D18" s="32" t="s">
         <v>73</v>
       </c>
@@ -5876,20 +6517,20 @@
         <v>0.7247126675619795</v>
       </c>
       <c r="J18" s="32" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K18" s="49">
         <f>NORMINV(K15, 0, 1)</f>
-        <v>0.18911842627279243</v>
+        <v>2.1700903775845601</v>
       </c>
       <c r="P18" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="Q18">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="4:17">
+    <row r="19" spans="1:17">
       <c r="D19" s="32"/>
       <c r="E19" s="34" t="s">
         <v>43</v>
@@ -5897,62 +6538,62 @@
       <c r="J19" s="32"/>
       <c r="K19" s="35"/>
       <c r="P19" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="Q19">
         <f>Q18/100</f>
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="20" spans="4:17">
+    <row r="20" spans="1:17">
       <c r="D20" s="32" t="s">
         <v>75</v>
       </c>
       <c r="E20" s="34"/>
       <c r="J20" s="32" t="s">
-        <v>153</v>
+        <v>324</v>
       </c>
       <c r="K20" s="35"/>
       <c r="L20" s="32"/>
     </row>
-    <row r="21" spans="4:17">
+    <row r="21" spans="1:17" ht="23" customHeight="1">
       <c r="D21" s="32" t="s">
         <v>76</v>
       </c>
       <c r="E21" s="34"/>
       <c r="J21" s="32" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K21" s="51">
         <f>K4 + (K17)*K5</f>
-        <v>48.054407868636041</v>
+        <v>1005.9293354450219</v>
       </c>
       <c r="P21" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="Q21">
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="4:17">
+    <row r="22" spans="1:17" ht="31" customHeight="1">
       <c r="D22" s="32"/>
       <c r="E22" s="34"/>
       <c r="J22" s="32" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K22" s="51">
         <f>K4+(K18*K5)</f>
-        <v>49.945592131363959</v>
+        <v>1518.0706645549781</v>
       </c>
       <c r="P22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="Q22">
         <f>Q21/100</f>
         <v>0.96</v>
       </c>
     </row>
-    <row r="23" spans="4:17">
+    <row r="23" spans="1:17">
       <c r="D23" s="32" t="s">
         <v>80</v>
       </c>
@@ -5960,70 +6601,141 @@
       <c r="J23" s="32"/>
       <c r="K23" s="35"/>
     </row>
-    <row r="24" spans="4:17">
+    <row r="24" spans="1:17">
       <c r="E24" s="2"/>
       <c r="J24" s="32"/>
       <c r="K24" s="35"/>
     </row>
-    <row r="25" spans="4:17">
+    <row r="25" spans="1:17">
       <c r="E25" s="2"/>
       <c r="J25" s="32"/>
       <c r="K25" s="35"/>
     </row>
-    <row r="26" spans="4:17">
+    <row r="26" spans="1:17">
+      <c r="A26" s="28" t="s">
+        <v>306</v>
+      </c>
       <c r="J26" s="34" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="K26" s="51">
         <f>K28-K27</f>
-        <v>6.7448975019608213</v>
-      </c>
-    </row>
-    <row r="27" spans="4:17">
+        <v>159.17958104627542</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="28" t="s">
+        <v>307</v>
+      </c>
       <c r="J27" s="34" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="K27" s="30">
         <f>_xlfn.NORM.INV((25/100),K$4,K$5)</f>
-        <v>45.627551249019589</v>
-      </c>
-    </row>
-    <row r="28" spans="4:17">
+        <v>1182.4102094768623</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" s="4" t="s">
+        <v>308</v>
+      </c>
       <c r="J28" s="34" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K28" s="30">
         <f>_xlfn.NORM.INV((75/100),K$4,K$5)</f>
-        <v>52.372448750980411</v>
-      </c>
-    </row>
-    <row r="31" spans="4:17">
+        <v>1341.5897905231377</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" s="28" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="17">
+      <c r="A30" s="15" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" s="28" t="s">
+        <v>315</v>
+      </c>
       <c r="P31" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="Q31">
         <f>NORMINV(0.28,1264,116)</f>
         <v>1196.390385156539</v>
       </c>
     </row>
-    <row r="32" spans="4:17">
+    <row r="32" spans="1:17">
+      <c r="A32" s="28" t="s">
+        <v>316</v>
+      </c>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="4:5">
+    <row r="33" spans="1:5" ht="17">
+      <c r="A33" s="15" t="s">
+        <v>317</v>
+      </c>
       <c r="D33" s="10"/>
       <c r="E33" s="2"/>
     </row>
+    <row r="34" spans="1:5" ht="17">
+      <c r="A34" s="15"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="148" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="148" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="148" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="148" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="153"/>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>342</v>
+      </c>
+      <c r="D68" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>345</v>
+      </c>
+      <c r="D69" t="s">
+        <v>344</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77044CB3-A584-0B47-8E5D-C4DB8D5DE250}">
-  <dimension ref="B2:K22"/>
+  <dimension ref="B2:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6031,9 +6743,10 @@
     <col min="2" max="2" width="28.83203125" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="8" max="8" width="18.83203125" customWidth="1"/>
+    <col min="13" max="13" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:14">
       <c r="B2" s="60"/>
       <c r="C2" s="60"/>
       <c r="D2" s="60"/>
@@ -6045,25 +6758,28 @@
       <c r="J2" s="60"/>
       <c r="K2" s="60"/>
     </row>
-    <row r="3" spans="2:11">
-      <c r="B3" s="143" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="143"/>
+    <row r="3" spans="2:14">
+      <c r="B3" s="145" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="145"/>
       <c r="D3" s="60"/>
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="143" t="s">
-        <v>191</v>
-      </c>
-      <c r="I3" s="143"/>
+      <c r="H3" s="145" t="s">
+        <v>184</v>
+      </c>
+      <c r="I3" s="145"/>
       <c r="J3" s="60"/>
       <c r="K3" s="60"/>
-    </row>
-    <row r="4" spans="2:11">
+      <c r="M3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
       <c r="B4" s="61" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C4" s="61">
         <v>95</v>
@@ -6081,9 +6797,9 @@
       <c r="J4" s="60"/>
       <c r="K4" s="60"/>
     </row>
-    <row r="5" spans="2:11">
+    <row r="5" spans="2:14">
       <c r="B5" s="61" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C5" s="61">
         <v>47</v>
@@ -6104,10 +6820,17 @@
       </c>
       <c r="J5" s="60"/>
       <c r="K5" s="60"/>
-    </row>
-    <row r="6" spans="2:11">
+      <c r="M5" t="s">
+        <v>341</v>
+      </c>
+      <c r="N5">
+        <f>AVERAGE(M15:M24)</f>
+        <v>166.6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14">
       <c r="B6" s="61" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C6" s="61">
         <v>3</v>
@@ -6122,7 +6845,7 @@
       </c>
       <c r="G6" s="60"/>
       <c r="H6" s="61" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="I6" s="61">
         <v>0.65700000000000003</v>
@@ -6130,7 +6853,7 @@
       <c r="J6" s="60"/>
       <c r="K6" s="60"/>
     </row>
-    <row r="7" spans="2:11">
+    <row r="7" spans="2:14">
       <c r="B7" s="62" t="s">
         <v>67</v>
       </c>
@@ -6140,7 +6863,7 @@
       </c>
       <c r="D7" s="60"/>
       <c r="E7" s="61" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="F7" s="61">
         <f>F5*F6*(1-F6)</f>
@@ -6148,7 +6871,7 @@
       </c>
       <c r="G7" s="60"/>
       <c r="H7" s="61" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="I7" s="61">
         <v>1200</v>
@@ -6156,7 +6879,7 @@
       <c r="J7" s="60"/>
       <c r="K7" s="60"/>
     </row>
-    <row r="8" spans="2:11">
+    <row r="8" spans="2:14">
       <c r="B8" s="62" t="s">
         <v>68</v>
       </c>
@@ -6166,7 +6889,7 @@
       </c>
       <c r="D8" s="60"/>
       <c r="E8" s="61" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="F8" s="61">
         <v>90</v>
@@ -6182,12 +6905,12 @@
       <c r="J8" s="60"/>
       <c r="K8" s="60"/>
     </row>
-    <row r="9" spans="2:11">
+    <row r="9" spans="2:14">
       <c r="B9" s="60"/>
       <c r="C9" s="60"/>
       <c r="D9" s="60"/>
       <c r="E9" s="61" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F9" s="63">
         <f>SQRT((F6*(1-F6))/F5)</f>
@@ -6195,7 +6918,7 @@
       </c>
       <c r="G9" s="60"/>
       <c r="H9" s="62" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="I9" s="62">
         <f>(I6-I5)/2</f>
@@ -6204,12 +6927,12 @@
       <c r="J9" s="60"/>
       <c r="K9" s="60"/>
     </row>
-    <row r="10" spans="2:11">
+    <row r="10" spans="2:14">
       <c r="B10" s="60"/>
       <c r="C10" s="60"/>
       <c r="D10" s="60"/>
       <c r="E10" s="61" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="F10" s="61">
         <f>((100-F8) /2)/100</f>
@@ -6226,12 +6949,12 @@
       <c r="J10" s="60"/>
       <c r="K10" s="60"/>
     </row>
-    <row r="11" spans="2:11">
+    <row r="11" spans="2:14">
       <c r="B11" s="60"/>
       <c r="C11" s="60"/>
       <c r="D11" s="60"/>
       <c r="E11" s="61" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="F11" s="61">
         <f>_xlfn.NORM.INV((1-F10),0,1)</f>
@@ -6243,12 +6966,12 @@
       <c r="J11" s="60"/>
       <c r="K11" s="60"/>
     </row>
-    <row r="12" spans="2:11">
+    <row r="12" spans="2:14">
       <c r="B12" s="60"/>
       <c r="C12" s="60"/>
       <c r="D12" s="60"/>
       <c r="E12" s="62" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="F12" s="64">
         <f>F6-F$11*F9</f>
@@ -6260,7 +6983,7 @@
       <c r="J12" s="60"/>
       <c r="K12" s="60"/>
     </row>
-    <row r="13" spans="2:11">
+    <row r="13" spans="2:14">
       <c r="B13" s="60"/>
       <c r="C13" s="60"/>
       <c r="D13" s="60"/>
@@ -6277,11 +7000,11 @@
       <c r="J13" s="60"/>
       <c r="K13" s="60"/>
     </row>
-    <row r="14" spans="2:11">
-      <c r="B14" s="143" t="s">
-        <v>203</v>
-      </c>
-      <c r="C14" s="143"/>
+    <row r="14" spans="2:14">
+      <c r="B14" s="145" t="s">
+        <v>196</v>
+      </c>
+      <c r="C14" s="145"/>
       <c r="D14" s="60"/>
       <c r="E14" s="60"/>
       <c r="F14" s="60"/>
@@ -6290,35 +7013,41 @@
       <c r="I14" s="60"/>
       <c r="J14" s="60"/>
       <c r="K14" s="60"/>
-    </row>
-    <row r="15" spans="2:11">
+      <c r="M14" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14">
       <c r="B15" s="61" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C15" s="61">
         <v>0.05</v>
       </c>
       <c r="D15" s="60"/>
-      <c r="E15" s="143" t="s">
-        <v>205</v>
-      </c>
-      <c r="F15" s="143"/>
+      <c r="E15" s="145" t="s">
+        <v>198</v>
+      </c>
+      <c r="F15" s="145"/>
       <c r="G15" s="66"/>
       <c r="H15" s="66"/>
       <c r="I15" s="66"/>
       <c r="J15" s="67"/>
       <c r="K15" s="60"/>
-    </row>
-    <row r="16" spans="2:11">
+      <c r="M15">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14">
       <c r="B16" s="61" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C16" s="61">
         <v>94</v>
       </c>
       <c r="D16" s="60"/>
       <c r="E16" s="61" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="F16" s="61">
         <v>1</v>
@@ -6328,10 +7057,13 @@
       <c r="I16" s="60"/>
       <c r="J16" s="68"/>
       <c r="K16" s="60"/>
-    </row>
-    <row r="17" spans="2:11">
+      <c r="M16">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
       <c r="B17" s="61" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C17" s="61">
         <v>0.51</v>
@@ -6346,10 +7078,13 @@
       <c r="I17" s="60"/>
       <c r="J17" s="68"/>
       <c r="K17" s="60"/>
-    </row>
-    <row r="18" spans="2:11">
+      <c r="M17">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13">
       <c r="B18" s="61" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C18" s="61">
         <f>((100-C16)/100)/2</f>
@@ -6357,7 +7092,7 @@
       </c>
       <c r="D18" s="60"/>
       <c r="E18" s="61" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="F18" s="61">
         <f>F17^2</f>
@@ -6368,10 +7103,13 @@
       <c r="I18" s="60"/>
       <c r="J18" s="68"/>
       <c r="K18" s="60"/>
-    </row>
-    <row r="19" spans="2:11">
+      <c r="M18">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
       <c r="B19" s="61" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C19" s="69">
         <f>_xlfn.NORM.INV(1-C18,0,1)</f>
@@ -6385,10 +7123,13 @@
       <c r="I19" s="60"/>
       <c r="J19" s="68"/>
       <c r="K19" s="60"/>
-    </row>
-    <row r="20" spans="2:11">
+      <c r="M19">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
       <c r="B20" s="62" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C20" s="64">
         <f xml:space="preserve"> C17*(1-C17)*((C19/C15)^2)</f>
@@ -6396,7 +7137,7 @@
       </c>
       <c r="D20" s="60"/>
       <c r="E20" s="70" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="F20" s="60"/>
       <c r="G20" s="60"/>
@@ -6404,10 +7145,13 @@
       <c r="I20" s="60"/>
       <c r="J20" s="68"/>
       <c r="K20" s="60"/>
-    </row>
-    <row r="21" spans="2:11">
+      <c r="M20">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13">
       <c r="B21" s="62" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C21" s="64">
         <f>0.25*((C19/C15)^2)</f>
@@ -6415,7 +7159,7 @@
       </c>
       <c r="D21" s="60"/>
       <c r="E21" s="71" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F21" s="72"/>
       <c r="G21" s="72"/>
@@ -6423,8 +7167,11 @@
       <c r="I21" s="72"/>
       <c r="J21" s="73"/>
       <c r="K21" s="60"/>
-    </row>
-    <row r="22" spans="2:11">
+      <c r="M21">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13">
       <c r="B22" s="60"/>
       <c r="C22" s="60"/>
       <c r="D22" s="60"/>
@@ -6435,6 +7182,19 @@
       <c r="I22" s="60"/>
       <c r="J22" s="60"/>
       <c r="K22" s="60"/>
+      <c r="M22">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13">
+      <c r="M23">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13">
+      <c r="M24">
+        <v>154</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6451,8 +7211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7934B88-A85A-EB42-B4EC-BEBEC08109DD}">
   <dimension ref="B4:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="160" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6466,19 +7226,19 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:10">
-      <c r="B4" s="141" t="s">
-        <v>215</v>
-      </c>
-      <c r="C4" s="141"/>
-      <c r="E4" s="141" t="s">
-        <v>216</v>
-      </c>
-      <c r="F4" s="141"/>
-      <c r="H4" s="141" t="s">
-        <v>217</v>
-      </c>
-      <c r="I4" s="141"/>
-      <c r="J4" s="141"/>
+      <c r="B4" s="144" t="s">
+        <v>208</v>
+      </c>
+      <c r="C4" s="144"/>
+      <c r="E4" s="144" t="s">
+        <v>209</v>
+      </c>
+      <c r="F4" s="144"/>
+      <c r="H4" s="144" t="s">
+        <v>210</v>
+      </c>
+      <c r="I4" s="144"/>
+      <c r="J4" s="144"/>
     </row>
     <row r="5" spans="2:10">
       <c r="B5" s="76"/>
@@ -6491,16 +7251,16 @@
     </row>
     <row r="6" spans="2:10">
       <c r="B6" s="74" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C6" s="74">
         <v>0.93799999999999994</v>
       </c>
       <c r="E6" s="78" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F6" s="79">
-        <v>19.600000000000001</v>
+        <v>32.5</v>
       </c>
       <c r="H6" s="74" t="s">
         <v>67</v>
@@ -6512,16 +7272,16 @@
     </row>
     <row r="7" spans="2:10">
       <c r="B7" s="75" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C7" s="75">
         <v>25</v>
       </c>
       <c r="E7" s="80" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F7" s="81">
-        <v>5.8</v>
+        <v>11.6</v>
       </c>
       <c r="H7" s="74" t="s">
         <v>68</v>
@@ -6533,17 +7293,17 @@
     </row>
     <row r="8" spans="2:10">
       <c r="B8" s="82" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C8" s="83">
         <f>_xlfn.T.INV(C6,C7)</f>
         <v>1.5917851223801218</v>
       </c>
       <c r="E8" s="84" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="F8" s="85">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="H8" s="74"/>
       <c r="I8" s="32"/>
@@ -6551,7 +7311,7 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" s="82" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C9" s="83">
         <f>ABS(C8)</f>
@@ -6561,10 +7321,10 @@
         <v>20</v>
       </c>
       <c r="F9" s="87">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="H9" s="88" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I9" s="89">
         <f>(I6+I7)/2</f>
@@ -6576,14 +7336,14 @@
       <c r="B10" s="74"/>
       <c r="C10" s="74"/>
       <c r="E10" s="74" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="F10" s="32">
         <f>((100-F8)/100 )/2</f>
-        <v>0.05</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="H10" s="88" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="I10" s="89">
         <f>I7-I9</f>
@@ -6593,37 +7353,37 @@
     </row>
     <row r="11" spans="2:10">
       <c r="B11" s="74" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C11" s="74">
         <v>80</v>
       </c>
       <c r="E11" s="74" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="F11" s="32">
         <f>ABS(_xlfn.T.INV(F10,F9-1))</f>
-        <v>1.7207429028118781</v>
+        <v>2.0226909200367595</v>
       </c>
     </row>
     <row r="12" spans="2:10">
       <c r="B12" s="74" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C12" s="74">
         <v>14</v>
       </c>
       <c r="E12" s="82" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="F12" s="90">
         <f>F6-(F11*(F7/SQRT(F9)))</f>
-        <v>17.472191006648718</v>
+        <v>28.79014002028255</v>
       </c>
     </row>
     <row r="13" spans="2:10">
       <c r="B13" s="74" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C13" s="74">
         <f>((100-C11)/100)/2</f>
@@ -6634,36 +7394,41 @@
       </c>
       <c r="F13" s="90">
         <f>F6+ (F11*(F7/SQRT(F9)))</f>
-        <v>21.727808993351285</v>
+        <v>36.20985997971745</v>
       </c>
     </row>
     <row r="14" spans="2:10">
       <c r="B14" s="82" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C14" s="83">
         <f>ABS(_xlfn.T.INV(C13,C12))</f>
         <v>1.3450303744546506</v>
       </c>
       <c r="H14" t="s">
-        <v>228</v>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="E15" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="16" spans="2:10">
       <c r="H16" s="32" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="I16" s="32">
         <v>23.86</v>
       </c>
     </row>
     <row r="17" spans="2:9">
-      <c r="B17" s="141" t="s">
-        <v>230</v>
-      </c>
-      <c r="C17" s="141"/>
+      <c r="B17" s="144" t="s">
+        <v>223</v>
+      </c>
+      <c r="C17" s="144"/>
       <c r="H17" s="32" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="I17" s="32">
         <v>2.9000000000000001E-2</v>
@@ -6673,7 +7438,7 @@
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
       <c r="H18" s="32" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="I18" s="32">
         <v>95</v>
@@ -6681,7 +7446,7 @@
     </row>
     <row r="19" spans="2:9">
       <c r="B19" s="74" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C19" s="74">
         <v>4</v>
@@ -6695,7 +7460,7 @@
     </row>
     <row r="20" spans="2:9">
       <c r="B20" s="74" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="C20" s="74">
         <v>99</v>
@@ -6709,7 +7474,7 @@
     </row>
     <row r="21" spans="2:9">
       <c r="B21" s="74" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="C21" s="74">
         <v>15.4</v>
@@ -6721,7 +7486,7 @@
       <c r="B22" s="74"/>
       <c r="C22" s="74"/>
       <c r="H22" s="89" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="I22" s="89">
         <f>I20-I16</f>
@@ -6730,19 +7495,19 @@
     </row>
     <row r="23" spans="2:9">
       <c r="B23" s="74" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C23" s="74">
         <f>((100-C20)/100 )/2</f>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="H23" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="2:9">
       <c r="B24" s="74" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C24" s="91">
         <f>_xlfn.NORM.INV(1-C23,0,1)</f>
@@ -6762,7 +7527,7 @@
         <v>98.345754868636917</v>
       </c>
       <c r="D26" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -6780,7 +7545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74898097-6201-8D4A-AA45-F89B2A2E7762}">
   <dimension ref="A2:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="94" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -6792,7 +7557,7 @@
   <sheetData>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -6800,7 +7565,7 @@
         <v>30120</v>
       </c>
       <c r="C3" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -6811,7 +7576,7 @@
         <v>30415</v>
       </c>
       <c r="C4" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="D4">
         <v>6000</v>
@@ -6822,7 +7587,7 @@
         <v>30729</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D5">
         <v>30000</v>
@@ -6833,16 +7598,16 @@
         <v>32114</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="D6" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="E6" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="F6" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6929,8 +7694,8 @@
       <c r="A11" s="7">
         <v>34676</v>
       </c>
-      <c r="D11" s="145" t="s">
-        <v>287</v>
+      <c r="D11" s="142" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -6948,7 +7713,7 @@
         <v>35576</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="F14">
         <f>COUNT(A3:A27)</f>
@@ -7027,271 +7792,343 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A47A757-16BD-0749-9653-C8284C431BBD}">
-  <dimension ref="A2:D42"/>
+  <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="62" workbookViewId="0">
+      <selection activeCell="Y22" sqref="Y22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.33203125" customWidth="1"/>
+    <col min="23" max="23" width="18.6640625" customWidth="1"/>
+    <col min="24" max="25" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="1" spans="1:25">
+      <c r="W1" t="s">
+        <v>89</v>
+      </c>
+      <c r="X1">
+        <f>AVERAGE(X11:X19)</f>
+        <v>72.444444444444443</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>275</v>
+      </c>
+      <c r="W2" t="s">
+        <v>305</v>
+      </c>
+      <c r="X2">
+        <f>_xlfn.STDEV.P(X11:X19)</f>
+        <v>7.7332056183579176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="17">
       <c r="A3">
-        <v>0.26</v>
+        <v>340</v>
       </c>
       <c r="C3" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="D3">
         <f>COUNT(A3:A202)</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>20</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="W3" t="s">
+        <v>304</v>
+      </c>
+      <c r="X3">
+        <f>_xlfn.STDEV.S(X11:X19)</f>
+        <v>8.2023031995761642</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="17">
       <c r="A4">
-        <v>0.47</v>
+        <v>390</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D4">
         <f>AVERAGE(A3:A200)</f>
-        <v>5.6750000000000002E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>432.9</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="W4" t="s">
+        <v>303</v>
+      </c>
+      <c r="X4">
+        <f>AVERAGE(Y11:Y19)</f>
+        <v>1.8503717077085943E-16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5">
-        <v>-0.05</v>
+        <v>408</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D5">
+        <v>127</v>
+      </c>
+      <c r="D5" s="141">
         <f>STDEV(A3:A220)</f>
-        <v>0.11958019517011616</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>76.226739333869418</v>
+      </c>
+      <c r="G5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
       <c r="A6">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7">
-        <v>0.01</v>
+        <v>338</v>
       </c>
       <c r="C7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D7" s="5">
-        <f>QUARTILE(A$3:A$22, 1)</f>
-        <v>-1.2500000000000001E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <f>QUARTILE(A3:A22,1)</f>
+        <v>365.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8">
-        <v>0.26</v>
+        <v>441</v>
       </c>
       <c r="C8" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="D8">
         <f>QUARTILE(A$3:A$22, 2)</f>
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9">
-        <v>0.06</v>
+        <v>415</v>
       </c>
       <c r="C9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" s="144">
-        <f>QUARTILE(A$3:A$22, 3)</f>
-        <v>0.10250000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>148</v>
+      </c>
+      <c r="D9" s="141">
+        <f>QUARTILE(A3:A22,3)</f>
+        <v>500.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
       <c r="A10">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>373</v>
+      </c>
+      <c r="W10" t="s">
+        <v>290</v>
+      </c>
+      <c r="X10" t="s">
+        <v>291</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
       <c r="A11">
-        <v>-0.01</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>522</v>
+      </c>
+      <c r="C11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D11" s="146">
+        <f>D9-D7</f>
+        <v>135</v>
+      </c>
+      <c r="W11" t="s">
+        <v>292</v>
+      </c>
+      <c r="X11">
+        <v>77</v>
+      </c>
+      <c r="Y11">
+        <f>(X11-X$1)/X$2</f>
+        <v>0.58909018851653028</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
       <c r="A12">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>343</v>
+      </c>
+      <c r="W12" t="s">
+        <v>293</v>
+      </c>
+      <c r="X12">
+        <v>60</v>
+      </c>
+      <c r="Y12">
+        <f>(X12-X$1)/X$2</f>
+        <v>-1.6092219783866186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
       <c r="A13">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>527</v>
+      </c>
+      <c r="W13" t="s">
+        <v>294</v>
+      </c>
+      <c r="X13">
+        <v>60</v>
+      </c>
+      <c r="Y13">
+        <f>(X13-X$1)/X$2</f>
+        <v>-1.6092219783866186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
       <c r="A14">
-        <v>-0.15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>337</v>
+      </c>
+      <c r="W14" t="s">
+        <v>295</v>
+      </c>
+      <c r="X14">
+        <v>81</v>
+      </c>
+      <c r="Y14">
+        <f>(X14-X$1)/X$2</f>
+        <v>1.1063401101408006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
       <c r="A15">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>547</v>
+      </c>
+      <c r="W15" t="s">
+        <v>296</v>
+      </c>
+      <c r="X15">
+        <v>73</v>
+      </c>
+      <c r="Y15">
+        <f>(X15-X$1)/X$2</f>
+        <v>7.1840266892259974E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
       <c r="A16">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>406</v>
+      </c>
+      <c r="G16" t="s">
+        <v>286</v>
+      </c>
+      <c r="W16" t="s">
+        <v>297</v>
+      </c>
+      <c r="X16">
+        <v>80</v>
+      </c>
+      <c r="Y16">
+        <f>(X16-X$1)/X$2</f>
+        <v>0.97702762973473312</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25">
       <c r="A17">
-        <v>-0.11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+        <v>447</v>
+      </c>
+      <c r="G17" t="s">
+        <v>285</v>
+      </c>
+      <c r="W17" t="s">
+        <v>298</v>
+      </c>
+      <c r="X17">
+        <v>80</v>
+      </c>
+      <c r="Y17">
+        <f>(X17-X$1)/X$2</f>
+        <v>0.97702762973473312</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="17">
       <c r="A18">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
+        <v>431</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="W18" t="s">
+        <v>299</v>
+      </c>
+      <c r="X18">
+        <v>68</v>
+      </c>
+      <c r="Y18">
+        <f>(X18-X$1)/X$2</f>
+        <v>-0.57472213513807791</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" ht="17">
       <c r="A19">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
+        <v>517</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="W19" t="s">
+        <v>300</v>
+      </c>
+      <c r="X19">
+        <v>73</v>
+      </c>
+      <c r="Y19">
+        <f>(X19-X$1)/X$2</f>
+        <v>7.1840266892259974E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" ht="17">
       <c r="A20">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
+        <v>560</v>
+      </c>
+      <c r="G20" s="15"/>
+    </row>
+    <row r="21" spans="1:25" ht="17">
       <c r="A21">
-        <v>-0.05</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
+        <v>339</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="Y21">
+        <f>SUM(Y11:Y19)</f>
+        <v>1.6653345369377348E-15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
       <c r="A22">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28">
-        <v>-0.04</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31">
-        <v>-0.1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33">
-        <v>-0.04</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35">
-        <v>-0.08</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42">
-        <v>0.03</v>
+        <v>495</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFCA351-70B0-5244-BA65-285CF6942DC3}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="159" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -7299,164 +8136,193 @@
   <cols>
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
     <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:13">
       <c r="A1" s="25" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C1" t="s">
         <v>43</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>173</v>
+      </c>
+      <c r="L1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17">
       <c r="A2" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="16">
-        <v>150.9</v>
+        <v>123</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="L2" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="M2">
+        <v>240000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17">
       <c r="A3" s="16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B3" s="54">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F3">
         <f>F2/100</f>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="L3" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="M3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17">
       <c r="A4" s="16" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B4" s="16">
-        <v>35</v>
+        <v>119</v>
       </c>
       <c r="E4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F4">
         <v>300</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="L4" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="M4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="B5" s="16"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:13">
       <c r="A6" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B6" s="52">
         <f>B2</f>
-        <v>150.9</v>
+        <v>123</v>
       </c>
       <c r="E6" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F6" s="53">
         <f>F3</f>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="L6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6">
+        <f>M3 *SQRT(M4)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="16" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B7" s="56">
         <f>B3/SQRT(B4)</f>
-        <v>5.5780180812082092</v>
+        <v>1.0083683467310325</v>
       </c>
       <c r="E7" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F7" s="53">
         <f>SQRT(F6*(1 - F6)/F4)</f>
         <v>1.2583057392117916E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:13">
       <c r="B8" s="16"/>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="16" t="s">
-        <v>172</v>
+    <row r="9" spans="1:13">
+      <c r="A9" s="25" t="s">
+        <v>334</v>
       </c>
       <c r="B9" s="16">
-        <v>180</v>
+        <v>119</v>
       </c>
       <c r="E9" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F9" s="53">
         <f>(F4*F6)*(1 - F6)</f>
         <v>14.25</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:13">
       <c r="A10" s="16" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B10" s="55">
         <f>(B9-B2)/B3</f>
-        <v>0.88181818181818161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>-0.36363636363636365</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="16" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B11" s="57">
         <f>(B9-B2)/B7</f>
-        <v>5.2169067178242061</v>
+        <v>-3.9668044053220779</v>
       </c>
       <c r="E11" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="F11">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:13">
       <c r="E12" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F12">
         <f>F11/100</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:13">
       <c r="A13" s="16" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B13">
         <f>_xlfn.NORM.S.DIST(B10, TRUE)</f>
-        <v>0.81106243112708065</v>
+        <v>0.35806478442778267</v>
       </c>
       <c r="E13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F13">
         <f>(F12-F6)/F7</f>
@@ -7469,16 +8335,16 @@
         <v>0.79341189999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:13" ht="17">
       <c r="A14" s="16" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B14" s="58">
         <f xml:space="preserve"> 1-B13</f>
-        <v>0.18893756887291935</v>
+        <v>0.64193521557221733</v>
       </c>
       <c r="E14" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="F14" s="53">
         <f>_xlfn.NORM.S.DIST(F13, TRUE)</f>
@@ -7490,10 +8356,13 @@
       <c r="I14">
         <v>0.70731049999999995</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="L14" s="15" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="17">
       <c r="E15" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F15" s="53">
         <f xml:space="preserve"> 1 - F14</f>
@@ -7503,28 +8372,34 @@
         <f>I13-I14</f>
         <v>8.6101399999999995E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="L15" s="15" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="17">
       <c r="A16" s="16" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B16" s="52">
         <f>_xlfn.NORM.S.DIST(B11, TRUE)</f>
-        <v>0.99999990903208769</v>
+        <v>3.6421361779336248E-5</v>
+      </c>
+      <c r="L16" s="15" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="16" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B17" s="52">
         <f xml:space="preserve"> 1 -B16</f>
-        <v>9.0967912313999477E-8</v>
+        <v>0.99996357863822072</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="25" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B20" s="16"/>
     </row>
@@ -7533,7 +8408,7 @@
         <v>67</v>
       </c>
       <c r="B21" s="16">
-        <v>120</v>
+        <v>87.75</v>
       </c>
       <c r="E21">
         <v>0.174543</v>
@@ -7544,7 +8419,7 @@
         <v>68</v>
       </c>
       <c r="B22" s="16">
-        <v>180</v>
+        <v>90.65</v>
       </c>
       <c r="E22">
         <v>0.81106243</v>
@@ -7552,18 +8427,18 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="16" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B23">
         <f>(B21-B$6)/B$7</f>
-        <v>-5.539601978720551</v>
+        <v>-34.957463821900809</v>
       </c>
       <c r="E23">
         <f>E22-E21</f>
         <v>0.63651943</v>
       </c>
       <c r="F23" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -7572,16 +8447,26 @@
       </c>
       <c r="B24">
         <f>(B22-B$6)/B$7</f>
-        <v>5.2169067178242061</v>
+        <v>-32.081530628042302</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="16" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B26" s="53">
         <f>_xlfn.NORM.S.DIST(B24, TRUE) - _xlfn.NORM.S.DIST(B23, TRUE)</f>
-        <v>0.99999989387409427</v>
+        <v>3.9897916573105739E-226</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="255">
+      <c r="A28" s="147" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -7592,10 +8477,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74F7077-45B6-E742-951B-BF30C929E163}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7728,7 +8613,13 @@
         <v>65</v>
       </c>
     </row>
+    <row r="22" spans="1:1" ht="17">
+      <c r="A22" s="15" t="s">
+        <v>346</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add final notes and formulas
</commit_message>
<xml_diff>
--- a/Midterm Excel Sheet.xlsx
+++ b/Midterm Excel Sheet.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanninoa/Desktop/wednesday/Statistics-Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504B0DF5-DD22-F843-8072-C13957891763}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE9A8A2-AF24-C542-9FE7-E6CF10209A72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20300" yWindow="460" windowWidth="12920" windowHeight="18740" activeTab="1" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
+    <workbookView xWindow="17620" yWindow="460" windowWidth="12920" windowHeight="18740" activeTab="1" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
   </bookViews>
   <sheets>
     <sheet name="Random Variable x" sheetId="1" r:id="rId1"/>
-    <sheet name="Chpater 10" sheetId="11" r:id="rId2"/>
+    <sheet name="Chapter 10" sheetId="11" r:id="rId2"/>
     <sheet name="Normal Distribution - Z-score" sheetId="6" r:id="rId3"/>
     <sheet name="Chapter 9" sheetId="9" r:id="rId4"/>
     <sheet name="t-values" sheetId="10" r:id="rId5"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="386">
   <si>
     <t>x</t>
   </si>
@@ -1174,6 +1174,9 @@
     <t>Suppose the lengths of the pregnancies of a certain animal are approximately normally distributed with mean μ=123 days and standard deviation sigma = 11 days.</t>
   </si>
   <si>
+    <t>x bar</t>
+  </si>
+  <si>
     <t>mean of x bar</t>
   </si>
   <si>
@@ -1273,6 +1276,60 @@
   </si>
   <si>
     <t xml:space="preserve">Population Proportion (Left/Right-Tailed Test) &lt; or &gt; </t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>reject?</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>Construct confidence interval</t>
+  </si>
+  <si>
+    <t>A golf association requires that golf balls have a diameter that is 1.68 inches. To determine if golf balls conform to the​ standard, a random sample of golf balls was selected. Their diameters are shown in the accompanying data table. Do the golf balls conform to the​ standards? Use the alphaαequals=0.050.05 level of significanc.</t>
+  </si>
+  <si>
+    <t>level of significance (alpha)</t>
+  </si>
+  <si>
+    <t>mean (u0) - given</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t0 </t>
+  </si>
+  <si>
+    <t>p-val</t>
+  </si>
+  <si>
+    <t>use this then go to chapter 9, using mean and s</t>
+  </si>
+  <si>
+    <t>can be from ch 10</t>
+  </si>
+  <si>
+    <t>confidence interval %</t>
+  </si>
+  <si>
+    <t>t(a/2)</t>
+  </si>
+  <si>
+    <t>upperbound</t>
+  </si>
+  <si>
+    <t>Look @ video</t>
+  </si>
+  <si>
+    <t>x (mean)</t>
+  </si>
+  <si>
+    <t>^^ change to 1 or 2 depending on tail</t>
+  </si>
+  <si>
+    <t>reject (P&lt;a)?</t>
   </si>
 </sst>
 </file>
@@ -1808,7 +1865,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2121,9 +2178,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2195,16 +2255,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>20158</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>120952</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>886984</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>161270</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>120145</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>96422</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>523320</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>136739</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2227,7 +2287,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17054285" y="4152698"/>
+          <a:off x="19110476" y="7821587"/>
           <a:ext cx="10058400" cy="1588168"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5191,10 +5251,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5B9FCC-C544-FD4E-85A9-D1AE64548C87}">
-  <dimension ref="A3:V75"/>
+  <dimension ref="A3:AB75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="U36" sqref="U36"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="67" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5206,11 +5266,13 @@
     <col min="7" max="7" width="28" customWidth="1"/>
     <col min="10" max="10" width="27.83203125" customWidth="1"/>
     <col min="11" max="11" width="11.83203125" customWidth="1"/>
-    <col min="15" max="15" width="13.1640625" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" customWidth="1"/>
     <col min="20" max="20" width="19.83203125" customWidth="1"/>
+    <col min="26" max="26" width="25.33203125" customWidth="1"/>
+    <col min="27" max="27" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:22">
+    <row r="3" spans="2:28">
       <c r="B3" s="143">
         <v>10.199999999999999</v>
       </c>
@@ -5220,13 +5282,13 @@
       <c r="F3" s="143"/>
       <c r="G3" s="143"/>
     </row>
-    <row r="5" spans="2:22">
+    <row r="5" spans="2:28">
       <c r="B5" s="144" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C5" s="144"/>
       <c r="F5" s="144" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="G5" s="144"/>
       <c r="J5" s="140" t="s">
@@ -5234,10 +5296,13 @@
       </c>
       <c r="K5" s="140"/>
       <c r="N5" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="6" spans="2:22">
+        <v>354</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="6" spans="2:28">
       <c r="B6" s="76"/>
       <c r="C6" s="94"/>
       <c r="F6" s="76"/>
@@ -5245,27 +5310,36 @@
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
       <c r="N6" s="32" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="O6" s="32" t="s">
-        <v>0</v>
+        <v>383</v>
       </c>
       <c r="P6" s="32">
-        <v>400</v>
+        <v>88.1</v>
       </c>
       <c r="T6" s="98" t="s">
         <v>251</v>
       </c>
       <c r="U6" s="98">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="2:22">
+        <v>1.68</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>275</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:28">
       <c r="B7" s="84" t="s">
         <v>229</v>
       </c>
       <c r="C7" s="85">
-        <v>0.1</v>
+        <v>0.86</v>
       </c>
       <c r="F7" s="84" t="s">
         <v>229</v>
@@ -5280,7 +5354,7 @@
         <v>13</v>
       </c>
       <c r="N7" s="32">
-        <v>310</v>
+        <v>109</v>
       </c>
       <c r="O7" s="32" t="s">
         <v>20</v>
@@ -5292,10 +5366,19 @@
         <v>252</v>
       </c>
       <c r="U7" s="98">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:22">
+        <v>1.681</v>
+      </c>
+      <c r="Z7">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>374</v>
+      </c>
+      <c r="AB7">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28">
       <c r="B8" s="78" t="s">
         <v>190</v>
       </c>
@@ -5303,10 +5386,10 @@
         <v>200</v>
       </c>
       <c r="F8" s="86" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="G8" s="87">
-        <v>400</v>
+        <v>893</v>
       </c>
       <c r="J8" s="114" t="s">
         <v>20</v>
@@ -5315,23 +5398,33 @@
         <v>48</v>
       </c>
       <c r="N8" s="32">
-        <v>311</v>
+        <v>67.3</v>
       </c>
       <c r="O8" s="32" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="P8" s="32">
         <f>AVERAGE(N7:N100)</f>
-        <v>365.2</v>
+        <v>79</v>
       </c>
       <c r="T8" s="98" t="s">
         <v>253</v>
       </c>
       <c r="U8">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="9" spans="2:22">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Z8">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>337</v>
+      </c>
+      <c r="AB8">
+        <f>AVERAGE(Z7:Z18)</f>
+        <v>0.15150000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="2:28">
       <c r="B9" s="86" t="s">
         <v>0</v>
       </c>
@@ -5339,10 +5432,10 @@
         <v>26</v>
       </c>
       <c r="F9" s="95" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="G9" s="96">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="J9" s="114" t="s">
         <v>242</v>
@@ -5351,23 +5444,32 @@
         <v>57</v>
       </c>
       <c r="N9" s="32">
-        <v>412</v>
-      </c>
-      <c r="O9" s="158" t="s">
-        <v>355</v>
+        <v>56.1</v>
+      </c>
+      <c r="O9" s="160" t="s">
+        <v>356</v>
       </c>
       <c r="P9" s="32">
         <f>P6</f>
-        <v>400</v>
+        <v>88.1</v>
       </c>
       <c r="T9" s="98" t="s">
         <v>20</v>
       </c>
       <c r="U9" s="98">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="10" spans="2:22">
+        <v>12</v>
+      </c>
+      <c r="Z9">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>373</v>
+      </c>
+      <c r="AB9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:28">
       <c r="B10" s="97" t="s">
         <v>211</v>
       </c>
@@ -5387,18 +5489,32 @@
         <v>39</v>
       </c>
       <c r="N10" s="32">
-        <v>368</v>
-      </c>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
+        <v>73.900000000000006</v>
+      </c>
+      <c r="O10" s="32" t="s">
+        <v>370</v>
+      </c>
+      <c r="P10" s="32">
+        <v>0.05</v>
+      </c>
       <c r="T10" s="98" t="s">
         <v>211</v>
       </c>
       <c r="U10" s="98">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="11" spans="2:22">
+      <c r="Z10">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>224</v>
+      </c>
+      <c r="AB10">
+        <f>_xlfn.STDEV.S(Z7:Z18)</f>
+        <v>9.2308961885856147E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:28">
       <c r="B11" s="74" t="s">
         <v>230</v>
       </c>
@@ -5408,25 +5524,28 @@
       <c r="F11" s="74" t="s">
         <v>230</v>
       </c>
-      <c r="G11" s="74">
-        <v>0.01</v>
+      <c r="G11" s="74" t="s">
+        <v>231</v>
       </c>
       <c r="J11" s="118"/>
       <c r="K11" s="119"/>
       <c r="N11" s="32">
-        <v>447</v>
+        <v>66.3</v>
       </c>
       <c r="O11" s="32" t="s">
         <v>253</v>
       </c>
       <c r="P11" s="32">
-        <f>_xlfn.STDEV.S(N7:N16)</f>
-        <v>48.416709695907549</v>
+        <f>_xlfn.STDEV.S(N7:N20)</f>
+        <v>15.214101645805059</v>
       </c>
       <c r="T11" s="32"/>
       <c r="U11" s="32"/>
-    </row>
-    <row r="12" spans="2:22">
+      <c r="Z11">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="12" spans="2:28">
       <c r="B12" s="32"/>
       <c r="C12" s="32"/>
       <c r="F12" s="32"/>
@@ -5439,7 +5558,7 @@
         <v>11.764800000000001</v>
       </c>
       <c r="N12" s="32">
-        <v>376</v>
+        <v>82.3</v>
       </c>
       <c r="O12" s="32"/>
       <c r="P12" s="32"/>
@@ -5448,23 +5567,33 @@
       </c>
       <c r="U12" s="134" t="str">
         <f>IF(U9&gt;=30, "Yes", "No")</f>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="13" spans="2:22">
+        <v>No</v>
+      </c>
+      <c r="Z12">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="AA12" s="156" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB12" s="156">
+        <f>(AB8-AB7)/(AB10/SQRT(AB6))</f>
+        <v>5.6290877034582951E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:28">
       <c r="B13" s="99" t="s">
         <v>232</v>
       </c>
       <c r="C13" s="100">
         <f>C8*C7*(1-C7)</f>
-        <v>18</v>
+        <v>24.080000000000002</v>
       </c>
       <c r="F13" s="99" t="s">
         <v>232</v>
       </c>
       <c r="G13" s="101">
         <f>G9*G7*(1-G7)</f>
-        <v>1.204</v>
+        <v>120.4</v>
       </c>
       <c r="J13" s="123" t="s">
         <v>189</v>
@@ -5474,19 +5603,22 @@
         <v>1</v>
       </c>
       <c r="N13" s="32">
-        <v>303</v>
-      </c>
-      <c r="O13" s="156" t="s">
-        <v>356</v>
+        <v>93</v>
+      </c>
+      <c r="O13" s="158" t="s">
+        <v>357</v>
       </c>
       <c r="P13" s="136">
         <f>(P8-P9)/(P11/SQRT(P7))</f>
-        <v>-2.2729190658563367</v>
+        <v>-1.8914509300302171</v>
       </c>
       <c r="T13" s="32"/>
       <c r="U13" s="32"/>
-    </row>
-    <row r="14" spans="2:22">
+      <c r="Z13">
+        <v>0.112</v>
+      </c>
+    </row>
+    <row r="14" spans="2:28">
       <c r="B14" s="82" t="s">
         <v>233</v>
       </c>
@@ -5499,28 +5631,38 @@
       </c>
       <c r="G14" s="82" t="b">
         <f>IF(G13&gt;=10, TRUE, FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="124"/>
       <c r="K14" s="94"/>
       <c r="N14" s="32">
-        <v>410</v>
+        <v>85.5</v>
       </c>
       <c r="O14" s="32" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="P14" s="32" t="s">
         <v>43</v>
       </c>
       <c r="T14" s="135" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="U14" s="135">
         <f>(U7-U6)/ (U8/SQRT(U9))</f>
-        <v>1.2162606385263026</v>
-      </c>
-    </row>
-    <row r="15" spans="2:22">
+        <v>0.86602540378453552</v>
+      </c>
+      <c r="Z14">
+        <v>0.214</v>
+      </c>
+      <c r="AA14" s="157" t="s">
+        <v>376</v>
+      </c>
+      <c r="AB14" s="131">
+        <f>TDIST(ABS(AB12),AB6-1,2)</f>
+        <v>0.95611954878067607</v>
+      </c>
+    </row>
+    <row r="15" spans="2:28">
       <c r="B15" s="74"/>
       <c r="C15" s="32"/>
       <c r="F15" s="74"/>
@@ -5533,22 +5675,37 @@
         <v>0.27083333333333331</v>
       </c>
       <c r="N15" s="32">
-        <v>365</v>
-      </c>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
+        <v>71.8</v>
+      </c>
+      <c r="O15" s="136" t="s">
+        <v>368</v>
+      </c>
+      <c r="P15" s="136">
+        <f>TDIST(ABS(P13),P7-1, 2)</f>
+        <v>9.1124762650744345E-2</v>
+      </c>
       <c r="T15" s="136" t="s">
         <v>255</v>
       </c>
       <c r="U15" s="131">
         <f>TDIST(ABS(U14),U9-1,1)</f>
-        <v>0.11251867808518326</v>
+        <v>0.20248476225385775</v>
       </c>
       <c r="V15" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="16" spans="2:22">
+        <v>362</v>
+      </c>
+      <c r="Z15">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>369</v>
+      </c>
+      <c r="AB15" t="b">
+        <f>AB14&gt;=AB9</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28">
       <c r="B16" s="103" t="s">
         <v>234</v>
       </c>
@@ -5557,23 +5714,28 @@
         <v>0.13</v>
       </c>
       <c r="F16" s="74" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="G16" s="32">
         <f>G8/G9</f>
-        <v>40</v>
+        <v>0.89300000000000002</v>
       </c>
       <c r="J16" s="74" t="s">
         <v>245</v>
       </c>
       <c r="K16" s="32"/>
       <c r="N16" s="32">
-        <v>350</v>
+        <v>84.8</v>
       </c>
       <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-    </row>
-    <row r="17" spans="2:21">
+      <c r="P16" s="32" t="s">
+        <v>384</v>
+      </c>
+      <c r="Z16">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28">
       <c r="B17" s="40"/>
       <c r="C17" s="105"/>
       <c r="F17" s="106" t="s">
@@ -5581,10 +5743,18 @@
       </c>
       <c r="G17" s="107">
         <f>(G16-G7)/SQRT((G7*(1-G7))/G9)</f>
-        <v>356.70367016004735</v>
+        <v>3.0074657933780204</v>
       </c>
       <c r="J17" s="74"/>
       <c r="K17" s="126"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="161" t="s">
+        <v>385</v>
+      </c>
+      <c r="P17" s="32" t="b">
+        <f>P15 &lt;= P10</f>
+        <v>0</v>
+      </c>
       <c r="T17" s="137" t="s">
         <v>256</v>
       </c>
@@ -5592,14 +5762,20 @@
         <f>IF(U15&gt;U10, "Do not reject", "Reject")</f>
         <v>Do not reject</v>
       </c>
-    </row>
-    <row r="18" spans="2:21">
+      <c r="AA17" t="s">
+        <v>379</v>
+      </c>
+      <c r="AB17">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="2:28">
       <c r="B18" s="106" t="s">
         <v>235</v>
       </c>
       <c r="C18" s="108">
         <f>(C16-C7)/SQRT((C7*(1-C7))/C8)</f>
-        <v>1.4142135623730949</v>
+        <v>-29.752578826781615</v>
       </c>
       <c r="D18" t="s">
         <v>236</v>
@@ -5613,8 +5789,18 @@
         <f>_xlfn.BINOM.DIST(K10-1,K8,K9/100,TRUE)</f>
         <v>0.99964533162387259</v>
       </c>
-    </row>
-    <row r="19" spans="2:21">
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="AA18" t="s">
+        <v>193</v>
+      </c>
+      <c r="AB18">
+        <f>AB9/2</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="2:28">
       <c r="B19" s="74"/>
       <c r="C19" s="32"/>
       <c r="F19" s="109" t="s">
@@ -5622,7 +5808,7 @@
       </c>
       <c r="G19" s="110">
         <f>TDIST(ABS(G17),G9-1,2)</f>
-        <v>5.4447377312745193E-20</v>
+        <v>2.7003156702174892E-3</v>
       </c>
       <c r="J19" s="130" t="s">
         <v>248</v>
@@ -5631,20 +5817,33 @@
         <f>1-K18</f>
         <v>3.5466837612740942E-4</v>
       </c>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
       <c r="T19" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="20" spans="2:21">
+        <v>363</v>
+      </c>
+      <c r="U19" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>380</v>
+      </c>
+      <c r="AB19">
+        <f>ABS(_xlfn.T.INV(AB18,AB6-1))</f>
+        <v>1.7958848187040437</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28">
       <c r="B20" s="109" t="s">
         <v>237</v>
       </c>
       <c r="C20" s="111">
         <f>TDIST(ABS(C18),C8-1,1)</f>
-        <v>7.9430911180115582E-2</v>
+        <v>1.7232439145239769E-75</v>
       </c>
       <c r="F20" s="155" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="J20" s="132" t="s">
         <v>250</v>
@@ -5653,33 +5852,62 @@
         <f>_xlfn.BINOM.DIST(K10,K8,K9/100,TRUE)</f>
         <v>0.99989936814098268</v>
       </c>
-    </row>
-    <row r="21" spans="2:21">
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+    </row>
+    <row r="21" spans="2:28">
       <c r="B21" s="112" t="s">
         <v>238</v>
       </c>
       <c r="C21" s="113" t="str">
         <f>IF(C20&gt;C10, "P &gt; a", "P &lt; a")</f>
-        <v>P &gt; a</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21">
+        <v>P &lt; a</v>
+      </c>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="AA21" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB21">
+        <f>AB$8 - AB$19*AB$10/SQRT(AB$6)</f>
+        <v>0.10364451488469201</v>
+      </c>
+    </row>
+    <row r="22" spans="2:28">
       <c r="B22" s="32"/>
       <c r="C22" s="115" t="str">
         <f>IF(C21="P &gt; a", "DON'T REJECT", "REJECT")</f>
-        <v>DON'T REJECT</v>
+        <v>REJECT</v>
       </c>
       <c r="D22" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="24" spans="2:21">
+      <c r="AA22" t="s">
+        <v>381</v>
+      </c>
+      <c r="AB22">
+        <f>AB$8 + AB$19*AB$10/SQRT(AB$6)</f>
+        <v>0.19935548511530804</v>
+      </c>
+    </row>
+    <row r="24" spans="2:28" ht="17">
       <c r="B24" s="144" t="s">
         <v>239</v>
       </c>
       <c r="C24" s="144"/>
-    </row>
-    <row r="25" spans="2:21">
+      <c r="O24" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="P24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" ht="17">
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
       <c r="F25" s="112" t="s">
@@ -5689,8 +5917,9 @@
         <f>IF(G19&gt;G10, "P &gt; a", "P &lt; a")</f>
         <v>P &lt; a</v>
       </c>
-    </row>
-    <row r="26" spans="2:21">
+      <c r="O25" s="15"/>
+    </row>
+    <row r="26" spans="2:28" ht="17">
       <c r="B26" s="85" t="s">
         <v>0</v>
       </c>
@@ -5701,24 +5930,27 @@
         <f>IF(G25="P &gt; a", "DON'T REJECT NULL HYPOTHESIS", "REJECT NULL HYPOTHESIS")</f>
         <v>REJECT NULL HYPOTHESIS</v>
       </c>
-    </row>
-    <row r="27" spans="2:21">
+      <c r="O26" s="15"/>
+    </row>
+    <row r="27" spans="2:28" ht="17">
       <c r="B27" s="116" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="116">
         <v>1195</v>
       </c>
-    </row>
-    <row r="28" spans="2:21">
+      <c r="O27" s="15"/>
+    </row>
+    <row r="28" spans="2:28" ht="17">
       <c r="B28" s="79" t="s">
         <v>241</v>
       </c>
       <c r="C28" s="79">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="29" spans="2:21">
+      <c r="O28" s="15"/>
+    </row>
+    <row r="29" spans="2:28">
       <c r="B29" s="117" t="s">
         <v>264</v>
       </c>
@@ -5726,11 +5958,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="2:21">
+    <row r="30" spans="2:28">
       <c r="B30" s="40"/>
       <c r="C30" s="105"/>
     </row>
-    <row r="31" spans="2:21">
+    <row r="31" spans="2:28">
       <c r="B31" s="32" t="s">
         <v>189</v>
       </c>
@@ -5739,11 +5971,11 @@
         <v>4.7608800000000002</v>
       </c>
     </row>
-    <row r="32" spans="2:21">
+    <row r="32" spans="2:28">
       <c r="B32" s="32"/>
       <c r="C32" s="122"/>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:27">
       <c r="B33" s="32" t="s">
         <v>193</v>
       </c>
@@ -5752,7 +5984,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" spans="2:27">
       <c r="B34" s="32" t="s">
         <v>194</v>
       </c>
@@ -5760,12 +5992,15 @@
         <f>_xlfn.NORM.INV((1-C33),0,1)</f>
         <v>2.5758293035488999</v>
       </c>
-    </row>
-    <row r="35" spans="2:4">
+      <c r="AA34" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="35" spans="2:27">
       <c r="B35" s="118"/>
       <c r="C35" s="119"/>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:27">
       <c r="B36" s="125" t="s">
         <v>246</v>
       </c>
@@ -5774,11 +6009,11 @@
         <v>0.41338912133891215</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:27">
       <c r="B37" s="127"/>
       <c r="C37" s="128"/>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="2:27">
       <c r="B38" s="102" t="s">
         <v>195</v>
       </c>
@@ -5787,7 +6022,7 @@
         <v>0.37669574247190074</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="2:27">
       <c r="B39" s="102" t="s">
         <v>68</v>
       </c>
@@ -5799,33 +6034,33 @@
         <v>249</v>
       </c>
     </row>
-    <row r="43" spans="2:4">
+    <row r="43" spans="2:27">
       <c r="B43" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="45" spans="2:27">
       <c r="B45" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="47" spans="2:4">
+    <row r="47" spans="2:27">
       <c r="B47" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="48" spans="2:4">
+    <row r="48" spans="2:27">
       <c r="B48" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="B49" t="s">
+      <c r="B49" s="4" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="B50" t="s">
+      <c r="B50" s="4" t="s">
         <v>259</v>
       </c>
     </row>
@@ -5877,17 +6112,17 @@
     </row>
     <row r="72" spans="2:2" ht="26">
       <c r="B72" s="154" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="74" spans="2:2" ht="17">
       <c r="B74" s="15" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="75" spans="2:2">
       <c r="B75" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -6227,7 +6462,7 @@
       <c r="L6" s="45"/>
       <c r="P6" s="33"/>
       <c r="Q6" s="32"/>
-      <c r="S6" s="157" t="s">
+      <c r="S6" s="159" t="s">
         <v>151</v>
       </c>
       <c r="T6" s="136">
@@ -6292,7 +6527,7 @@
     </row>
     <row r="8" spans="1:35" ht="21" customHeight="1">
       <c r="A8" s="152" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B8" s="2">
         <f>B3</f>
@@ -6313,8 +6548,8 @@
         <f>_xlfn.NORM.DIST(Q5, 0, 1, TRUE)</f>
         <v>0.50797831371690205</v>
       </c>
-      <c r="S8" s="156" t="s">
-        <v>352</v>
+      <c r="S8" s="158" t="s">
+        <v>353</v>
       </c>
       <c r="T8" s="136">
         <f>_xlfn.NORM.INV(0.97, 15, 3)</f>
@@ -6360,7 +6595,7 @@
     </row>
     <row r="10" spans="1:35" ht="17">
       <c r="A10" s="152" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B10" s="2">
         <f>B4/SQRT(B9)</f>
@@ -6710,18 +6945,18 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D68" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
+        <v>346</v>
+      </c>
+      <c r="D69" t="s">
         <v>345</v>
-      </c>
-      <c r="D69" t="s">
-        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -6734,8 +6969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77044CB3-A584-0B47-8E5D-C4DB8D5DE250}">
   <dimension ref="B2:N24"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView topLeftCell="B1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6750,7 +6985,9 @@
       <c r="B2" s="60"/>
       <c r="C2" s="60"/>
       <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="E2" s="60" t="s">
+        <v>378</v>
+      </c>
       <c r="F2" s="60"/>
       <c r="G2" s="60"/>
       <c r="H2" s="60"/>
@@ -6774,7 +7011,7 @@
       <c r="J3" s="60"/>
       <c r="K3" s="60"/>
       <c r="M3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="2:14">
@@ -6821,7 +7058,7 @@
       <c r="J5" s="60"/>
       <c r="K5" s="60"/>
       <c r="M5" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="N5">
         <f>AVERAGE(M15:M24)</f>
@@ -7014,7 +7251,7 @@
       <c r="J14" s="60"/>
       <c r="K14" s="60"/>
       <c r="M14" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="2:14">
@@ -7022,7 +7259,7 @@
         <v>197</v>
       </c>
       <c r="C15" s="61">
-        <v>0.05</v>
+        <v>0.98</v>
       </c>
       <c r="D15" s="60"/>
       <c r="E15" s="145" t="s">
@@ -7066,7 +7303,7 @@
         <v>201</v>
       </c>
       <c r="C17" s="61">
-        <v>0.51</v>
+        <v>0.15</v>
       </c>
       <c r="D17" s="60"/>
       <c r="E17" s="61"/>
@@ -7133,7 +7370,7 @@
       </c>
       <c r="C20" s="64">
         <f xml:space="preserve"> C17*(1-C17)*((C19/C15)^2)</f>
-        <v>353.59696426240129</v>
+        <v>0.46961321954287938</v>
       </c>
       <c r="D20" s="60"/>
       <c r="E20" s="70" t="s">
@@ -7155,7 +7392,7 @@
       </c>
       <c r="C21" s="64">
         <f>0.25*((C19/C15)^2)</f>
-        <v>353.7384596462598</v>
+        <v>0.92081023439780274</v>
       </c>
       <c r="D21" s="60"/>
       <c r="E21" s="71" t="s">
@@ -7211,8 +7448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7934B88-A85A-EB42-B4EC-BEBEC08109DD}">
   <dimension ref="B4:J26"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="B1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7411,7 +7648,7 @@
     </row>
     <row r="15" spans="2:10">
       <c r="E15" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="16" spans="2:10">
@@ -7449,7 +7686,7 @@
         <v>192</v>
       </c>
       <c r="C19" s="74">
-        <v>4</v>
+        <v>0.89300000000000002</v>
       </c>
       <c r="H19" s="32" t="s">
         <v>67</v>
@@ -7463,7 +7700,7 @@
         <v>226</v>
       </c>
       <c r="C20" s="74">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H20" s="32" t="s">
         <v>68</v>
@@ -7477,7 +7714,7 @@
         <v>224</v>
       </c>
       <c r="C21" s="74">
-        <v>15.4</v>
+        <v>1.96</v>
       </c>
       <c r="H21" s="32"/>
       <c r="I21" s="32"/>
@@ -7499,7 +7736,7 @@
       </c>
       <c r="C23" s="74">
         <f>((100-C20)/100 )/2</f>
-        <v>5.0000000000000001E-3</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="H23" t="s">
         <v>227</v>
@@ -7511,7 +7748,7 @@
       </c>
       <c r="C24" s="91">
         <f>_xlfn.NORM.INV(1-C23,0,1)</f>
-        <v>2.5758293035488999</v>
+        <v>1.9599639845400536</v>
       </c>
     </row>
     <row r="25" spans="2:9">
@@ -7524,7 +7761,7 @@
       </c>
       <c r="C26" s="93">
         <f>((C24*C21)/C19)^2</f>
-        <v>98.345754868636917</v>
+        <v>18.505695292838212</v>
       </c>
       <c r="D26" t="s">
         <v>228</v>
@@ -8615,7 +8852,7 @@
     </row>
     <row r="22" spans="1:1" ht="17">
       <c r="A22" s="15" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add final normal distribution functions
</commit_message>
<xml_diff>
--- a/Midterm Excel Sheet.xlsx
+++ b/Midterm Excel Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanninoa/Desktop/wednesday/Statistics-Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980B00BB-5397-1149-8B6B-10BD23F4859A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346F50BC-948E-0C47-A067-B3FB31A18EAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17620" yWindow="460" windowWidth="12920" windowHeight="18740" activeTab="1" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
+    <workbookView xWindow="17620" yWindow="460" windowWidth="12920" windowHeight="18740" firstSheet="6" activeTab="7" xr2:uid="{34D5F05A-A698-714B-8EF6-AC36EAC16669}"/>
   </bookViews>
   <sheets>
     <sheet name="Random Variable x" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="t-values" sheetId="10" r:id="rId5"/>
     <sheet name="Histogram" sheetId="13" r:id="rId6"/>
     <sheet name="Quartiles" sheetId="12" r:id="rId7"/>
-    <sheet name="Chapter 8" sheetId="8" r:id="rId8"/>
+    <sheet name="Chapter 8 (also normal)" sheetId="8" r:id="rId8"/>
     <sheet name="Binomial Probability" sheetId="2" r:id="rId9"/>
     <sheet name="x &amp; Probability" sheetId="4" r:id="rId10"/>
     <sheet name="Expected Value" sheetId="5" r:id="rId11"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="397">
   <si>
     <t>x</t>
   </si>
@@ -526,9 +526,6 @@
     <t>mean x bar</t>
   </si>
   <si>
-    <t>x bar SD</t>
-  </si>
-  <si>
     <t>Central limit theorem states that a sample distribution has a normal distribution shape</t>
   </si>
   <si>
@@ -569,12 +566,6 @@
   </si>
   <si>
     <t>proportion</t>
-  </si>
-  <si>
-    <t>mean of p</t>
-  </si>
-  <si>
-    <t>sd of p</t>
   </si>
   <si>
     <t>if &gt; 10, then it's approx. normal</t>
@@ -1331,6 +1322,59 @@
   <si>
     <t>reject (P&lt;a)?</t>
   </si>
+  <si>
+    <t>Q1 - 25th percentile</t>
+  </si>
+  <si>
+    <t>Q3 - 75th percentile</t>
+  </si>
+  <si>
+    <t>Q2 = median - 50th percentile </t>
+  </si>
+  <si>
+    <t>central limit theorem yes if n &gt; 30</t>
+  </si>
+  <si>
+    <t>x bar SD (𝜎𝑋̅)</t>
+  </si>
+  <si>
+    <t>Ex: the upper leg length of 20 to 29 yo males is normally distributaed with a mean and a SD. What is the prob that a randomly slected is less than some number?</t>
+  </si>
+  <si>
+    <t>Normally distributed</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>number i</t>
+  </si>
+  <si>
+    <t>P(x &lt; number i)</t>
+  </si>
+  <si>
+    <t>P(x bar &lt; number I with size n)</t>
+  </si>
+  <si>
+    <r>
+      <t>𝝈</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>𝑿̅</t>
+    </r>
+  </si>
+  <si>
+    <t>sd of p (𝜎𝑝̂)</t>
+  </si>
+  <si>
+    <t>mean of p (𝜇𝑝)</t>
+  </si>
 </sst>
 </file>
 
@@ -1346,7 +1390,7 @@
     <numFmt numFmtId="169" formatCode="0.000"/>
     <numFmt numFmtId="170" formatCode="0.0"/>
     <numFmt numFmtId="171" formatCode="0.00000"/>
-    <numFmt numFmtId="176" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="172" formatCode="0.000000000000000"/>
   </numFmts>
   <fonts count="38">
     <font>
@@ -1865,7 +1909,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2147,16 +2191,7 @@
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2184,6 +2219,16 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2208,6 +2253,99 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1048457</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>200925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8B75028-791F-4048-B8BD-89F1473C3408}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6248400" y="4064000"/>
+          <a:ext cx="3317524" cy="3452125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>16934</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>201552</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>296334</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>59266</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE13808C-6B72-404C-9C5B-4D9014195DCF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6265334" y="7719952"/>
+          <a:ext cx="6273800" cy="3718514"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2300,7 +2438,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2366,7 +2504,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2714,8 +2852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E068083-BD50-CB42-8AAE-F1525497B3A5}">
   <dimension ref="A1:AN226"/>
   <sheetViews>
-    <sheetView topLeftCell="AL1" zoomScale="75" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="C11" zoomScale="75" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4650,6 +4788,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5253,7 +5392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5B9FCC-C544-FD4E-85A9-D1AE64548C87}">
   <dimension ref="A3:AB75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="67" workbookViewId="0">
+    <sheetView zoomScale="67" workbookViewId="0">
       <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
@@ -5273,33 +5412,33 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:28">
-      <c r="B3" s="143">
+      <c r="B3" s="159">
         <v>10.199999999999999</v>
       </c>
-      <c r="C3" s="143"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="143"/>
-      <c r="F3" s="143"/>
-      <c r="G3" s="143"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
     </row>
     <row r="5" spans="2:28">
-      <c r="B5" s="144" t="s">
-        <v>367</v>
-      </c>
-      <c r="C5" s="144"/>
-      <c r="F5" s="144" t="s">
-        <v>366</v>
-      </c>
-      <c r="G5" s="144"/>
+      <c r="B5" s="160" t="s">
+        <v>364</v>
+      </c>
+      <c r="C5" s="160"/>
+      <c r="F5" s="160" t="s">
+        <v>363</v>
+      </c>
+      <c r="G5" s="160"/>
       <c r="J5" s="140" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="K5" s="140"/>
       <c r="N5" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="Z5" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" spans="2:28">
@@ -5310,22 +5449,22 @@
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
       <c r="N6" s="32" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="O6" s="32" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="P6" s="32">
         <v>88.1</v>
       </c>
       <c r="T6" s="98" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="U6" s="98">
         <v>1.68</v>
       </c>
       <c r="Z6" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="AA6" t="s">
         <v>20</v>
@@ -5336,13 +5475,13 @@
     </row>
     <row r="7" spans="2:28">
       <c r="B7" s="84" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C7" s="85">
         <v>0.86</v>
       </c>
       <c r="F7" s="84" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G7" s="85">
         <v>0.86</v>
@@ -5363,7 +5502,7 @@
         <v>10</v>
       </c>
       <c r="T7" s="98" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="U7" s="98">
         <v>1.681</v>
@@ -5372,7 +5511,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="AA7" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="AB7">
         <v>0.15</v>
@@ -5380,13 +5519,13 @@
     </row>
     <row r="8" spans="2:28">
       <c r="B8" s="78" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C8" s="79">
         <v>200</v>
       </c>
       <c r="F8" s="86" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G8" s="87">
         <v>893</v>
@@ -5401,14 +5540,14 @@
         <v>67.3</v>
       </c>
       <c r="O8" s="32" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="P8" s="32">
         <f>AVERAGE(N7:N100)</f>
         <v>79</v>
       </c>
       <c r="T8" s="98" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="U8">
         <v>4.0000000000000001E-3</v>
@@ -5417,7 +5556,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="AA8" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="AB8">
         <f>AVERAGE(Z7:Z18)</f>
@@ -5432,13 +5571,13 @@
         <v>26</v>
       </c>
       <c r="F9" s="95" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G9" s="96">
         <v>1000</v>
       </c>
       <c r="J9" s="114" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="K9" s="115">
         <v>57</v>
@@ -5446,8 +5585,8 @@
       <c r="N9" s="32">
         <v>56.1</v>
       </c>
-      <c r="O9" s="160" t="s">
-        <v>356</v>
+      <c r="O9" s="157" t="s">
+        <v>353</v>
       </c>
       <c r="P9" s="32">
         <f>P6</f>
@@ -5463,7 +5602,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="AA9" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="AB9">
         <v>0.1</v>
@@ -5471,19 +5610,19 @@
     </row>
     <row r="10" spans="2:28">
       <c r="B10" s="97" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C10" s="98">
         <v>0.05</v>
       </c>
       <c r="F10" s="97" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G10" s="98">
         <v>0.05</v>
       </c>
       <c r="J10" s="114" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="K10" s="115">
         <v>39</v>
@@ -5492,13 +5631,13 @@
         <v>73.900000000000006</v>
       </c>
       <c r="O10" s="32" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="P10" s="32">
         <v>0.05</v>
       </c>
       <c r="T10" s="98" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="U10" s="98">
         <v>0.05</v>
@@ -5507,7 +5646,7 @@
         <v>0.27600000000000002</v>
       </c>
       <c r="AA10" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="AB10">
         <f>_xlfn.STDEV.S(Z7:Z18)</f>
@@ -5516,16 +5655,16 @@
     </row>
     <row r="11" spans="2:28">
       <c r="B11" s="74" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C11" s="74" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F11" s="74" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G11" s="74" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="J11" s="118"/>
       <c r="K11" s="119"/>
@@ -5533,7 +5672,7 @@
         <v>66.3</v>
       </c>
       <c r="O11" s="32" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="P11" s="32">
         <f>_xlfn.STDEV.S(N7:N20)</f>
@@ -5551,7 +5690,7 @@
       <c r="F12" s="32"/>
       <c r="G12" s="32"/>
       <c r="J12" s="120" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="K12" s="121">
         <f>K8*(K9/100)*(1-(K9/100))</f>
@@ -5563,7 +5702,7 @@
       <c r="O12" s="32"/>
       <c r="P12" s="32"/>
       <c r="T12" s="31" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="U12" s="134" t="str">
         <f>IF(U9&gt;=30, "Yes", "No")</f>
@@ -5572,31 +5711,31 @@
       <c r="Z12">
         <v>0.17399999999999999</v>
       </c>
-      <c r="AA12" s="156" t="s">
-        <v>375</v>
-      </c>
-      <c r="AB12" s="156">
+      <c r="AA12" s="153" t="s">
+        <v>372</v>
+      </c>
+      <c r="AB12" s="153">
         <f>(AB8-AB7)/(AB10/SQRT(AB6))</f>
         <v>5.6290877034582951E-2</v>
       </c>
     </row>
     <row r="13" spans="2:28">
       <c r="B13" s="99" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C13" s="100">
         <f>C8*C7*(1-C7)</f>
         <v>24.080000000000002</v>
       </c>
       <c r="F13" s="99" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G13" s="101">
         <f>G9*G7*(1-G7)</f>
         <v>120.4</v>
       </c>
       <c r="J13" s="123" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K13" s="123" t="b">
         <f>IF(K12 &gt;= 10, TRUE, FALSE)</f>
@@ -5605,8 +5744,8 @@
       <c r="N13" s="32">
         <v>93</v>
       </c>
-      <c r="O13" s="158" t="s">
-        <v>357</v>
+      <c r="O13" s="155" t="s">
+        <v>354</v>
       </c>
       <c r="P13" s="136">
         <f>(P8-P9)/(P11/SQRT(P7))</f>
@@ -5620,14 +5759,14 @@
     </row>
     <row r="14" spans="2:28">
       <c r="B14" s="82" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C14" s="102" t="b">
         <f>IF(C13&gt;=10, TRUE, FALSE)</f>
         <v>1</v>
       </c>
       <c r="F14" s="82" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G14" s="82" t="b">
         <f>IF(G13&gt;=10, TRUE, FALSE)</f>
@@ -5639,13 +5778,13 @@
         <v>85.5</v>
       </c>
       <c r="O14" s="32" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="P14" s="32" t="s">
         <v>43</v>
       </c>
       <c r="T14" s="135" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="U14" s="135">
         <f>(U7-U6)/ (U8/SQRT(U9))</f>
@@ -5654,8 +5793,8 @@
       <c r="Z14">
         <v>0.214</v>
       </c>
-      <c r="AA14" s="157" t="s">
-        <v>376</v>
+      <c r="AA14" s="154" t="s">
+        <v>373</v>
       </c>
       <c r="AB14" s="131">
         <f>TDIST(ABS(AB12),AB6-1,2)</f>
@@ -5668,7 +5807,7 @@
       <c r="F15" s="74"/>
       <c r="G15" s="32"/>
       <c r="J15" s="74" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="K15" s="32">
         <f>K7/K8</f>
@@ -5678,27 +5817,27 @@
         <v>71.8</v>
       </c>
       <c r="O15" s="136" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="P15" s="136">
         <f>TDIST(ABS(P13),P7-1, 2)</f>
         <v>9.1124762650744345E-2</v>
       </c>
       <c r="T15" s="136" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="U15" s="131">
         <f>TDIST(ABS(U14),U9-1,1)</f>
         <v>0.20248476225385775</v>
       </c>
       <c r="V15" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="Z15">
         <v>0.32400000000000001</v>
       </c>
       <c r="AA15" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="AB15" t="b">
         <f>AB14&gt;=AB9</f>
@@ -5707,21 +5846,21 @@
     </row>
     <row r="16" spans="2:28">
       <c r="B16" s="103" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C16" s="104">
         <f>C9/C8</f>
         <v>0.13</v>
       </c>
       <c r="F16" s="74" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G16" s="32">
         <f>G8/G9</f>
         <v>0.89300000000000002</v>
       </c>
       <c r="J16" s="74" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="K16" s="32"/>
       <c r="N16" s="32">
@@ -5729,7 +5868,7 @@
       </c>
       <c r="O16" s="32"/>
       <c r="P16" s="32" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="Z16">
         <v>9.9000000000000005E-2</v>
@@ -5739,7 +5878,7 @@
       <c r="B17" s="40"/>
       <c r="C17" s="105"/>
       <c r="F17" s="106" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G17" s="107">
         <f>(G16-G7)/SQRT((G7*(1-G7))/G9)</f>
@@ -5748,22 +5887,22 @@
       <c r="J17" s="74"/>
       <c r="K17" s="126"/>
       <c r="N17" s="32"/>
-      <c r="O17" s="161" t="s">
-        <v>385</v>
+      <c r="O17" s="158" t="s">
+        <v>382</v>
       </c>
       <c r="P17" s="32" t="b">
         <f>P15 &lt;= P10</f>
         <v>0</v>
       </c>
       <c r="T17" s="137" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="U17" s="134" t="str">
         <f>IF(U15&gt;U10, "Do not reject", "Reject")</f>
         <v>Do not reject</v>
       </c>
       <c r="AA17" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="AB17">
         <v>98</v>
@@ -5771,19 +5910,19 @@
     </row>
     <row r="18" spans="2:28">
       <c r="B18" s="106" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C18" s="108">
         <f>(C16-C7)/SQRT((C7*(1-C7))/C8)</f>
         <v>-29.752578826781615</v>
       </c>
       <c r="D18" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F18" s="74"/>
       <c r="G18" s="32"/>
       <c r="J18" s="74" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="K18" s="126">
         <f>_xlfn.BINOM.DIST(K10-1,K8,K9/100,TRUE)</f>
@@ -5793,7 +5932,7 @@
       <c r="O18" s="32"/>
       <c r="P18" s="32"/>
       <c r="AA18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="AB18">
         <f>AB9/2</f>
@@ -5804,14 +5943,14 @@
       <c r="B19" s="74"/>
       <c r="C19" s="32"/>
       <c r="F19" s="109" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G19" s="110">
         <f>TDIST(ABS(G17),G9-1,2)</f>
         <v>2.7003156702174892E-3</v>
       </c>
       <c r="J19" s="130" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="K19" s="131">
         <f>1-K18</f>
@@ -5821,13 +5960,13 @@
       <c r="O19" s="32"/>
       <c r="P19" s="32"/>
       <c r="T19" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="U19" t="s">
         <v>43</v>
       </c>
       <c r="AA19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="AB19">
         <f>ABS(_xlfn.T.INV(AB18,AB6-1))</f>
@@ -5836,17 +5975,17 @@
     </row>
     <row r="20" spans="2:28">
       <c r="B20" s="109" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C20" s="111">
         <f>TDIST(ABS(C18),C8-1,1)</f>
         <v>1.7232439145239769E-75</v>
       </c>
-      <c r="F20" s="155" t="s">
-        <v>352</v>
+      <c r="F20" s="152" t="s">
+        <v>349</v>
       </c>
       <c r="J20" s="132" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="K20" s="133">
         <f>_xlfn.BINOM.DIST(K10,K8,K9/100,TRUE)</f>
@@ -5858,7 +5997,7 @@
     </row>
     <row r="21" spans="2:28">
       <c r="B21" s="112" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C21" s="113" t="str">
         <f>IF(C20&gt;C10, "P &gt; a", "P &lt; a")</f>
@@ -5882,10 +6021,10 @@
         <v>REJECT</v>
       </c>
       <c r="D22" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="AA22" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="AB22">
         <f>AB$8 + AB$19*AB$10/SQRT(AB$6)</f>
@@ -5893,25 +6032,25 @@
       </c>
     </row>
     <row r="24" spans="2:28" ht="17">
-      <c r="B24" s="144" t="s">
-        <v>239</v>
-      </c>
-      <c r="C24" s="144"/>
+      <c r="B24" s="160" t="s">
+        <v>236</v>
+      </c>
+      <c r="C24" s="160"/>
       <c r="O24" s="15" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="P24" t="s">
         <v>43</v>
       </c>
       <c r="AA24" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="25" spans="2:28" ht="17">
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
       <c r="F25" s="112" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G25" s="113" t="str">
         <f>IF(G19&gt;G10, "P &gt; a", "P &lt; a")</f>
@@ -5943,7 +6082,7 @@
     </row>
     <row r="28" spans="2:28" ht="17">
       <c r="B28" s="79" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C28" s="79">
         <v>0.4</v>
@@ -5952,7 +6091,7 @@
     </row>
     <row r="29" spans="2:28">
       <c r="B29" s="117" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C29" s="117">
         <v>99</v>
@@ -5964,7 +6103,7 @@
     </row>
     <row r="31" spans="2:28">
       <c r="B31" s="32" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C31" s="32">
         <f>C27*(C28/100)*(1-(C28/100))</f>
@@ -5977,7 +6116,7 @@
     </row>
     <row r="33" spans="2:27">
       <c r="B33" s="32" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C33" s="32">
         <f>((100-C29) /2)/100</f>
@@ -5986,14 +6125,14 @@
     </row>
     <row r="34" spans="2:27">
       <c r="B34" s="32" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C34" s="32">
         <f>_xlfn.NORM.INV((1-C33),0,1)</f>
         <v>2.5758293035488999</v>
       </c>
       <c r="AA34" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="35" spans="2:27">
@@ -6002,7 +6141,7 @@
     </row>
     <row r="36" spans="2:27">
       <c r="B36" s="125" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C36" s="125">
         <f>C26/C27</f>
@@ -6015,7 +6154,7 @@
     </row>
     <row r="38" spans="2:27">
       <c r="B38" s="102" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C38" s="129">
         <f>C36-(C34*SQRT((C36*(1-C36))/C27))</f>
@@ -6031,50 +6170,50 @@
         <v>0.45008250020592355</v>
       </c>
       <c r="D39" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="43" spans="2:27">
       <c r="B43" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="45" spans="2:27">
       <c r="B45" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="47" spans="2:27">
       <c r="B47" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" spans="2:27">
       <c r="B48" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="B49" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="B50" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="29">
       <c r="A52" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B52" s="138" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="29">
       <c r="B53" s="138" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="21">
@@ -6082,47 +6221,47 @@
     </row>
     <row r="61" spans="1:2" ht="17">
       <c r="B61" s="15" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="B62" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="69" spans="2:2" ht="17">
       <c r="B69" s="15" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="72" spans="2:2" ht="26">
-      <c r="B72" s="154" t="s">
-        <v>348</v>
+      <c r="B72" s="151" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="74" spans="2:2" ht="17">
       <c r="B74" s="15" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="75" spans="2:2">
       <c r="B75" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -6141,8 +6280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C96CE9-B77B-704D-8A1F-7836B7353FCF}">
   <dimension ref="A1:AI69"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="94" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView zoomScale="94" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6191,7 +6330,7 @@
       </c>
       <c r="T1" s="32"/>
       <c r="V1" s="32" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="W1" s="32"/>
       <c r="X1" s="32"/>
@@ -6218,9 +6357,9 @@
       <c r="D2" s="32"/>
       <c r="E2" s="34"/>
       <c r="G2" s="34" t="s">
-        <v>318</v>
-      </c>
-      <c r="H2" s="149">
+        <v>315</v>
+      </c>
+      <c r="H2" s="146">
         <v>-2</v>
       </c>
       <c r="J2" s="32" t="s">
@@ -6278,9 +6417,9 @@
         <v>1252</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>319</v>
-      </c>
-      <c r="H3" s="149">
+        <v>316</v>
+      </c>
+      <c r="H3" s="146">
         <v>2</v>
       </c>
       <c r="J3" s="32"/>
@@ -6331,9 +6470,9 @@
         <v>129</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>320</v>
-      </c>
-      <c r="H4" s="149">
+        <v>317</v>
+      </c>
+      <c r="H4" s="146">
         <f>_xlfn.NORM.DIST(H2, 0, 1, TRUE)</f>
         <v>2.2750131948179191E-2</v>
       </c>
@@ -6392,9 +6531,9 @@
       <c r="D5" s="32"/>
       <c r="E5" s="34"/>
       <c r="G5" s="34" t="s">
-        <v>321</v>
-      </c>
-      <c r="H5" s="149">
+        <v>318</v>
+      </c>
+      <c r="H5" s="146">
         <f>1 - _xlfn.NORM.DIST(H3, 0, 1, TRUE)</f>
         <v>2.2750131948179209E-2</v>
       </c>
@@ -6402,7 +6541,7 @@
         <v>23</v>
       </c>
       <c r="K5" s="42">
-        <v>118</v>
+        <v>200</v>
       </c>
       <c r="L5" s="45"/>
       <c r="P5" s="32" t="s">
@@ -6449,7 +6588,7 @@
       <c r="G6" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="H6" s="149">
+      <c r="H6" s="146">
         <f>SUM(H4:H5)</f>
         <v>4.5500263896358403E-2</v>
       </c>
@@ -6457,12 +6596,12 @@
         <v>78</v>
       </c>
       <c r="K6" s="42">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="L6" s="45"/>
       <c r="P6" s="33"/>
       <c r="Q6" s="32"/>
-      <c r="S6" s="159" t="s">
+      <c r="S6" s="156" t="s">
         <v>151</v>
       </c>
       <c r="T6" s="136">
@@ -6501,7 +6640,7 @@
       </c>
       <c r="K7" s="42">
         <f>K6/100</f>
-        <v>0.97</v>
+        <v>0.59</v>
       </c>
       <c r="L7" s="45"/>
       <c r="P7" s="32" t="s">
@@ -6526,8 +6665,8 @@
       </c>
     </row>
     <row r="8" spans="1:35" ht="21" customHeight="1">
-      <c r="A8" s="152" t="s">
-        <v>338</v>
+      <c r="A8" s="149" t="s">
+        <v>335</v>
       </c>
       <c r="B8" s="2">
         <f>B3</f>
@@ -6535,8 +6674,8 @@
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="34"/>
-      <c r="G8" s="150" t="s">
-        <v>322</v>
+      <c r="G8" s="147" t="s">
+        <v>319</v>
       </c>
       <c r="J8" s="32"/>
       <c r="K8" s="40"/>
@@ -6548,19 +6687,19 @@
         <f>_xlfn.NORM.DIST(Q5, 0, 1, TRUE)</f>
         <v>0.50797831371690205</v>
       </c>
-      <c r="S8" s="158" t="s">
-        <v>353</v>
+      <c r="S8" s="155" t="s">
+        <v>350</v>
       </c>
       <c r="T8" s="136">
         <f>_xlfn.NORM.INV(0.97, 15, 3)</f>
         <v>20.642380824453753</v>
       </c>
-      <c r="AH8" s="151" t="s">
-        <v>336</v>
+      <c r="AH8" s="148" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="19">
-      <c r="A9" s="152" t="s">
+      <c r="A9" s="149" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="2">
@@ -6572,15 +6711,15 @@
       <c r="E9" s="34">
         <v>1400</v>
       </c>
-      <c r="G9" s="150" t="s">
-        <v>323</v>
+      <c r="G9" s="147" t="s">
+        <v>320</v>
       </c>
       <c r="J9" s="47" t="s">
         <v>129</v>
       </c>
       <c r="K9" s="48">
         <f>_xlfn.NORM.INV(($K$6/100),K$4,K$5)</f>
-        <v>1483.9336457618476</v>
+        <v>1307.50899532823</v>
       </c>
       <c r="L9" s="45"/>
       <c r="P9" s="32"/>
@@ -6594,8 +6733,8 @@
       <c r="AH9" s="15"/>
     </row>
     <row r="10" spans="1:35" ht="17">
-      <c r="A10" s="152" t="s">
-        <v>339</v>
+      <c r="A10" s="149" t="s">
+        <v>336</v>
       </c>
       <c r="B10" s="2">
         <f>B4/SQRT(B9)</f>
@@ -6667,7 +6806,7 @@
       </c>
       <c r="K14" s="49">
         <f>(1 - K7)/2</f>
-        <v>1.5000000000000013E-2</v>
+        <v>0.20500000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:35">
@@ -6688,7 +6827,7 @@
       </c>
       <c r="K15" s="49">
         <f>K7+K14</f>
-        <v>0.98499999999999999</v>
+        <v>0.79499999999999993</v>
       </c>
       <c r="P15" t="s">
         <v>138</v>
@@ -6727,7 +6866,7 @@
       </c>
       <c r="K17" s="49">
         <f>NORMINV(K14, 0, 1)</f>
-        <v>-2.1700903775845601</v>
+        <v>-0.823893630338557</v>
       </c>
       <c r="P17" t="s">
         <v>127</v>
@@ -6756,7 +6895,7 @@
       </c>
       <c r="K18" s="49">
         <f>NORMINV(K15, 0, 1)</f>
-        <v>2.1700903775845601</v>
+        <v>0.82389363033855734</v>
       </c>
       <c r="P18" t="s">
         <v>139</v>
@@ -6786,7 +6925,7 @@
       </c>
       <c r="E20" s="34"/>
       <c r="J20" s="32" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="K20" s="35"/>
       <c r="L20" s="32"/>
@@ -6801,7 +6940,7 @@
       </c>
       <c r="K21" s="51">
         <f>K4 + (K17)*K5</f>
-        <v>1005.9293354450219</v>
+        <v>1097.2212739322886</v>
       </c>
       <c r="P21" t="s">
         <v>142</v>
@@ -6818,7 +6957,7 @@
       </c>
       <c r="K22" s="51">
         <f>K4+(K18*K5)</f>
-        <v>1518.0706645549781</v>
+        <v>1426.7787260677114</v>
       </c>
       <c r="P22" t="s">
         <v>143</v>
@@ -6848,53 +6987,53 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="28" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="J26" s="34" t="s">
         <v>146</v>
       </c>
       <c r="K26" s="51">
         <f>K28-K27</f>
-        <v>159.17958104627542</v>
+        <v>269.79590007843262</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="28" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="J27" s="34" t="s">
         <v>147</v>
       </c>
       <c r="K27" s="30">
         <f>_xlfn.NORM.INV((25/100),K$4,K$5)</f>
-        <v>1182.4102094768623</v>
+        <v>1127.1020499607837</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="4" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="J28" s="34" t="s">
         <v>148</v>
       </c>
       <c r="K28" s="30">
         <f>_xlfn.NORM.INV((75/100),K$4,K$5)</f>
-        <v>1341.5897905231377</v>
+        <v>1396.8979500392163</v>
       </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="28" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="17">
       <c r="A30" s="15" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="28" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="P31" t="s">
         <v>141</v>
@@ -6906,57 +7045,70 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="28" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" ht="17">
+    <row r="33" spans="1:7" ht="17">
       <c r="A33" s="15" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" ht="17">
+    <row r="34" spans="1:7" ht="17">
       <c r="A34" s="15"/>
     </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="148" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="148" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="148" t="s">
+    <row r="36" spans="1:7">
+      <c r="A36" s="145" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="145" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="145" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="145" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="148" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="153"/>
+    <row r="45" spans="1:7">
+      <c r="G45" s="150" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="G46" s="150" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="150"/>
+      <c r="G47" s="150" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D68" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D69" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -6986,7 +7138,7 @@
       <c r="C2" s="60"/>
       <c r="D2" s="60"/>
       <c r="E2" s="60" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F2" s="60"/>
       <c r="G2" s="60"/>
@@ -6996,27 +7148,27 @@
       <c r="K2" s="60"/>
     </row>
     <row r="3" spans="2:14">
-      <c r="B3" s="145" t="s">
-        <v>183</v>
-      </c>
-      <c r="C3" s="145"/>
+      <c r="B3" s="161" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="161"/>
       <c r="D3" s="60"/>
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="145" t="s">
-        <v>184</v>
-      </c>
-      <c r="I3" s="145"/>
+      <c r="H3" s="161" t="s">
+        <v>181</v>
+      </c>
+      <c r="I3" s="161"/>
       <c r="J3" s="60"/>
       <c r="K3" s="60"/>
       <c r="M3" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="2:14">
       <c r="B4" s="61" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C4" s="61">
         <v>95</v>
@@ -7036,7 +7188,7 @@
     </row>
     <row r="5" spans="2:14">
       <c r="B5" s="61" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C5" s="61">
         <v>47</v>
@@ -7058,7 +7210,7 @@
       <c r="J5" s="60"/>
       <c r="K5" s="60"/>
       <c r="M5" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="N5">
         <f>AVERAGE(M15:M24)</f>
@@ -7067,7 +7219,7 @@
     </row>
     <row r="6" spans="2:14">
       <c r="B6" s="61" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C6" s="61">
         <v>3</v>
@@ -7082,7 +7234,7 @@
       </c>
       <c r="G6" s="60"/>
       <c r="H6" s="61" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I6" s="61">
         <v>0.65700000000000003</v>
@@ -7100,7 +7252,7 @@
       </c>
       <c r="D7" s="60"/>
       <c r="E7" s="61" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F7" s="61">
         <f>F5*F6*(1-F6)</f>
@@ -7108,7 +7260,7 @@
       </c>
       <c r="G7" s="60"/>
       <c r="H7" s="61" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I7" s="61">
         <v>1200</v>
@@ -7126,7 +7278,7 @@
       </c>
       <c r="D8" s="60"/>
       <c r="E8" s="61" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F8" s="61">
         <v>90</v>
@@ -7155,7 +7307,7 @@
       </c>
       <c r="G9" s="60"/>
       <c r="H9" s="62" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I9" s="62">
         <f>(I6-I5)/2</f>
@@ -7169,7 +7321,7 @@
       <c r="C10" s="60"/>
       <c r="D10" s="60"/>
       <c r="E10" s="61" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F10" s="61">
         <f>((100-F8) /2)/100</f>
@@ -7191,7 +7343,7 @@
       <c r="C11" s="60"/>
       <c r="D11" s="60"/>
       <c r="E11" s="61" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F11" s="61">
         <f>_xlfn.NORM.INV((1-F10),0,1)</f>
@@ -7208,7 +7360,7 @@
       <c r="C12" s="60"/>
       <c r="D12" s="60"/>
       <c r="E12" s="62" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F12" s="64">
         <f>F6-F$11*F9</f>
@@ -7238,10 +7390,10 @@
       <c r="K13" s="60"/>
     </row>
     <row r="14" spans="2:14">
-      <c r="B14" s="145" t="s">
-        <v>196</v>
-      </c>
-      <c r="C14" s="145"/>
+      <c r="B14" s="161" t="s">
+        <v>193</v>
+      </c>
+      <c r="C14" s="161"/>
       <c r="D14" s="60"/>
       <c r="E14" s="60"/>
       <c r="F14" s="60"/>
@@ -7251,21 +7403,21 @@
       <c r="J14" s="60"/>
       <c r="K14" s="60"/>
       <c r="M14" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="15" spans="2:14">
       <c r="B15" s="61" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C15" s="61">
         <v>0.98</v>
       </c>
       <c r="D15" s="60"/>
-      <c r="E15" s="145" t="s">
-        <v>198</v>
-      </c>
-      <c r="F15" s="145"/>
+      <c r="E15" s="161" t="s">
+        <v>195</v>
+      </c>
+      <c r="F15" s="161"/>
       <c r="G15" s="66"/>
       <c r="H15" s="66"/>
       <c r="I15" s="66"/>
@@ -7277,14 +7429,14 @@
     </row>
     <row r="16" spans="2:14">
       <c r="B16" s="61" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C16" s="61">
         <v>94</v>
       </c>
       <c r="D16" s="60"/>
       <c r="E16" s="61" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F16" s="61">
         <v>1</v>
@@ -7300,7 +7452,7 @@
     </row>
     <row r="17" spans="2:13">
       <c r="B17" s="61" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C17" s="61">
         <v>0.15</v>
@@ -7321,7 +7473,7 @@
     </row>
     <row r="18" spans="2:13">
       <c r="B18" s="61" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C18" s="61">
         <f>((100-C16)/100)/2</f>
@@ -7329,7 +7481,7 @@
       </c>
       <c r="D18" s="60"/>
       <c r="E18" s="61" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F18" s="61">
         <f>F17^2</f>
@@ -7346,7 +7498,7 @@
     </row>
     <row r="19" spans="2:13">
       <c r="B19" s="61" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C19" s="69">
         <f>_xlfn.NORM.INV(1-C18,0,1)</f>
@@ -7366,7 +7518,7 @@
     </row>
     <row r="20" spans="2:13">
       <c r="B20" s="62" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C20" s="64">
         <f xml:space="preserve"> C17*(1-C17)*((C19/C15)^2)</f>
@@ -7374,7 +7526,7 @@
       </c>
       <c r="D20" s="60"/>
       <c r="E20" s="70" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F20" s="60"/>
       <c r="G20" s="60"/>
@@ -7388,7 +7540,7 @@
     </row>
     <row r="21" spans="2:13">
       <c r="B21" s="62" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C21" s="64">
         <f>0.25*((C19/C15)^2)</f>
@@ -7396,7 +7548,7 @@
       </c>
       <c r="D21" s="60"/>
       <c r="E21" s="71" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F21" s="72"/>
       <c r="G21" s="72"/>
@@ -7463,19 +7615,19 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:10">
-      <c r="B4" s="144" t="s">
-        <v>208</v>
-      </c>
-      <c r="C4" s="144"/>
-      <c r="E4" s="144" t="s">
-        <v>209</v>
-      </c>
-      <c r="F4" s="144"/>
-      <c r="H4" s="144" t="s">
-        <v>210</v>
-      </c>
-      <c r="I4" s="144"/>
-      <c r="J4" s="144"/>
+      <c r="B4" s="160" t="s">
+        <v>205</v>
+      </c>
+      <c r="C4" s="160"/>
+      <c r="E4" s="160" t="s">
+        <v>206</v>
+      </c>
+      <c r="F4" s="160"/>
+      <c r="H4" s="160" t="s">
+        <v>207</v>
+      </c>
+      <c r="I4" s="160"/>
+      <c r="J4" s="160"/>
     </row>
     <row r="5" spans="2:10">
       <c r="B5" s="76"/>
@@ -7488,7 +7640,7 @@
     </row>
     <row r="6" spans="2:10">
       <c r="B6" s="74" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C6" s="74">
         <v>0.93799999999999994</v>
@@ -7509,13 +7661,13 @@
     </row>
     <row r="7" spans="2:10">
       <c r="B7" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C7" s="75">
         <v>25</v>
       </c>
       <c r="E7" s="80" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F7" s="81">
         <v>11.6</v>
@@ -7530,14 +7682,14 @@
     </row>
     <row r="8" spans="2:10">
       <c r="B8" s="82" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C8" s="83">
         <f>_xlfn.T.INV(C6,C7)</f>
         <v>1.5917851223801218</v>
       </c>
       <c r="E8" s="84" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F8" s="85">
         <v>95</v>
@@ -7548,7 +7700,7 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" s="82" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C9" s="83">
         <f>ABS(C8)</f>
@@ -7573,14 +7725,14 @@
       <c r="B10" s="74"/>
       <c r="C10" s="74"/>
       <c r="E10" s="74" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F10" s="32">
         <f>((100-F8)/100 )/2</f>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="H10" s="88" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I10" s="89">
         <f>I7-I9</f>
@@ -7596,7 +7748,7 @@
         <v>80</v>
       </c>
       <c r="E11" s="74" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F11" s="32">
         <f>ABS(_xlfn.T.INV(F10,F9-1))</f>
@@ -7605,13 +7757,13 @@
     </row>
     <row r="12" spans="2:10">
       <c r="B12" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C12" s="74">
         <v>14</v>
       </c>
       <c r="E12" s="82" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F12" s="90">
         <f>F6-(F11*(F7/SQRT(F9)))</f>
@@ -7620,7 +7772,7 @@
     </row>
     <row r="13" spans="2:10">
       <c r="B13" s="74" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C13" s="74">
         <f>((100-C11)/100)/2</f>
@@ -7636,36 +7788,36 @@
     </row>
     <row r="14" spans="2:10">
       <c r="B14" s="82" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C14" s="83">
         <f>ABS(_xlfn.T.INV(C13,C12))</f>
         <v>1.3450303744546506</v>
       </c>
       <c r="H14" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="2:10">
       <c r="E15" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="16" spans="2:10">
       <c r="H16" s="32" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I16" s="32">
         <v>23.86</v>
       </c>
     </row>
     <row r="17" spans="2:9">
-      <c r="B17" s="144" t="s">
-        <v>223</v>
-      </c>
-      <c r="C17" s="144"/>
+      <c r="B17" s="160" t="s">
+        <v>220</v>
+      </c>
+      <c r="C17" s="160"/>
       <c r="H17" s="32" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I17" s="32">
         <v>2.9000000000000001E-2</v>
@@ -7675,7 +7827,7 @@
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
       <c r="H18" s="32" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="I18" s="32">
         <v>95</v>
@@ -7683,7 +7835,7 @@
     </row>
     <row r="19" spans="2:9">
       <c r="B19" s="74" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C19" s="74">
         <v>0.89300000000000002</v>
@@ -7697,7 +7849,7 @@
     </row>
     <row r="20" spans="2:9">
       <c r="B20" s="74" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C20" s="74">
         <v>95</v>
@@ -7711,7 +7863,7 @@
     </row>
     <row r="21" spans="2:9">
       <c r="B21" s="74" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C21" s="74">
         <v>1.96</v>
@@ -7723,7 +7875,7 @@
       <c r="B22" s="74"/>
       <c r="C22" s="74"/>
       <c r="H22" s="89" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I22" s="89">
         <f>I20-I16</f>
@@ -7732,19 +7884,19 @@
     </row>
     <row r="23" spans="2:9">
       <c r="B23" s="74" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C23" s="74">
         <f>((100-C20)/100 )/2</f>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="H23" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="2:9">
       <c r="B24" s="74" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C24" s="91">
         <f>_xlfn.NORM.INV(1-C23,0,1)</f>
@@ -7764,7 +7916,7 @@
         <v>18.505695292838212</v>
       </c>
       <c r="D26" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -7794,7 +7946,7 @@
   <sheetData>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -7802,7 +7954,7 @@
         <v>30120</v>
       </c>
       <c r="C3" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -7813,7 +7965,7 @@
         <v>30415</v>
       </c>
       <c r="C4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D4">
         <v>6000</v>
@@ -7835,16 +7987,16 @@
         <v>32114</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D6" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F6" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -7932,7 +8084,7 @@
         <v>34676</v>
       </c>
       <c r="D11" s="142" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -7950,7 +8102,7 @@
         <v>35576</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F14">
         <f>COUNT(A3:A27)</f>
@@ -8054,10 +8206,10 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="W2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="X2">
         <f>_xlfn.STDEV.P(X11:X19)</f>
@@ -8069,17 +8221,17 @@
         <v>340</v>
       </c>
       <c r="C3" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D3">
         <f>COUNT(A3:A202)</f>
         <v>20</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="W3" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="X3">
         <f>_xlfn.STDEV.S(X11:X19)</f>
@@ -8098,10 +8250,10 @@
         <v>432.9</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="W4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="X4">
         <f>AVERAGE(Y11:Y19)</f>
@@ -8120,7 +8272,7 @@
         <v>76.226739333869418</v>
       </c>
       <c r="G5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -8145,7 +8297,7 @@
         <v>441</v>
       </c>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D8">
         <f>QUARTILE(A$3:A$22, 2)</f>
@@ -8169,10 +8321,10 @@
         <v>373</v>
       </c>
       <c r="W10" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="X10" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="Y10" t="s">
         <v>121</v>
@@ -8185,18 +8337,18 @@
       <c r="C11" t="s">
         <v>146</v>
       </c>
-      <c r="D11" s="146">
+      <c r="D11" s="143">
         <f>D9-D7</f>
         <v>135</v>
       </c>
       <c r="W11" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="X11">
         <v>77</v>
       </c>
       <c r="Y11">
-        <f>(X11-X$1)/X$2</f>
+        <f t="shared" ref="Y11:Y19" si="0">(X11-X$1)/X$2</f>
         <v>0.58909018851653028</v>
       </c>
     </row>
@@ -8205,13 +8357,13 @@
         <v>343</v>
       </c>
       <c r="W12" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="X12">
         <v>60</v>
       </c>
       <c r="Y12">
-        <f>(X12-X$1)/X$2</f>
+        <f t="shared" si="0"/>
         <v>-1.6092219783866186</v>
       </c>
     </row>
@@ -8220,13 +8372,13 @@
         <v>527</v>
       </c>
       <c r="W13" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="X13">
         <v>60</v>
       </c>
       <c r="Y13">
-        <f>(X13-X$1)/X$2</f>
+        <f t="shared" si="0"/>
         <v>-1.6092219783866186</v>
       </c>
     </row>
@@ -8235,13 +8387,13 @@
         <v>337</v>
       </c>
       <c r="W14" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="X14">
         <v>81</v>
       </c>
       <c r="Y14">
-        <f>(X14-X$1)/X$2</f>
+        <f t="shared" si="0"/>
         <v>1.1063401101408006</v>
       </c>
     </row>
@@ -8250,13 +8402,13 @@
         <v>547</v>
       </c>
       <c r="W15" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="X15">
         <v>73</v>
       </c>
       <c r="Y15">
-        <f>(X15-X$1)/X$2</f>
+        <f t="shared" si="0"/>
         <v>7.1840266892259974E-2</v>
       </c>
     </row>
@@ -8265,16 +8417,16 @@
         <v>406</v>
       </c>
       <c r="G16" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="W16" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="X16">
         <v>80</v>
       </c>
       <c r="Y16">
-        <f>(X16-X$1)/X$2</f>
+        <f t="shared" si="0"/>
         <v>0.97702762973473312</v>
       </c>
     </row>
@@ -8283,16 +8435,16 @@
         <v>447</v>
       </c>
       <c r="G17" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="W17" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="X17">
         <v>80</v>
       </c>
       <c r="Y17">
-        <f>(X17-X$1)/X$2</f>
+        <f t="shared" si="0"/>
         <v>0.97702762973473312</v>
       </c>
     </row>
@@ -8301,16 +8453,16 @@
         <v>431</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="W18" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="X18">
         <v>68</v>
       </c>
       <c r="Y18">
-        <f>(X18-X$1)/X$2</f>
+        <f t="shared" si="0"/>
         <v>-0.57472213513807791</v>
       </c>
     </row>
@@ -8319,16 +8471,16 @@
         <v>517</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="W19" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="X19">
         <v>73</v>
       </c>
       <c r="Y19">
-        <f>(X19-X$1)/X$2</f>
+        <f t="shared" si="0"/>
         <v>7.1840266892259974E-2</v>
       </c>
     </row>
@@ -8343,7 +8495,7 @@
         <v>339</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="Y21">
         <f>SUM(Y11:Y19)</f>
@@ -8365,14 +8517,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFCA351-70B0-5244-BA65-285CF6942DC3}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
     <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="8" max="8" width="26.5" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8381,19 +8534,25 @@
         <v>157</v>
       </c>
       <c r="B1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C1" t="s">
         <v>43</v>
       </c>
       <c r="E1" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" t="s">
         <v>172</v>
       </c>
-      <c r="F1" t="s">
-        <v>173</v>
+      <c r="H1" t="s">
+        <v>388</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
       </c>
       <c r="L1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17">
@@ -8401,16 +8560,19 @@
         <v>89</v>
       </c>
       <c r="B2" s="16">
-        <v>123</v>
+        <v>43.7</v>
       </c>
       <c r="E2" t="s">
         <v>109</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>51</v>
+      </c>
+      <c r="H2" t="s">
+        <v>389</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="M2">
         <v>240000</v>
@@ -8421,17 +8583,23 @@
         <v>127</v>
       </c>
       <c r="B3" s="54">
-        <v>11</v>
+        <v>4.2</v>
       </c>
       <c r="E3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F3">
         <f>F2/100</f>
-        <v>0.05</v>
+        <v>0.51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3">
+        <v>43.7</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="M3">
         <v>10</v>
@@ -8439,10 +8607,10 @@
     </row>
     <row r="4" spans="1:13" ht="17">
       <c r="A4" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" s="16">
-        <v>119</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
         <v>158</v>
@@ -8450,14 +8618,23 @@
       <c r="F4">
         <v>300</v>
       </c>
+      <c r="H4" t="s">
+        <v>390</v>
+      </c>
+      <c r="I4">
+        <v>4.2</v>
+      </c>
       <c r="L4" s="15" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="M4">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:13">
+      <c r="A5" s="25" t="s">
+        <v>386</v>
+      </c>
       <c r="B5" s="16"/>
     </row>
     <row r="6" spans="1:13">
@@ -8466,14 +8643,20 @@
       </c>
       <c r="B6" s="52">
         <f>B2</f>
-        <v>123</v>
+        <v>43.7</v>
       </c>
       <c r="E6" t="s">
-        <v>175</v>
+        <v>396</v>
       </c>
       <c r="F6" s="53">
         <f>F3</f>
-        <v>0.05</v>
+        <v>0.51</v>
+      </c>
+      <c r="H6" t="s">
+        <v>391</v>
+      </c>
+      <c r="I6">
+        <v>40</v>
       </c>
       <c r="L6" t="s">
         <v>23</v>
@@ -8485,158 +8668,169 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="16" t="s">
-        <v>160</v>
+        <v>387</v>
       </c>
       <c r="B7" s="56">
         <f>B3/SQRT(B4)</f>
-        <v>1.0083683467310325</v>
+        <v>0.46957427527495582</v>
       </c>
       <c r="E7" t="s">
-        <v>176</v>
+        <v>395</v>
       </c>
       <c r="F7" s="53">
         <f>SQRT(F6*(1 - F6)/F4)</f>
-        <v>1.2583057392117916E-2</v>
+        <v>2.8861739379323625E-2</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="B8" s="16"/>
+      <c r="H8" t="s">
+        <v>392</v>
+      </c>
+      <c r="I8">
+        <f>_xlfn.NORM.DIST(I6,I3,I4, TRUE)</f>
+        <v>0.18917179719797161</v>
+      </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="25" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B9" s="16">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="E9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F9" s="53">
         <f>(F4*F6)*(1 - F6)</f>
-        <v>14.25</v>
+        <v>74.97</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B10" s="55">
         <f>(B9-B2)/B3</f>
-        <v>-0.36363636363636365</v>
+        <v>26.499999999999996</v>
+      </c>
+      <c r="H10" t="s">
+        <v>391</v>
+      </c>
+      <c r="I10">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B11" s="57">
         <f>(B9-B2)/B7</f>
-        <v>-3.9668044053220779</v>
+        <v>237.02320561497771</v>
       </c>
       <c r="E11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F11">
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="E12" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F12">
         <f>F11/100</f>
-        <v>0.2</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B13">
         <f>_xlfn.NORM.S.DIST(B10, TRUE)</f>
-        <v>0.35806478442778267</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
         <v>121</v>
       </c>
       <c r="F13">
         <f>(F12-F6)/F7</f>
-        <v>11.920791213585396</v>
-      </c>
-      <c r="H13">
-        <v>19</v>
+        <v>-2.0788767860257109</v>
+      </c>
+      <c r="H13" s="162" t="s">
+        <v>394</v>
       </c>
       <c r="I13">
-        <v>0.79341189999999995</v>
+        <f>I4/SQRT(I10)</f>
+        <v>1.2124355652982142</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="17">
       <c r="A14" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B14" s="58">
-        <f xml:space="preserve"> 1-B13</f>
-        <v>0.64193521557221733</v>
+        <f xml:space="preserve"> 1 - B13</f>
+        <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F14" s="53">
         <f>_xlfn.NORM.S.DIST(F13, TRUE)</f>
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>14</v>
+        <v>1.8814338445845531E-2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>393</v>
       </c>
       <c r="I14">
-        <v>0.70731049999999995</v>
+        <f>_xlfn.NORM.DIST(I6,I3,I13,TRUE)</f>
+        <v>1.1377145360498184E-3</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="17">
       <c r="E15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F15" s="53">
         <f xml:space="preserve"> 1 - F14</f>
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <f>I13-I14</f>
-        <v>8.6101399999999995E-2</v>
+        <v>0.98118566155415443</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="17">
       <c r="A16" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B16" s="52">
         <f>_xlfn.NORM.S.DIST(B11, TRUE)</f>
-        <v>3.6421361779336248E-5</v>
+        <v>1</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B17" s="52">
         <f xml:space="preserve"> 1 -B16</f>
-        <v>0.99996357863822072</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B20" s="16"/>
     </row>
@@ -8645,7 +8839,7 @@
         <v>67</v>
       </c>
       <c r="B21" s="16">
-        <v>87.75</v>
+        <v>155</v>
       </c>
       <c r="E21">
         <v>0.174543</v>
@@ -8656,7 +8850,7 @@
         <v>68</v>
       </c>
       <c r="B22" s="16">
-        <v>90.65</v>
+        <v>160</v>
       </c>
       <c r="E22">
         <v>0.81106243</v>
@@ -8664,18 +8858,18 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B23">
         <f>(B21-B$6)/B$7</f>
-        <v>-34.957463821900809</v>
+        <v>237.02320561497771</v>
       </c>
       <c r="E23">
         <f>E22-E21</f>
         <v>0.63651943</v>
       </c>
       <c r="F23" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -8684,26 +8878,26 @@
       </c>
       <c r="B24">
         <f>(B22-B$6)/B$7</f>
-        <v>-32.081530628042302</v>
+        <v>247.67114836497672</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B26" s="53">
         <f>_xlfn.NORM.S.DIST(B24, TRUE) - _xlfn.NORM.S.DIST(B23, TRUE)</f>
-        <v>3.9897916573105739E-226</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="4" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="255">
-      <c r="A28" s="147" t="s">
-        <v>333</v>
+        <v>332</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="40" customHeight="1">
+      <c r="A28" s="144" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -8852,7 +9046,7 @@
     </row>
     <row r="22" spans="1:1" ht="17">
       <c r="A22" s="15" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>